<commit_message>
Update automàtic: dades i banners [2026-02-07 17:35]
</commit_message>
<xml_diff>
--- a/config/data/resum_diari_meteocat.xlsx
+++ b/config/data/resum_diari_meteocat.xlsx
@@ -565,7 +565,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:38</t>
+          <t>2026-02-07 17:27:53</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
@@ -576,7 +576,7 @@
       <c r="G2" s="3" t="inlineStr"/>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I2" s="3" t="inlineStr">
@@ -587,7 +587,7 @@
       <c r="J2" s="3" t="inlineStr"/>
       <c r="K2" s="3" t="inlineStr">
         <is>
-          <t>11.9 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L2" s="3" t="inlineStr">
@@ -607,7 +607,7 @@
       </c>
       <c r="O2" s="3" t="inlineStr">
         <is>
-          <t>7.3 °C</t>
+          <t>7.5 °C</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:40</t>
+          <t>2026-02-07 17:27:56</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
@@ -645,7 +645,7 @@
       <c r="G3" s="3" t="inlineStr"/>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I3" s="3" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="O3" s="3" t="inlineStr">
         <is>
-          <t>7.9 °C</t>
+          <t>8.2 °C</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:43</t>
+          <t>2026-02-07 17:27:58</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
@@ -721,7 +721,7 @@
       <c r="J4" s="3" t="inlineStr"/>
       <c r="K4" s="3" t="inlineStr">
         <is>
-          <t>11.6 MJ/m2</t>
+          <t>11.8 MJ/m2</t>
         </is>
       </c>
       <c r="L4" s="3" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="O4" s="3" t="inlineStr">
         <is>
-          <t>13.6 °C</t>
+          <t>13.7 °C</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:45</t>
+          <t>2026-02-07 17:28:01</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
@@ -779,7 +779,7 @@
       <c r="G5" s="3" t="inlineStr"/>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="I5" s="3" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="O5" s="3" t="inlineStr">
         <is>
-          <t>7.2 °C</t>
+          <t>7.4 °C</t>
         </is>
       </c>
     </row>
@@ -833,7 +833,7 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:48</t>
+          <t>2026-02-07 17:28:03</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
@@ -844,7 +844,7 @@
       <c r="G6" s="3" t="inlineStr"/>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I6" s="3" t="inlineStr">
@@ -855,7 +855,7 @@
       <c r="J6" s="3" t="inlineStr"/>
       <c r="K6" s="3" t="inlineStr">
         <is>
-          <t>12.4 MJ/m2</t>
+          <t>12.6 MJ/m2</t>
         </is>
       </c>
       <c r="L6" s="3" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="O6" s="3" t="inlineStr">
         <is>
-          <t>7.3 °C</t>
+          <t>7.5 °C</t>
         </is>
       </c>
     </row>
@@ -902,7 +902,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:50</t>
+          <t>2026-02-07 17:28:05</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
@@ -913,7 +913,7 @@
       <c r="G7" s="3" t="inlineStr"/>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="K7" s="3" t="inlineStr">
         <is>
-          <t>11.9 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L7" s="3" t="inlineStr">
@@ -948,7 +948,7 @@
       </c>
       <c r="O7" s="3" t="inlineStr">
         <is>
-          <t>6.2 °C</t>
+          <t>6.4 °C</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:52</t>
+          <t>2026-02-07 17:28:08</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="L8" s="3" t="inlineStr">
         <is>
-          <t>12.2 km/h - 69º 13:38 TU</t>
+          <t>16.9 km/h - 189º 16:55 TU</t>
         </is>
       </c>
       <c r="M8" s="3" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="O8" s="3" t="inlineStr">
         <is>
-          <t>-5.8 °C</t>
+          <t>-5.7 °C</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:55</t>
+          <t>2026-02-07 17:28:10</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="I9" s="3" t="inlineStr">
@@ -1074,7 +1074,7 @@
       <c r="J9" s="3" t="inlineStr"/>
       <c r="K9" s="3" t="inlineStr">
         <is>
-          <t>8.5 MJ/m2</t>
+          <t>8.6 MJ/m2</t>
         </is>
       </c>
       <c r="L9" s="3" t="inlineStr"/>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:57</t>
+          <t>2026-02-07 17:28:13</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
@@ -1143,7 +1143,7 @@
       <c r="J10" s="3" t="inlineStr"/>
       <c r="K10" s="3" t="inlineStr">
         <is>
-          <t>14.0 MJ/m2</t>
+          <t>14.3 MJ/m2</t>
         </is>
       </c>
       <c r="L10" s="3" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:36:59</t>
+          <t>2026-02-07 17:28:15</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
@@ -1201,7 +1201,7 @@
       <c r="G11" s="3" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="I11" s="3" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="K11" s="3" t="inlineStr">
         <is>
-          <t>11.4 MJ/m2</t>
+          <t>11.6 MJ/m2</t>
         </is>
       </c>
       <c r="L11" s="3" t="inlineStr">
@@ -1236,7 +1236,7 @@
       </c>
       <c r="O11" s="3" t="inlineStr">
         <is>
-          <t>12.9 °C</t>
+          <t>13.0 °C</t>
         </is>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:02</t>
+          <t>2026-02-07 17:28:18</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
@@ -1274,7 +1274,7 @@
       <c r="G12" s="3" t="inlineStr"/>
       <c r="H12" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="I12" s="3" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="O12" s="3" t="inlineStr">
         <is>
-          <t>7.2 °C</t>
+          <t>7.4 °C</t>
         </is>
       </c>
     </row>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:04</t>
+          <t>2026-02-07 17:28:20</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
@@ -1349,12 +1349,12 @@
       </c>
       <c r="J13" s="3" t="inlineStr">
         <is>
-          <t>1003.4 hPa</t>
+          <t>1003.6 hPa</t>
         </is>
       </c>
       <c r="K13" s="3" t="inlineStr">
         <is>
-          <t>10.2 MJ/m2</t>
+          <t>10.5 MJ/m2</t>
         </is>
       </c>
       <c r="L13" s="3" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:07</t>
+          <t>2026-02-07 17:28:23</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="I14" s="3" t="inlineStr">
@@ -1427,12 +1427,12 @@
       <c r="J14" s="3" t="inlineStr"/>
       <c r="K14" s="3" t="inlineStr">
         <is>
-          <t>11.3 MJ/m2</t>
+          <t>11.5 MJ/m2</t>
         </is>
       </c>
       <c r="L14" s="3" t="inlineStr">
         <is>
-          <t>18.4 km/h - 186º 15:48 TU</t>
+          <t>24.5 km/h - 114º 16:58 TU</t>
         </is>
       </c>
       <c r="M14" s="3" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:09</t>
+          <t>2026-02-07 17:28:25</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -1485,7 +1485,7 @@
       <c r="G15" s="3" t="inlineStr"/>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr">
@@ -1496,7 +1496,7 @@
       <c r="J15" s="3" t="inlineStr"/>
       <c r="K15" s="3" t="inlineStr">
         <is>
-          <t>11.3 MJ/m2</t>
+          <t>11.4 MJ/m2</t>
         </is>
       </c>
       <c r="L15" s="3" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="O15" s="3" t="inlineStr">
         <is>
-          <t>7.1 °C</t>
+          <t>7.3 °C</t>
         </is>
       </c>
     </row>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:12</t>
+          <t>2026-02-07 17:28:28</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
@@ -1554,7 +1554,7 @@
       <c r="G16" s="3" t="inlineStr"/>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="O16" s="3" t="inlineStr">
         <is>
-          <t>7.7 °C</t>
+          <t>7.9 °C</t>
         </is>
       </c>
     </row>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:14</t>
+          <t>2026-02-07 17:28:30</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
@@ -1615,7 +1615,7 @@
       <c r="G17" s="3" t="inlineStr"/>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>68%</t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
@@ -1626,7 +1626,7 @@
       <c r="J17" s="3" t="inlineStr"/>
       <c r="K17" s="3" t="inlineStr">
         <is>
-          <t>11.4 MJ/m2</t>
+          <t>11.6 MJ/m2</t>
         </is>
       </c>
       <c r="L17" s="3" t="inlineStr">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="O17" s="3" t="inlineStr">
         <is>
-          <t>9.3 °C</t>
+          <t>9.4 °C</t>
         </is>
       </c>
     </row>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:16</t>
+          <t>2026-02-07 17:28:32</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
@@ -1694,12 +1694,12 @@
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>1005.5 hPa</t>
+          <t>1005.6 hPa</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr">
         <is>
-          <t>12.7 MJ/m2</t>
+          <t>12.9 MJ/m2</t>
         </is>
       </c>
       <c r="L18" s="3" t="inlineStr">
@@ -1719,7 +1719,7 @@
       </c>
       <c r="O18" s="3" t="inlineStr">
         <is>
-          <t>12.3 °C</t>
+          <t>12.4 °C</t>
         </is>
       </c>
     </row>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:19</t>
+          <t>2026-02-07 17:28:35</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
@@ -1757,7 +1757,7 @@
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
@@ -1767,12 +1767,12 @@
       </c>
       <c r="J19" s="3" t="inlineStr">
         <is>
-          <t>1003.4 hPa</t>
+          <t>1003.5 hPa</t>
         </is>
       </c>
       <c r="K19" s="3" t="inlineStr">
         <is>
-          <t>11.8 MJ/m2</t>
+          <t>12.1 MJ/m2</t>
         </is>
       </c>
       <c r="L19" s="3" t="inlineStr">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="O19" s="3" t="inlineStr">
         <is>
-          <t>10.5 °C</t>
+          <t>10.7 °C</t>
         </is>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:21</t>
+          <t>2026-02-07 17:28:37</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
@@ -1830,7 +1830,7 @@
       <c r="G20" s="3" t="inlineStr"/>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t>48%</t>
+          <t>47%</t>
         </is>
       </c>
       <c r="I20" s="3" t="inlineStr">
@@ -1840,12 +1840,12 @@
       </c>
       <c r="J20" s="3" t="inlineStr">
         <is>
-          <t>1005.0 hPa</t>
+          <t>1005.2 hPa</t>
         </is>
       </c>
       <c r="K20" s="3" t="inlineStr">
         <is>
-          <t>12.1 MJ/m2</t>
+          <t>12.3 MJ/m2</t>
         </is>
       </c>
       <c r="L20" s="3" t="inlineStr">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="O20" s="3" t="inlineStr">
         <is>
-          <t>13.1 °C</t>
+          <t>13.2 °C</t>
         </is>
       </c>
     </row>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:24</t>
+          <t>2026-02-07 17:28:40</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
@@ -1913,12 +1913,12 @@
       </c>
       <c r="J21" s="3" t="inlineStr">
         <is>
-          <t>1004.5 hPa</t>
+          <t>1004.7 hPa</t>
         </is>
       </c>
       <c r="K21" s="3" t="inlineStr">
         <is>
-          <t>12.6 MJ/m2</t>
+          <t>12.8 MJ/m2</t>
         </is>
       </c>
       <c r="L21" s="3" t="inlineStr">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="O21" s="3" t="inlineStr">
         <is>
-          <t>9.3 °C</t>
+          <t>9.4 °C</t>
         </is>
       </c>
     </row>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:26</t>
+          <t>2026-02-07 17:28:42</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
@@ -1986,12 +1986,12 @@
       </c>
       <c r="J22" s="3" t="inlineStr">
         <is>
-          <t>1004.9 hPa</t>
+          <t>1005.0 hPa</t>
         </is>
       </c>
       <c r="K22" s="3" t="inlineStr">
         <is>
-          <t>12.5 MJ/m2</t>
+          <t>12.6 MJ/m2</t>
         </is>
       </c>
       <c r="L22" s="3" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="O22" s="3" t="inlineStr">
         <is>
-          <t>12.4 °C</t>
+          <t>12.5 °C</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:29</t>
+          <t>2026-02-07 17:28:45</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
@@ -2060,7 +2060,7 @@
       <c r="J23" s="3" t="inlineStr"/>
       <c r="K23" s="3" t="inlineStr">
         <is>
-          <t>11.6 MJ/m2</t>
+          <t>11.8 MJ/m2</t>
         </is>
       </c>
       <c r="L23" s="3" t="inlineStr"/>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="O23" s="3" t="inlineStr">
         <is>
-          <t>7.9 °C</t>
+          <t>8.0 °C</t>
         </is>
       </c>
     </row>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:31</t>
+          <t>2026-02-07 17:28:47</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
@@ -2114,7 +2114,7 @@
       <c r="G24" s="3" t="inlineStr"/>
       <c r="H24" s="3" t="inlineStr">
         <is>
-          <t>63%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="I24" s="3" t="inlineStr">
@@ -2125,7 +2125,7 @@
       <c r="J24" s="3" t="inlineStr"/>
       <c r="K24" s="3" t="inlineStr">
         <is>
-          <t>12.8 MJ/m2</t>
+          <t>12.9 MJ/m2</t>
         </is>
       </c>
       <c r="L24" s="3" t="inlineStr">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:34</t>
+          <t>2026-02-07 17:28:50</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
@@ -2194,7 +2194,7 @@
       <c r="J25" s="3" t="inlineStr"/>
       <c r="K25" s="3" t="inlineStr">
         <is>
-          <t>11.3 MJ/m2</t>
+          <t>11.5 MJ/m2</t>
         </is>
       </c>
       <c r="L25" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="O25" s="3" t="inlineStr">
         <is>
-          <t>10.4 °C</t>
+          <t>10.6 °C</t>
         </is>
       </c>
     </row>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:36</t>
+          <t>2026-02-07 17:28:52</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
@@ -2252,7 +2252,7 @@
       <c r="G26" s="3" t="inlineStr"/>
       <c r="H26" s="3" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>74%</t>
         </is>
       </c>
       <c r="I26" s="3" t="inlineStr">
@@ -2263,12 +2263,12 @@
       <c r="J26" s="3" t="inlineStr"/>
       <c r="K26" s="3" t="inlineStr">
         <is>
-          <t>12.6 MJ/m2</t>
+          <t>12.7 MJ/m2</t>
         </is>
       </c>
       <c r="L26" s="3" t="inlineStr">
         <is>
-          <t>28.8 km/h - 320º 12:50 TU</t>
+          <t>38.2 km/h - 305º 16:24 TU</t>
         </is>
       </c>
       <c r="M26" s="3" t="inlineStr">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:38</t>
+          <t>2026-02-07 17:28:54</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
@@ -2321,7 +2321,7 @@
       <c r="G27" s="3" t="inlineStr"/>
       <c r="H27" s="3" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="I27" s="3" t="inlineStr">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="O27" s="3" t="inlineStr">
         <is>
-          <t>7.8 °C</t>
+          <t>7.9 °C</t>
         </is>
       </c>
     </row>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:41</t>
+          <t>2026-02-07 17:28:56</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
@@ -2393,7 +2393,7 @@
       <c r="J28" s="3" t="inlineStr"/>
       <c r="K28" s="3" t="inlineStr">
         <is>
-          <t>10.6 MJ/m2</t>
+          <t>10.8 MJ/m2</t>
         </is>
       </c>
       <c r="L28" s="3" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="O28" s="3" t="inlineStr">
         <is>
-          <t>11.8 °C</t>
+          <t>11.9 °C</t>
         </is>
       </c>
     </row>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:43</t>
+          <t>2026-02-07 17:28:58</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
@@ -2461,12 +2461,12 @@
       </c>
       <c r="J29" s="3" t="inlineStr">
         <is>
-          <t>1004.3 hPa</t>
+          <t>1004.5 hPa</t>
         </is>
       </c>
       <c r="K29" s="3" t="inlineStr">
         <is>
-          <t>11.9 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L29" s="3" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="O29" s="3" t="inlineStr">
         <is>
-          <t>12.5 °C</t>
+          <t>12.6 °C</t>
         </is>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:46</t>
+          <t>2026-02-07 17:29:01</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
@@ -2534,12 +2534,12 @@
       </c>
       <c r="J30" s="3" t="inlineStr">
         <is>
-          <t>1004.5 hPa</t>
+          <t>1004.7 hPa</t>
         </is>
       </c>
       <c r="K30" s="3" t="inlineStr">
         <is>
-          <t>12.6 MJ/m2</t>
+          <t>12.7 MJ/m2</t>
         </is>
       </c>
       <c r="L30" s="3" t="inlineStr">
@@ -2559,7 +2559,7 @@
       </c>
       <c r="O30" s="3" t="inlineStr">
         <is>
-          <t>10.9 °C</t>
+          <t>11.0 °C</t>
         </is>
       </c>
     </row>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:48</t>
+          <t>2026-02-07 17:29:03</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
@@ -2597,7 +2597,7 @@
       <c r="G31" s="3" t="inlineStr"/>
       <c r="H31" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I31" s="3" t="inlineStr">
@@ -2608,7 +2608,7 @@
       <c r="J31" s="3" t="inlineStr"/>
       <c r="K31" s="3" t="inlineStr">
         <is>
-          <t>12.2 MJ/m2</t>
+          <t>12.4 MJ/m2</t>
         </is>
       </c>
       <c r="L31" s="3" t="inlineStr">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="O31" s="3" t="inlineStr">
         <is>
-          <t>5.4 °C</t>
+          <t>5.5 °C</t>
         </is>
       </c>
     </row>
@@ -2655,7 +2655,7 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:51</t>
+          <t>2026-02-07 17:29:06</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
@@ -2666,7 +2666,7 @@
       <c r="G32" s="3" t="inlineStr"/>
       <c r="H32" s="3" t="inlineStr">
         <is>
-          <t>52%</t>
+          <t>53%</t>
         </is>
       </c>
       <c r="I32" s="3" t="inlineStr">
@@ -2677,7 +2677,7 @@
       <c r="J32" s="3" t="inlineStr"/>
       <c r="K32" s="3" t="inlineStr">
         <is>
-          <t>12.4 MJ/m2</t>
+          <t>12.5 MJ/m2</t>
         </is>
       </c>
       <c r="L32" s="3" t="inlineStr">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="O32" s="3" t="inlineStr">
         <is>
-          <t>11.8 °C</t>
+          <t>11.9 °C</t>
         </is>
       </c>
     </row>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:53</t>
+          <t>2026-02-07 17:29:08</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
@@ -2735,7 +2735,7 @@
       <c r="G33" s="3" t="inlineStr"/>
       <c r="H33" s="3" t="inlineStr">
         <is>
-          <t>76%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="I33" s="3" t="inlineStr">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="O33" s="3" t="inlineStr">
         <is>
-          <t>8.1 °C</t>
+          <t>8.2 °C</t>
         </is>
       </c>
     </row>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:55</t>
+          <t>2026-02-07 17:29:11</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
@@ -2796,7 +2796,7 @@
       <c r="G34" s="3" t="inlineStr"/>
       <c r="H34" s="3" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>74%</t>
         </is>
       </c>
       <c r="I34" s="3" t="inlineStr">
@@ -2807,7 +2807,7 @@
       <c r="J34" s="3" t="inlineStr"/>
       <c r="K34" s="3" t="inlineStr">
         <is>
-          <t>11.5 MJ/m2</t>
+          <t>11.7 MJ/m2</t>
         </is>
       </c>
       <c r="L34" s="3" t="inlineStr">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="O34" s="3" t="inlineStr">
         <is>
-          <t>8.8 °C</t>
+          <t>9.0 °C</t>
         </is>
       </c>
     </row>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:37:58</t>
+          <t>2026-02-07 17:29:13</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
@@ -2865,7 +2865,7 @@
       <c r="G35" s="3" t="inlineStr"/>
       <c r="H35" s="3" t="inlineStr">
         <is>
-          <t>68%</t>
+          <t>67%</t>
         </is>
       </c>
       <c r="I35" s="3" t="inlineStr">
@@ -2875,12 +2875,12 @@
       </c>
       <c r="J35" s="3" t="inlineStr">
         <is>
-          <t>1003.8 hPa</t>
+          <t>1003.9 hPa</t>
         </is>
       </c>
       <c r="K35" s="3" t="inlineStr">
         <is>
-          <t>11.5 MJ/m2</t>
+          <t>11.7 MJ/m2</t>
         </is>
       </c>
       <c r="L35" s="3" t="inlineStr">
@@ -2900,7 +2900,7 @@
       </c>
       <c r="O35" s="3" t="inlineStr">
         <is>
-          <t>10.7 °C</t>
+          <t>10.9 °C</t>
         </is>
       </c>
     </row>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:00</t>
+          <t>2026-02-07 17:29:16</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
@@ -2938,7 +2938,7 @@
       <c r="G36" s="3" t="inlineStr"/>
       <c r="H36" s="3" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="I36" s="3" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="O36" s="3" t="inlineStr">
         <is>
-          <t>3.7 °C</t>
+          <t>3.8 °C</t>
         </is>
       </c>
     </row>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:03</t>
+          <t>2026-02-07 17:29:18</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
@@ -3009,12 +3009,12 @@
       </c>
       <c r="J37" s="3" t="inlineStr">
         <is>
-          <t>1005.6 hPa</t>
+          <t>1005.7 hPa</t>
         </is>
       </c>
       <c r="K37" s="3" t="inlineStr">
         <is>
-          <t>12.4 MJ/m2</t>
+          <t>12.6 MJ/m2</t>
         </is>
       </c>
       <c r="L37" s="3" t="inlineStr">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="O37" s="3" t="inlineStr">
         <is>
-          <t>11.0 °C</t>
+          <t>11.1 °C</t>
         </is>
       </c>
     </row>
@@ -3061,7 +3061,7 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:05</t>
+          <t>2026-02-07 17:29:20</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
@@ -3072,7 +3072,7 @@
       <c r="G38" s="3" t="inlineStr"/>
       <c r="H38" s="3" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="I38" s="3" t="inlineStr">
@@ -3083,7 +3083,7 @@
       <c r="J38" s="3" t="inlineStr"/>
       <c r="K38" s="3" t="inlineStr">
         <is>
-          <t>12.1 MJ/m2</t>
+          <t>12.3 MJ/m2</t>
         </is>
       </c>
       <c r="L38" s="3" t="inlineStr">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="O38" s="3" t="inlineStr">
         <is>
-          <t>7.5 °C</t>
+          <t>7.6 °C</t>
         </is>
       </c>
     </row>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:07</t>
+          <t>2026-02-07 17:29:23</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
@@ -3141,7 +3141,7 @@
       <c r="G39" s="3" t="inlineStr"/>
       <c r="H39" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I39" s="3" t="inlineStr">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="K39" s="3" t="inlineStr">
         <is>
-          <t>12.1 MJ/m2</t>
+          <t>12.3 MJ/m2</t>
         </is>
       </c>
       <c r="L39" s="3" t="inlineStr">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="O39" s="3" t="inlineStr">
         <is>
-          <t>7.8 °C</t>
+          <t>7.9 °C</t>
         </is>
       </c>
     </row>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:10</t>
+          <t>2026-02-07 17:29:25</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
@@ -3214,7 +3214,7 @@
       <c r="G40" s="3" t="inlineStr"/>
       <c r="H40" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I40" s="3" t="inlineStr">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="O40" s="3" t="inlineStr">
         <is>
-          <t>10.4 °C</t>
+          <t>10.6 °C</t>
         </is>
       </c>
     </row>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:12</t>
+          <t>2026-02-07 17:29:27</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
@@ -3275,7 +3275,7 @@
       <c r="G41" s="3" t="inlineStr"/>
       <c r="H41" s="3" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="I41" s="3" t="inlineStr">
@@ -3285,12 +3285,12 @@
       </c>
       <c r="J41" s="3" t="inlineStr">
         <is>
-          <t>1006.5 hPa</t>
+          <t>1006.6 hPa</t>
         </is>
       </c>
       <c r="K41" s="3" t="inlineStr">
         <is>
-          <t>12.2 MJ/m2</t>
+          <t>12.3 MJ/m2</t>
         </is>
       </c>
       <c r="L41" s="3" t="inlineStr">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="O41" s="3" t="inlineStr">
         <is>
-          <t>6.1 °C</t>
+          <t>6.2 °C</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:14</t>
+          <t>2026-02-07 17:29:30</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="K42" s="3" t="inlineStr">
         <is>
-          <t>12.0 MJ/m2</t>
+          <t>12.1 MJ/m2</t>
         </is>
       </c>
       <c r="L42" s="3" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:17</t>
+          <t>2026-02-07 17:29:32</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="K43" s="3" t="inlineStr">
         <is>
-          <t>11.0 MJ/m2</t>
+          <t>11.1 MJ/m2</t>
         </is>
       </c>
       <c r="L43" s="3" t="inlineStr">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="O43" s="3" t="inlineStr">
         <is>
-          <t>8.6 °C</t>
+          <t>8.7 °C</t>
         </is>
       </c>
     </row>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:19</t>
+          <t>2026-02-07 17:29:35</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
@@ -3494,7 +3494,7 @@
       <c r="G44" s="3" t="inlineStr"/>
       <c r="H44" s="3" t="inlineStr">
         <is>
-          <t>53%</t>
+          <t>54%</t>
         </is>
       </c>
       <c r="I44" s="3" t="inlineStr">
@@ -3504,12 +3504,12 @@
       </c>
       <c r="J44" s="3" t="inlineStr">
         <is>
-          <t>1006.2 hPa</t>
+          <t>1006.3 hPa</t>
         </is>
       </c>
       <c r="K44" s="3" t="inlineStr">
         <is>
-          <t>11.8 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L44" s="3" t="inlineStr">
@@ -3556,7 +3556,7 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:22</t>
+          <t>2026-02-07 17:29:37</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="H45" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="I45" s="3" t="inlineStr">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="K45" s="3" t="inlineStr">
         <is>
-          <t>8.6 MJ/m2</t>
+          <t>8.8 MJ/m2</t>
         </is>
       </c>
       <c r="L45" s="3" t="inlineStr">
@@ -3606,7 +3606,7 @@
       </c>
       <c r="O45" s="3" t="inlineStr">
         <is>
-          <t>3.3 °C</t>
+          <t>3.4 °C</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:24</t>
+          <t>2026-02-07 17:29:40</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
@@ -3644,7 +3644,7 @@
       <c r="G46" s="3" t="inlineStr"/>
       <c r="H46" s="3" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="I46" s="3" t="inlineStr">
@@ -3655,7 +3655,7 @@
       <c r="J46" s="3" t="inlineStr"/>
       <c r="K46" s="3" t="inlineStr">
         <is>
-          <t>12.9 MJ/m2</t>
+          <t>13.1 MJ/m2</t>
         </is>
       </c>
       <c r="L46" s="3" t="inlineStr">
@@ -3675,7 +3675,7 @@
       </c>
       <c r="O46" s="3" t="inlineStr">
         <is>
-          <t>9.1 °C</t>
+          <t>9.2 °C</t>
         </is>
       </c>
     </row>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:26</t>
+          <t>2026-02-07 17:29:42</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
@@ -3713,7 +3713,7 @@
       <c r="G47" s="3" t="inlineStr"/>
       <c r="H47" s="3" t="inlineStr">
         <is>
-          <t>72%</t>
+          <t>71%</t>
         </is>
       </c>
       <c r="I47" s="3" t="inlineStr">
@@ -3740,7 +3740,7 @@
       </c>
       <c r="O47" s="3" t="inlineStr">
         <is>
-          <t>9.3 °C</t>
+          <t>9.5 °C</t>
         </is>
       </c>
     </row>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:29</t>
+          <t>2026-02-07 17:29:44</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
@@ -3789,7 +3789,7 @@
       <c r="J48" s="3" t="inlineStr"/>
       <c r="K48" s="3" t="inlineStr">
         <is>
-          <t>12.5 MJ/m2</t>
+          <t>12.6 MJ/m2</t>
         </is>
       </c>
       <c r="L48" s="3" t="inlineStr">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:31</t>
+          <t>2026-02-07 17:29:47</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
@@ -3847,7 +3847,7 @@
       <c r="G49" s="3" t="inlineStr"/>
       <c r="H49" s="3" t="inlineStr">
         <is>
-          <t>51%</t>
+          <t>52%</t>
         </is>
       </c>
       <c r="I49" s="3" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="K49" s="3" t="inlineStr">
         <is>
-          <t>11.8 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L49" s="3" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:34</t>
+          <t>2026-02-07 17:29:49</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
@@ -3920,7 +3920,7 @@
       <c r="G50" s="3" t="inlineStr"/>
       <c r="H50" s="3" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I50" s="3" t="inlineStr">
@@ -3931,7 +3931,7 @@
       <c r="J50" s="3" t="inlineStr"/>
       <c r="K50" s="3" t="inlineStr">
         <is>
-          <t>11.9 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L50" s="3" t="inlineStr">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="O50" s="3" t="inlineStr">
         <is>
-          <t>7.7 °C</t>
+          <t>7.9 °C</t>
         </is>
       </c>
     </row>
@@ -3978,7 +3978,7 @@
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:36</t>
+          <t>2026-02-07 17:29:52</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
@@ -3989,7 +3989,7 @@
       <c r="G51" s="3" t="inlineStr"/>
       <c r="H51" s="3" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I51" s="3" t="inlineStr">
@@ -4004,7 +4004,7 @@
       </c>
       <c r="K51" s="3" t="inlineStr">
         <is>
-          <t>6.9 MJ/m2</t>
+          <t>7.0 MJ/m2</t>
         </is>
       </c>
       <c r="L51" s="3" t="inlineStr">
@@ -4024,7 +4024,7 @@
       </c>
       <c r="O51" s="3" t="inlineStr">
         <is>
-          <t>4.2 °C</t>
+          <t>4.3 °C</t>
         </is>
       </c>
     </row>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:39</t>
+          <t>2026-02-07 17:29:54</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
@@ -4073,7 +4073,7 @@
       <c r="J52" s="3" t="inlineStr"/>
       <c r="K52" s="3" t="inlineStr">
         <is>
-          <t>12.3 MJ/m2</t>
+          <t>12.4 MJ/m2</t>
         </is>
       </c>
       <c r="L52" s="3" t="inlineStr">
@@ -4093,7 +4093,7 @@
       </c>
       <c r="O52" s="3" t="inlineStr">
         <is>
-          <t>12.3 °C</t>
+          <t>12.4 °C</t>
         </is>
       </c>
     </row>
@@ -4120,7 +4120,7 @@
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:41</t>
+          <t>2026-02-07 17:29:57</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:44</t>
+          <t>2026-02-07 17:29:59</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
@@ -4172,7 +4172,7 @@
       <c r="G54" s="3" t="inlineStr"/>
       <c r="H54" s="3" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>51%</t>
         </is>
       </c>
       <c r="I54" s="3" t="inlineStr">
@@ -4182,12 +4182,12 @@
       </c>
       <c r="J54" s="3" t="inlineStr">
         <is>
-          <t>1005.1 hPa</t>
+          <t>1005.3 hPa</t>
         </is>
       </c>
       <c r="K54" s="3" t="inlineStr">
         <is>
-          <t>12.4 MJ/m2</t>
+          <t>12.6 MJ/m2</t>
         </is>
       </c>
       <c r="L54" s="3" t="inlineStr">
@@ -4207,7 +4207,7 @@
       </c>
       <c r="O54" s="3" t="inlineStr">
         <is>
-          <t>12.9 °C</t>
+          <t>13.0 °C</t>
         </is>
       </c>
     </row>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:46</t>
+          <t>2026-02-07 17:30:01</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
@@ -4255,12 +4255,12 @@
       </c>
       <c r="J55" s="3" t="inlineStr">
         <is>
-          <t>1006.2 hPa</t>
+          <t>1006.3 hPa</t>
         </is>
       </c>
       <c r="K55" s="3" t="inlineStr">
         <is>
-          <t>12.0 MJ/m2</t>
+          <t>12.1 MJ/m2</t>
         </is>
       </c>
       <c r="L55" s="3" t="inlineStr">
@@ -4280,7 +4280,7 @@
       </c>
       <c r="O55" s="3" t="inlineStr">
         <is>
-          <t>12.0 °C</t>
+          <t>12.1 °C</t>
         </is>
       </c>
     </row>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:49</t>
+          <t>2026-02-07 17:30:04</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
@@ -4318,7 +4318,7 @@
       <c r="G56" s="3" t="inlineStr"/>
       <c r="H56" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I56" s="3" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="O56" s="3" t="inlineStr">
         <is>
-          <t>7.8 °C</t>
+          <t>8.0 °C</t>
         </is>
       </c>
     </row>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:51</t>
+          <t>2026-02-07 17:30:06</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
@@ -4383,7 +4383,7 @@
       <c r="G57" s="3" t="inlineStr"/>
       <c r="H57" s="3" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="I57" s="3" t="inlineStr">
@@ -4393,12 +4393,12 @@
       </c>
       <c r="J57" s="3" t="inlineStr">
         <is>
-          <t>1005.4 hPa</t>
+          <t>1005.5 hPa</t>
         </is>
       </c>
       <c r="K57" s="3" t="inlineStr">
         <is>
-          <t>12.1 MJ/m2</t>
+          <t>12.3 MJ/m2</t>
         </is>
       </c>
       <c r="L57" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="O57" s="3" t="inlineStr">
         <is>
-          <t>9.4 °C</t>
+          <t>9.5 °C</t>
         </is>
       </c>
     </row>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:53</t>
+          <t>2026-02-07 17:30:09</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
@@ -4456,7 +4456,7 @@
       <c r="G58" s="3" t="inlineStr"/>
       <c r="H58" s="3" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="I58" s="3" t="inlineStr">
@@ -4467,7 +4467,7 @@
       <c r="J58" s="3" t="inlineStr"/>
       <c r="K58" s="3" t="inlineStr">
         <is>
-          <t>12.2 MJ/m2</t>
+          <t>12.4 MJ/m2</t>
         </is>
       </c>
       <c r="L58" s="3" t="inlineStr">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="O58" s="3" t="inlineStr">
         <is>
-          <t>6.8 °C</t>
+          <t>6.9 °C</t>
         </is>
       </c>
     </row>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:56</t>
+          <t>2026-02-07 17:30:11</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="O59" s="3" t="inlineStr">
         <is>
-          <t>11.4 °C</t>
+          <t>11.5 °C</t>
         </is>
       </c>
     </row>
@@ -4575,7 +4575,7 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:38:58</t>
+          <t>2026-02-07 17:30:13</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
@@ -4590,7 +4590,7 @@
       </c>
       <c r="H60" s="3" t="inlineStr">
         <is>
-          <t>61%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="I60" s="3" t="inlineStr">
@@ -4601,12 +4601,12 @@
       <c r="J60" s="3" t="inlineStr"/>
       <c r="K60" s="3" t="inlineStr">
         <is>
-          <t>8.4 MJ/m2</t>
+          <t>8.6 MJ/m2</t>
         </is>
       </c>
       <c r="L60" s="3" t="inlineStr">
         <is>
-          <t>34.2 km/h - 242º 15:22 TU</t>
+          <t>49.7 km/h - 249º 16:23 TU</t>
         </is>
       </c>
       <c r="M60" s="3" t="inlineStr">
@@ -4621,7 +4621,7 @@
       </c>
       <c r="O60" s="3" t="inlineStr">
         <is>
-          <t>-5.8 °C</t>
+          <t>-5.7 °C</t>
         </is>
       </c>
     </row>
@@ -4648,7 +4648,7 @@
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:01</t>
+          <t>2026-02-07 17:30:16</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
@@ -4659,7 +4659,7 @@
       <c r="G61" s="3" t="inlineStr"/>
       <c r="H61" s="3" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="I61" s="3" t="inlineStr">
@@ -4674,7 +4674,7 @@
       </c>
       <c r="K61" s="3" t="inlineStr">
         <is>
-          <t>11.8 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L61" s="3" t="inlineStr">
@@ -4694,7 +4694,7 @@
       </c>
       <c r="O61" s="3" t="inlineStr">
         <is>
-          <t>8.6 °C</t>
+          <t>8.7 °C</t>
         </is>
       </c>
     </row>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:03</t>
+          <t>2026-02-07 17:30:18</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
@@ -4732,7 +4732,7 @@
       <c r="G62" s="3" t="inlineStr"/>
       <c r="H62" s="3" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="I62" s="3" t="inlineStr">
@@ -4755,7 +4755,7 @@
       </c>
       <c r="O62" s="3" t="inlineStr">
         <is>
-          <t>10.7 °C</t>
+          <t>10.8 °C</t>
         </is>
       </c>
     </row>
@@ -4782,7 +4782,7 @@
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:05</t>
+          <t>2026-02-07 17:30:21</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="H63" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I63" s="3" t="inlineStr">
@@ -4855,7 +4855,7 @@
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:07</t>
+          <t>2026-02-07 17:30:23</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
@@ -4876,12 +4876,12 @@
       </c>
       <c r="J64" s="3" t="inlineStr">
         <is>
-          <t>1005.3 hPa</t>
+          <t>1005.4 hPa</t>
         </is>
       </c>
       <c r="K64" s="3" t="inlineStr">
         <is>
-          <t>12.0 MJ/m2</t>
+          <t>12.1 MJ/m2</t>
         </is>
       </c>
       <c r="L64" s="3" t="inlineStr">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:10</t>
+          <t>2026-02-07 17:30:26</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
@@ -4962,7 +4962,7 @@
       </c>
       <c r="O65" s="3" t="inlineStr">
         <is>
-          <t>8.8 °C</t>
+          <t>9.0 °C</t>
         </is>
       </c>
     </row>
@@ -4989,7 +4989,7 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:12</t>
+          <t>2026-02-07 17:30:28</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
@@ -5000,7 +5000,7 @@
       <c r="G66" s="3" t="inlineStr"/>
       <c r="H66" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I66" s="3" t="inlineStr">
@@ -5050,7 +5050,7 @@
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:15</t>
+          <t>2026-02-07 17:30:30</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
@@ -5061,7 +5061,7 @@
       <c r="G67" s="3" t="inlineStr"/>
       <c r="H67" s="3" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="I67" s="3" t="inlineStr">
@@ -5119,7 +5119,7 @@
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:17</t>
+          <t>2026-02-07 17:30:33</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
@@ -5130,7 +5130,7 @@
       <c r="G68" s="3" t="inlineStr"/>
       <c r="H68" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I68" s="3" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="O68" s="3" t="inlineStr">
         <is>
-          <t>7.3 °C</t>
+          <t>7.4 °C</t>
         </is>
       </c>
     </row>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:19</t>
+          <t>2026-02-07 17:30:35</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
@@ -5234,7 +5234,7 @@
       </c>
       <c r="O69" s="3" t="inlineStr">
         <is>
-          <t>9.9 °C</t>
+          <t>10.0 °C</t>
         </is>
       </c>
     </row>
@@ -5261,7 +5261,7 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:21</t>
+          <t>2026-02-07 17:30:37</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:24</t>
+          <t>2026-02-07 17:30:40</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
@@ -5344,7 +5344,7 @@
       <c r="J71" s="3" t="inlineStr"/>
       <c r="K71" s="3" t="inlineStr">
         <is>
-          <t>12.0 MJ/m2</t>
+          <t>12.1 MJ/m2</t>
         </is>
       </c>
       <c r="L71" s="3" t="inlineStr">
@@ -5364,7 +5364,7 @@
       </c>
       <c r="O71" s="3" t="inlineStr">
         <is>
-          <t>8.1 °C</t>
+          <t>8.2 °C</t>
         </is>
       </c>
     </row>
@@ -5391,7 +5391,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:26</t>
+          <t>2026-02-07 17:30:42</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
@@ -5402,7 +5402,7 @@
       <c r="G72" s="3" t="inlineStr"/>
       <c r="H72" s="3" t="inlineStr">
         <is>
-          <t>58%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="I72" s="3" t="inlineStr">
@@ -5425,7 +5425,7 @@
       </c>
       <c r="O72" s="3" t="inlineStr">
         <is>
-          <t>11.0 °C</t>
+          <t>11.1 °C</t>
         </is>
       </c>
     </row>
@@ -5452,7 +5452,7 @@
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:29</t>
+          <t>2026-02-07 17:30:45</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
@@ -5463,7 +5463,7 @@
       <c r="G73" s="3" t="inlineStr"/>
       <c r="H73" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I73" s="3" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="J73" s="3" t="inlineStr">
         <is>
-          <t>1005.1 hPa</t>
+          <t>1005.2 hPa</t>
         </is>
       </c>
       <c r="K73" s="3" t="inlineStr">
@@ -5525,7 +5525,7 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:31</t>
+          <t>2026-02-07 17:30:47</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
@@ -5559,7 +5559,7 @@
       </c>
       <c r="O74" s="3" t="inlineStr">
         <is>
-          <t>3.6 °C</t>
+          <t>3.7 °C</t>
         </is>
       </c>
     </row>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:33</t>
+          <t>2026-02-07 17:30:49</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
@@ -5597,7 +5597,7 @@
       <c r="G75" s="3" t="inlineStr"/>
       <c r="H75" s="3" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>68%</t>
         </is>
       </c>
       <c r="I75" s="3" t="inlineStr">
@@ -5659,7 +5659,7 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:36</t>
+          <t>2026-02-07 17:30:52</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
@@ -5705,7 +5705,7 @@
       </c>
       <c r="O76" s="3" t="inlineStr">
         <is>
-          <t>5.9 °C</t>
+          <t>6.0 °C</t>
         </is>
       </c>
     </row>
@@ -5732,7 +5732,7 @@
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:38</t>
+          <t>2026-02-07 17:30:54</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
@@ -5743,7 +5743,7 @@
       <c r="G77" s="3" t="inlineStr"/>
       <c r="H77" s="3" t="inlineStr">
         <is>
-          <t>47%</t>
+          <t>48%</t>
         </is>
       </c>
       <c r="I77" s="3" t="inlineStr">
@@ -5754,7 +5754,7 @@
       <c r="J77" s="3" t="inlineStr"/>
       <c r="K77" s="3" t="inlineStr">
         <is>
-          <t>11.9 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L77" s="3" t="inlineStr">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:41</t>
+          <t>2026-02-07 17:30:57</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
@@ -5812,7 +5812,7 @@
       <c r="G78" s="3" t="inlineStr"/>
       <c r="H78" s="3" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="I78" s="3" t="inlineStr">
@@ -5870,7 +5870,7 @@
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:43</t>
+          <t>2026-02-07 17:30:59</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
@@ -5891,7 +5891,7 @@
       </c>
       <c r="J79" s="3" t="inlineStr">
         <is>
-          <t>1006.7 hPa</t>
+          <t>1006.8 hPa</t>
         </is>
       </c>
       <c r="K79" s="3" t="inlineStr">
@@ -5943,7 +5943,7 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:46</t>
+          <t>2026-02-07 17:31:02</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
@@ -5954,7 +5954,7 @@
       <c r="G80" s="3" t="inlineStr"/>
       <c r="H80" s="3" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="I80" s="3" t="inlineStr">
@@ -5965,7 +5965,7 @@
       <c r="J80" s="3" t="inlineStr"/>
       <c r="K80" s="3" t="inlineStr">
         <is>
-          <t>6.7 MJ/m2</t>
+          <t>6.8 MJ/m2</t>
         </is>
       </c>
       <c r="L80" s="3" t="inlineStr">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="O80" s="3" t="inlineStr">
         <is>
-          <t>4.0 °C</t>
+          <t>4.1 °C</t>
         </is>
       </c>
     </row>
@@ -6012,7 +6012,7 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:48</t>
+          <t>2026-02-07 17:31:04</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
@@ -6033,7 +6033,7 @@
       </c>
       <c r="J81" s="3" t="inlineStr">
         <is>
-          <t>1003.5 hPa</t>
+          <t>1003.6 hPa</t>
         </is>
       </c>
       <c r="K81" s="3" t="inlineStr">
@@ -6058,7 +6058,7 @@
       </c>
       <c r="O81" s="3" t="inlineStr">
         <is>
-          <t>10.4 °C</t>
+          <t>10.5 °C</t>
         </is>
       </c>
     </row>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:51</t>
+          <t>2026-02-07 17:31:07</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:53</t>
+          <t>2026-02-07 17:31:09</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
@@ -6172,7 +6172,7 @@
       <c r="J83" s="3" t="inlineStr"/>
       <c r="K83" s="3" t="inlineStr">
         <is>
-          <t>8.3 MJ/m2</t>
+          <t>8.4 MJ/m2</t>
         </is>
       </c>
       <c r="L83" s="3" t="inlineStr">
@@ -6219,7 +6219,7 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:55</t>
+          <t>2026-02-07 17:31:11</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
@@ -6288,7 +6288,7 @@
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:39:58</t>
+          <t>2026-02-07 17:31:14</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
@@ -6322,7 +6322,7 @@
       </c>
       <c r="O85" s="3" t="inlineStr">
         <is>
-          <t>7.3 °C</t>
+          <t>7.4 °C</t>
         </is>
       </c>
     </row>
@@ -6349,7 +6349,7 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:00</t>
+          <t>2026-02-07 17:31:16</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
@@ -6422,7 +6422,7 @@
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:03</t>
+          <t>2026-02-07 17:31:19</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
@@ -6443,7 +6443,7 @@
       </c>
       <c r="J87" s="3" t="inlineStr">
         <is>
-          <t>1005.2 hPa</t>
+          <t>1005.3 hPa</t>
         </is>
       </c>
       <c r="K87" s="3" t="inlineStr"/>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:05</t>
+          <t>2026-02-07 17:31:21</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:07</t>
+          <t>2026-02-07 17:31:23</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
@@ -6543,7 +6543,7 @@
       <c r="G89" s="3" t="inlineStr"/>
       <c r="H89" s="3" t="inlineStr">
         <is>
-          <t>61%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="I89" s="3" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:10</t>
+          <t>2026-02-07 17:31:26</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
@@ -6651,7 +6651,7 @@
       </c>
       <c r="O90" s="3" t="inlineStr">
         <is>
-          <t>5.0 °C</t>
+          <t>5.1 °C</t>
         </is>
       </c>
     </row>
@@ -6678,7 +6678,7 @@
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:12</t>
+          <t>2026-02-07 17:31:29</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
@@ -6689,7 +6689,7 @@
       <c r="G91" s="3" t="inlineStr"/>
       <c r="H91" s="3" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="I91" s="3" t="inlineStr">
@@ -6700,7 +6700,7 @@
       <c r="J91" s="3" t="inlineStr"/>
       <c r="K91" s="3" t="inlineStr">
         <is>
-          <t>10.8 MJ/m2</t>
+          <t>11.0 MJ/m2</t>
         </is>
       </c>
       <c r="L91" s="3" t="inlineStr">
@@ -6720,7 +6720,7 @@
       </c>
       <c r="O91" s="3" t="inlineStr">
         <is>
-          <t>9.9 °C</t>
+          <t>10.1 °C</t>
         </is>
       </c>
     </row>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:15</t>
+          <t>2026-02-07 17:31:31</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
@@ -6812,7 +6812,7 @@
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:17</t>
+          <t>2026-02-07 17:31:33</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
@@ -6881,7 +6881,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:20</t>
+          <t>2026-02-07 17:31:36</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
       </c>
       <c r="O94" s="3" t="inlineStr">
         <is>
-          <t>-5.6 °C</t>
+          <t>-5.7 °C</t>
         </is>
       </c>
     </row>
@@ -6954,7 +6954,7 @@
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:22</t>
+          <t>2026-02-07 17:31:38</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
@@ -6980,7 +6980,7 @@
       </c>
       <c r="K95" s="3" t="inlineStr">
         <is>
-          <t>11.7 MJ/m2</t>
+          <t>11.8 MJ/m2</t>
         </is>
       </c>
       <c r="L95" s="3" t="inlineStr">
@@ -7000,7 +7000,7 @@
       </c>
       <c r="O95" s="3" t="inlineStr">
         <is>
-          <t>8.7 °C</t>
+          <t>8.8 °C</t>
         </is>
       </c>
     </row>
@@ -7027,7 +7027,7 @@
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:25</t>
+          <t>2026-02-07 17:31:41</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
@@ -7038,7 +7038,7 @@
       <c r="G96" s="3" t="inlineStr"/>
       <c r="H96" s="3" t="inlineStr">
         <is>
-          <t>58%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="I96" s="3" t="inlineStr">
@@ -7049,7 +7049,7 @@
       <c r="J96" s="3" t="inlineStr"/>
       <c r="K96" s="3" t="inlineStr">
         <is>
-          <t>11.9 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L96" s="3" t="inlineStr">
@@ -7096,7 +7096,7 @@
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:27</t>
+          <t>2026-02-07 17:31:43</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="H97" s="3" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="I97" s="3" t="inlineStr">
@@ -7122,7 +7122,7 @@
       <c r="J97" s="3" t="inlineStr"/>
       <c r="K97" s="3" t="inlineStr">
         <is>
-          <t>6.5 MJ/m2</t>
+          <t>6.6 MJ/m2</t>
         </is>
       </c>
       <c r="L97" s="3" t="inlineStr">
@@ -7169,7 +7169,7 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:30</t>
+          <t>2026-02-07 17:31:45</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
@@ -7191,7 +7191,7 @@
       <c r="J98" s="3" t="inlineStr"/>
       <c r="K98" s="3" t="inlineStr">
         <is>
-          <t>11.0 MJ/m2</t>
+          <t>11.1 MJ/m2</t>
         </is>
       </c>
       <c r="L98" s="3" t="inlineStr">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:32</t>
+          <t>2026-02-07 17:31:48</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
@@ -7280,7 +7280,7 @@
       </c>
       <c r="O99" s="3" t="inlineStr">
         <is>
-          <t>8.3 °C</t>
+          <t>8.4 °C</t>
         </is>
       </c>
     </row>
@@ -7307,7 +7307,7 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:34</t>
+          <t>2026-02-07 17:31:50</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
@@ -7318,7 +7318,7 @@
       <c r="G100" s="3" t="inlineStr"/>
       <c r="H100" s="3" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I100" s="3" t="inlineStr">
@@ -7353,7 +7353,7 @@
       </c>
       <c r="O100" s="3" t="inlineStr">
         <is>
-          <t>7.1 °C</t>
+          <t>7.3 °C</t>
         </is>
       </c>
     </row>
@@ -7380,7 +7380,7 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:37</t>
+          <t>2026-02-07 17:31:53</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="O101" s="3" t="inlineStr">
         <is>
-          <t>7.0 °C</t>
+          <t>7.1 °C</t>
         </is>
       </c>
     </row>
@@ -7449,7 +7449,7 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:39</t>
+          <t>2026-02-07 17:31:55</t>
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
@@ -7460,7 +7460,7 @@
       <c r="G102" s="3" t="inlineStr"/>
       <c r="H102" s="3" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="I102" s="3" t="inlineStr">
@@ -7480,7 +7480,7 @@
       </c>
       <c r="L102" s="3" t="inlineStr">
         <is>
-          <t>34.9 km/h - 217º 10:49 TU</t>
+          <t>36.7 km/h - 253º 16:39 TU</t>
         </is>
       </c>
       <c r="M102" s="3" t="inlineStr">
@@ -7495,7 +7495,7 @@
       </c>
       <c r="O102" s="3" t="inlineStr">
         <is>
-          <t>11.6 °C</t>
+          <t>11.7 °C</t>
         </is>
       </c>
     </row>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:42</t>
+          <t>2026-02-07 17:31:58</t>
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
@@ -7568,7 +7568,7 @@
       </c>
       <c r="O103" s="3" t="inlineStr">
         <is>
-          <t>6.9 °C</t>
+          <t>7.0 °C</t>
         </is>
       </c>
     </row>
@@ -7595,7 +7595,7 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:44</t>
+          <t>2026-02-07 17:32:00</t>
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
@@ -7606,7 +7606,7 @@
       <c r="G104" s="3" t="inlineStr"/>
       <c r="H104" s="3" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>46%</t>
         </is>
       </c>
       <c r="I104" s="3" t="inlineStr">
@@ -7621,7 +7621,7 @@
       </c>
       <c r="K104" s="3" t="inlineStr">
         <is>
-          <t>11.4 MJ/m2</t>
+          <t>11.5 MJ/m2</t>
         </is>
       </c>
       <c r="L104" s="3" t="inlineStr">
@@ -7668,7 +7668,7 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:47</t>
+          <t>2026-02-07 17:32:03</t>
         </is>
       </c>
       <c r="F105" s="3" t="inlineStr">
@@ -7710,7 +7710,7 @@
       </c>
       <c r="O105" s="3" t="inlineStr">
         <is>
-          <t>6.3 °C</t>
+          <t>6.4 °C</t>
         </is>
       </c>
     </row>
@@ -7737,7 +7737,7 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:49</t>
+          <t>2026-02-07 17:32:05</t>
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
@@ -7802,7 +7802,7 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:51</t>
+          <t>2026-02-07 17:32:08</t>
         </is>
       </c>
       <c r="F107" s="3" t="inlineStr">
@@ -7871,7 +7871,7 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:54</t>
+          <t>2026-02-07 17:32:10</t>
         </is>
       </c>
       <c r="F108" s="3" t="inlineStr">
@@ -7886,7 +7886,7 @@
       </c>
       <c r="H108" s="3" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="I108" s="3" t="inlineStr">
@@ -7944,7 +7944,7 @@
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:56</t>
+          <t>2026-02-07 17:32:12</t>
         </is>
       </c>
       <c r="F109" s="3" t="inlineStr">
@@ -8017,7 +8017,7 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:40:59</t>
+          <t>2026-02-07 17:32:15</t>
         </is>
       </c>
       <c r="F110" s="3" t="inlineStr">
@@ -8094,7 +8094,7 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:01</t>
+          <t>2026-02-07 17:32:17</t>
         </is>
       </c>
       <c r="F111" s="3" t="inlineStr">
@@ -8163,7 +8163,7 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:04</t>
+          <t>2026-02-07 17:32:20</t>
         </is>
       </c>
       <c r="F112" s="3" t="inlineStr">
@@ -8189,7 +8189,7 @@
       </c>
       <c r="K112" s="3" t="inlineStr">
         <is>
-          <t>11.6 MJ/m2</t>
+          <t>11.7 MJ/m2</t>
         </is>
       </c>
       <c r="L112" s="3" t="inlineStr">
@@ -8236,7 +8236,7 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:06</t>
+          <t>2026-02-07 17:32:22</t>
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
@@ -8262,7 +8262,7 @@
       <c r="J113" s="3" t="inlineStr"/>
       <c r="K113" s="3" t="inlineStr">
         <is>
-          <t>12.4 MJ/m2</t>
+          <t>12.5 MJ/m2</t>
         </is>
       </c>
       <c r="L113" s="3" t="inlineStr">
@@ -8309,7 +8309,7 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:09</t>
+          <t>2026-02-07 17:32:25</t>
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
@@ -8320,7 +8320,7 @@
       <c r="G114" s="3" t="inlineStr"/>
       <c r="H114" s="3" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I114" s="3" t="inlineStr">
@@ -8343,7 +8343,7 @@
       </c>
       <c r="O114" s="3" t="inlineStr">
         <is>
-          <t>5.9 °C</t>
+          <t>6.0 °C</t>
         </is>
       </c>
     </row>
@@ -8370,7 +8370,7 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:11</t>
+          <t>2026-02-07 17:32:27</t>
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
@@ -8381,7 +8381,7 @@
       <c r="G115" s="3" t="inlineStr"/>
       <c r="H115" s="3" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="I115" s="3" t="inlineStr">
@@ -8391,12 +8391,12 @@
       </c>
       <c r="J115" s="3" t="inlineStr">
         <is>
-          <t>1007.2 hPa</t>
+          <t>1007.3 hPa</t>
         </is>
       </c>
       <c r="K115" s="3" t="inlineStr">
         <is>
-          <t>11.7 MJ/m2</t>
+          <t>11.8 MJ/m2</t>
         </is>
       </c>
       <c r="L115" s="3" t="inlineStr">
@@ -8443,7 +8443,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:14</t>
+          <t>2026-02-07 17:32:30</t>
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
@@ -8464,12 +8464,12 @@
       </c>
       <c r="J116" s="3" t="inlineStr">
         <is>
-          <t>1004.6 hPa</t>
+          <t>1004.7 hPa</t>
         </is>
       </c>
       <c r="K116" s="3" t="inlineStr">
         <is>
-          <t>12.3 MJ/m2</t>
+          <t>12.4 MJ/m2</t>
         </is>
       </c>
       <c r="L116" s="3" t="inlineStr">
@@ -8516,7 +8516,7 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:16</t>
+          <t>2026-02-07 17:32:32</t>
         </is>
       </c>
       <c r="F117" s="3" t="inlineStr">
@@ -8558,7 +8558,7 @@
       </c>
       <c r="O117" s="3" t="inlineStr">
         <is>
-          <t>10.1 °C</t>
+          <t>10.2 °C</t>
         </is>
       </c>
     </row>
@@ -8585,7 +8585,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:18</t>
+          <t>2026-02-07 17:32:34</t>
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
@@ -8626,7 +8626,7 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:21</t>
+          <t>2026-02-07 17:32:37</t>
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
@@ -8687,7 +8687,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:23</t>
+          <t>2026-02-07 17:32:39</t>
         </is>
       </c>
       <c r="F120" s="3" t="inlineStr">
@@ -8698,7 +8698,7 @@
       <c r="G120" s="3" t="inlineStr"/>
       <c r="H120" s="3" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="I120" s="3" t="inlineStr">
@@ -8709,7 +8709,7 @@
       <c r="J120" s="3" t="inlineStr"/>
       <c r="K120" s="3" t="inlineStr">
         <is>
-          <t>11.0 MJ/m2</t>
+          <t>11.1 MJ/m2</t>
         </is>
       </c>
       <c r="L120" s="3" t="inlineStr">
@@ -8756,7 +8756,7 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:25</t>
+          <t>2026-02-07 17:32:41</t>
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
@@ -8767,7 +8767,7 @@
       <c r="G121" s="3" t="inlineStr"/>
       <c r="H121" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I121" s="3" t="inlineStr">
@@ -8798,7 +8798,7 @@
       </c>
       <c r="O121" s="3" t="inlineStr">
         <is>
-          <t>6.7 °C</t>
+          <t>6.8 °C</t>
         </is>
       </c>
     </row>
@@ -8825,7 +8825,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:27</t>
+          <t>2026-02-07 17:32:44</t>
         </is>
       </c>
       <c r="F122" s="3" t="inlineStr">
@@ -8836,7 +8836,7 @@
       <c r="G122" s="3" t="inlineStr"/>
       <c r="H122" s="3" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="I122" s="3" t="inlineStr">
@@ -8871,7 +8871,7 @@
       </c>
       <c r="O122" s="3" t="inlineStr">
         <is>
-          <t>8.6 °C</t>
+          <t>8.7 °C</t>
         </is>
       </c>
     </row>
@@ -8898,7 +8898,7 @@
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:30</t>
+          <t>2026-02-07 17:32:46</t>
         </is>
       </c>
       <c r="F123" s="3" t="inlineStr">
@@ -8909,7 +8909,7 @@
       <c r="G123" s="3" t="inlineStr"/>
       <c r="H123" s="3" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="I123" s="3" t="inlineStr">
@@ -8924,7 +8924,7 @@
       </c>
       <c r="K123" s="3" t="inlineStr">
         <is>
-          <t>7.0 MJ/m2</t>
+          <t>7.1 MJ/m2</t>
         </is>
       </c>
       <c r="L123" s="3" t="inlineStr">
@@ -8944,7 +8944,7 @@
       </c>
       <c r="O123" s="3" t="inlineStr">
         <is>
-          <t>5.2 °C</t>
+          <t>5.4 °C</t>
         </is>
       </c>
     </row>
@@ -8971,7 +8971,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:32</t>
+          <t>2026-02-07 17:32:49</t>
         </is>
       </c>
       <c r="F124" s="3" t="inlineStr">
@@ -8982,7 +8982,7 @@
       <c r="G124" s="3" t="inlineStr"/>
       <c r="H124" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I124" s="3" t="inlineStr">
@@ -9002,7 +9002,7 @@
       </c>
       <c r="L124" s="3" t="inlineStr">
         <is>
-          <t>24.1 km/h - 190º 14:54 TU</t>
+          <t>26.6 km/h - 251º 16:37 TU</t>
         </is>
       </c>
       <c r="M124" s="3" t="inlineStr">
@@ -9017,7 +9017,7 @@
       </c>
       <c r="O124" s="3" t="inlineStr">
         <is>
-          <t>5.9 °C</t>
+          <t>6.0 °C</t>
         </is>
       </c>
     </row>
@@ -9044,7 +9044,7 @@
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:35</t>
+          <t>2026-02-07 17:32:51</t>
         </is>
       </c>
       <c r="F125" s="3" t="inlineStr">
@@ -9055,7 +9055,7 @@
       <c r="G125" s="3" t="inlineStr"/>
       <c r="H125" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I125" s="3" t="inlineStr">
@@ -9066,7 +9066,7 @@
       <c r="J125" s="3" t="inlineStr"/>
       <c r="K125" s="3" t="inlineStr">
         <is>
-          <t>12.8 MJ/m2</t>
+          <t>12.9 MJ/m2</t>
         </is>
       </c>
       <c r="L125" s="3" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:37</t>
+          <t>2026-02-07 17:32:54</t>
         </is>
       </c>
       <c r="F126" s="3" t="inlineStr">
@@ -9155,7 +9155,7 @@
       </c>
       <c r="O126" s="3" t="inlineStr">
         <is>
-          <t>10.5 °C</t>
+          <t>10.6 °C</t>
         </is>
       </c>
     </row>
@@ -9182,7 +9182,7 @@
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:40</t>
+          <t>2026-02-07 17:32:56</t>
         </is>
       </c>
       <c r="F127" s="3" t="inlineStr">
@@ -9203,7 +9203,7 @@
       </c>
       <c r="J127" s="3" t="inlineStr">
         <is>
-          <t>1003.4 hPa</t>
+          <t>1003.5 hPa</t>
         </is>
       </c>
       <c r="K127" s="3" t="inlineStr">
@@ -9255,7 +9255,7 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:42</t>
+          <t>2026-02-07 17:32:58</t>
         </is>
       </c>
       <c r="F128" s="3" t="inlineStr">
@@ -9266,7 +9266,7 @@
       <c r="G128" s="3" t="inlineStr"/>
       <c r="H128" s="3" t="inlineStr">
         <is>
-          <t>61%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="I128" s="3" t="inlineStr">
@@ -9276,12 +9276,12 @@
       </c>
       <c r="J128" s="3" t="inlineStr">
         <is>
-          <t>1005.1 hPa</t>
+          <t>1005.2 hPa</t>
         </is>
       </c>
       <c r="K128" s="3" t="inlineStr">
         <is>
-          <t>12.6 MJ/m2</t>
+          <t>12.7 MJ/m2</t>
         </is>
       </c>
       <c r="L128" s="3" t="inlineStr">
@@ -9301,7 +9301,7 @@
       </c>
       <c r="O128" s="3" t="inlineStr">
         <is>
-          <t>11.4 °C</t>
+          <t>11.5 °C</t>
         </is>
       </c>
     </row>
@@ -9328,7 +9328,7 @@
       </c>
       <c r="E129" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:44</t>
+          <t>2026-02-07 17:33:01</t>
         </is>
       </c>
       <c r="F129" s="3" t="inlineStr">
@@ -9350,7 +9350,7 @@
       <c r="J129" s="3" t="inlineStr"/>
       <c r="K129" s="3" t="inlineStr">
         <is>
-          <t>8.8 MJ/m2</t>
+          <t>8.9 MJ/m2</t>
         </is>
       </c>
       <c r="L129" s="3" t="inlineStr">
@@ -9397,7 +9397,7 @@
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:47</t>
+          <t>2026-02-07 17:33:03</t>
         </is>
       </c>
       <c r="F130" s="3" t="inlineStr">
@@ -9408,7 +9408,7 @@
       <c r="G130" s="3" t="inlineStr"/>
       <c r="H130" s="3" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="I130" s="3" t="inlineStr">
@@ -9466,7 +9466,7 @@
       </c>
       <c r="E131" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:49</t>
+          <t>2026-02-07 17:33:06</t>
         </is>
       </c>
       <c r="F131" s="3" t="inlineStr">
@@ -9487,7 +9487,7 @@
       </c>
       <c r="J131" s="3" t="inlineStr">
         <is>
-          <t>1002.9 hPa</t>
+          <t>1003.0 hPa</t>
         </is>
       </c>
       <c r="K131" s="3" t="inlineStr">
@@ -9539,7 +9539,7 @@
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:51</t>
+          <t>2026-02-07 17:33:08</t>
         </is>
       </c>
       <c r="F132" s="3" t="inlineStr">
@@ -9612,7 +9612,7 @@
       </c>
       <c r="E133" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:54</t>
+          <t>2026-02-07 17:33:11</t>
         </is>
       </c>
       <c r="F133" s="3" t="inlineStr">
@@ -9623,7 +9623,7 @@
       <c r="G133" s="3" t="inlineStr"/>
       <c r="H133" s="3" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I133" s="3" t="inlineStr">
@@ -9638,7 +9638,7 @@
       </c>
       <c r="K133" s="3" t="inlineStr">
         <is>
-          <t>7.2 MJ/m2</t>
+          <t>7.3 MJ/m2</t>
         </is>
       </c>
       <c r="L133" s="3" t="inlineStr">
@@ -9658,7 +9658,7 @@
       </c>
       <c r="O133" s="3" t="inlineStr">
         <is>
-          <t>2.3 °C</t>
+          <t>2.4 °C</t>
         </is>
       </c>
     </row>
@@ -9685,7 +9685,7 @@
       </c>
       <c r="E134" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:56</t>
+          <t>2026-02-07 17:33:13</t>
         </is>
       </c>
       <c r="F134" s="3" t="inlineStr">
@@ -9707,7 +9707,7 @@
       <c r="J134" s="3" t="inlineStr"/>
       <c r="K134" s="3" t="inlineStr">
         <is>
-          <t>12.2 MJ/m2</t>
+          <t>12.3 MJ/m2</t>
         </is>
       </c>
       <c r="L134" s="3" t="inlineStr">
@@ -9754,7 +9754,7 @@
       </c>
       <c r="E135" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:41:59</t>
+          <t>2026-02-07 17:33:15</t>
         </is>
       </c>
       <c r="F135" s="3" t="inlineStr">
@@ -9780,7 +9780,7 @@
       <c r="J135" s="3" t="inlineStr"/>
       <c r="K135" s="3" t="inlineStr">
         <is>
-          <t>10.5 MJ/m2</t>
+          <t>10.6 MJ/m2</t>
         </is>
       </c>
       <c r="L135" s="3" t="inlineStr">
@@ -9800,7 +9800,7 @@
       </c>
       <c r="O135" s="3" t="inlineStr">
         <is>
-          <t>-1.8 °C</t>
+          <t>-1.9 °C</t>
         </is>
       </c>
     </row>
@@ -9827,7 +9827,7 @@
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:01</t>
+          <t>2026-02-07 17:33:18</t>
         </is>
       </c>
       <c r="F136" s="3" t="inlineStr">
@@ -9896,7 +9896,7 @@
       </c>
       <c r="E137" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:04</t>
+          <t>2026-02-07 17:33:20</t>
         </is>
       </c>
       <c r="F137" s="3" t="inlineStr">
@@ -9918,7 +9918,7 @@
       <c r="J137" s="3" t="inlineStr"/>
       <c r="K137" s="3" t="inlineStr">
         <is>
-          <t>11.5 MJ/m2</t>
+          <t>11.6 MJ/m2</t>
         </is>
       </c>
       <c r="L137" s="3" t="inlineStr">
@@ -9938,7 +9938,7 @@
       </c>
       <c r="O137" s="3" t="inlineStr">
         <is>
-          <t>9.8 °C</t>
+          <t>9.9 °C</t>
         </is>
       </c>
     </row>
@@ -9965,7 +9965,7 @@
       </c>
       <c r="E138" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:06</t>
+          <t>2026-02-07 17:33:23</t>
         </is>
       </c>
       <c r="F138" s="3" t="inlineStr">
@@ -9987,7 +9987,7 @@
       <c r="J138" s="3" t="inlineStr"/>
       <c r="K138" s="3" t="inlineStr">
         <is>
-          <t>11.6 MJ/m2</t>
+          <t>11.7 MJ/m2</t>
         </is>
       </c>
       <c r="L138" s="3" t="inlineStr">
@@ -10034,7 +10034,7 @@
       </c>
       <c r="E139" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:09</t>
+          <t>2026-02-07 17:33:25</t>
         </is>
       </c>
       <c r="F139" s="3" t="inlineStr">
@@ -10111,7 +10111,7 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:11</t>
+          <t>2026-02-07 17:33:28</t>
         </is>
       </c>
       <c r="F140" s="3" t="inlineStr">
@@ -10132,12 +10132,12 @@
       </c>
       <c r="J140" s="3" t="inlineStr">
         <is>
-          <t>1003.6 hPa</t>
+          <t>1003.7 hPa</t>
         </is>
       </c>
       <c r="K140" s="3" t="inlineStr">
         <is>
-          <t>11.1 MJ/m2</t>
+          <t>11.2 MJ/m2</t>
         </is>
       </c>
       <c r="L140" s="3" t="inlineStr">
@@ -10184,7 +10184,7 @@
       </c>
       <c r="E141" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:14</t>
+          <t>2026-02-07 17:33:30</t>
         </is>
       </c>
       <c r="F141" s="3" t="inlineStr">
@@ -10205,7 +10205,7 @@
       </c>
       <c r="J141" s="3" t="inlineStr">
         <is>
-          <t>1004.9 hPa</t>
+          <t>1005.0 hPa</t>
         </is>
       </c>
       <c r="K141" s="3" t="inlineStr">
@@ -10257,7 +10257,7 @@
       </c>
       <c r="E142" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:16</t>
+          <t>2026-02-07 17:33:33</t>
         </is>
       </c>
       <c r="F142" s="3" t="inlineStr">
@@ -10279,7 +10279,7 @@
       <c r="J142" s="3" t="inlineStr"/>
       <c r="K142" s="3" t="inlineStr">
         <is>
-          <t>12.3 MJ/m2</t>
+          <t>12.4 MJ/m2</t>
         </is>
       </c>
       <c r="L142" s="3" t="inlineStr">
@@ -10299,7 +10299,7 @@
       </c>
       <c r="O142" s="3" t="inlineStr">
         <is>
-          <t>11.1 °C</t>
+          <t>11.2 °C</t>
         </is>
       </c>
     </row>
@@ -10326,7 +10326,7 @@
       </c>
       <c r="E143" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:19</t>
+          <t>2026-02-07 17:33:35</t>
         </is>
       </c>
       <c r="F143" s="3" t="inlineStr">
@@ -10395,7 +10395,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:21</t>
+          <t>2026-02-07 17:33:38</t>
         </is>
       </c>
       <c r="F144" s="3" t="inlineStr">
@@ -10406,7 +10406,7 @@
       <c r="G144" s="3" t="inlineStr"/>
       <c r="H144" s="3" t="inlineStr">
         <is>
-          <t>58%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="I144" s="3" t="inlineStr">
@@ -10421,7 +10421,7 @@
       </c>
       <c r="K144" s="3" t="inlineStr">
         <is>
-          <t>12.2 MJ/m2</t>
+          <t>12.3 MJ/m2</t>
         </is>
       </c>
       <c r="L144" s="3" t="inlineStr">
@@ -10468,7 +10468,7 @@
       </c>
       <c r="E145" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:24</t>
+          <t>2026-02-07 17:33:40</t>
         </is>
       </c>
       <c r="F145" s="3" t="inlineStr">
@@ -10509,7 +10509,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:26</t>
+          <t>2026-02-07 17:33:42</t>
         </is>
       </c>
       <c r="F146" s="3" t="inlineStr">
@@ -10547,7 +10547,7 @@
       </c>
       <c r="O146" s="3" t="inlineStr">
         <is>
-          <t>7.6 °C</t>
+          <t>7.7 °C</t>
         </is>
       </c>
     </row>
@@ -10574,7 +10574,7 @@
       </c>
       <c r="E147" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:28</t>
+          <t>2026-02-07 17:33:45</t>
         </is>
       </c>
       <c r="F147" s="3" t="inlineStr">
@@ -10585,7 +10585,7 @@
       <c r="G147" s="3" t="inlineStr"/>
       <c r="H147" s="3" t="inlineStr">
         <is>
-          <t>76%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="I147" s="3" t="inlineStr">
@@ -10596,7 +10596,7 @@
       <c r="J147" s="3" t="inlineStr"/>
       <c r="K147" s="3" t="inlineStr">
         <is>
-          <t>11.4 MJ/m2</t>
+          <t>11.5 MJ/m2</t>
         </is>
       </c>
       <c r="L147" s="3" t="inlineStr">
@@ -10616,7 +10616,7 @@
       </c>
       <c r="O147" s="3" t="inlineStr">
         <is>
-          <t>7.5 °C</t>
+          <t>7.6 °C</t>
         </is>
       </c>
     </row>
@@ -10643,7 +10643,7 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:30</t>
+          <t>2026-02-07 17:33:47</t>
         </is>
       </c>
       <c r="F148" s="3" t="inlineStr">
@@ -10665,7 +10665,7 @@
       <c r="J148" s="3" t="inlineStr"/>
       <c r="K148" s="3" t="inlineStr">
         <is>
-          <t>12.7 MJ/m2</t>
+          <t>12.8 MJ/m2</t>
         </is>
       </c>
       <c r="L148" s="3" t="inlineStr">
@@ -10712,7 +10712,7 @@
       </c>
       <c r="E149" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:33</t>
+          <t>2026-02-07 17:33:50</t>
         </is>
       </c>
       <c r="F149" s="3" t="inlineStr">
@@ -10723,7 +10723,7 @@
       <c r="G149" s="3" t="inlineStr"/>
       <c r="H149" s="3" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I149" s="3" t="inlineStr">
@@ -10733,7 +10733,7 @@
       </c>
       <c r="J149" s="3" t="inlineStr">
         <is>
-          <t>1005.4 hPa</t>
+          <t>1005.5 hPa</t>
         </is>
       </c>
       <c r="K149" s="3" t="inlineStr"/>
@@ -10754,7 +10754,7 @@
       </c>
       <c r="O149" s="3" t="inlineStr">
         <is>
-          <t>4.8 °C</t>
+          <t>4.9 °C</t>
         </is>
       </c>
     </row>
@@ -10781,7 +10781,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:35</t>
+          <t>2026-02-07 17:33:52</t>
         </is>
       </c>
       <c r="F150" s="3" t="inlineStr">
@@ -10792,7 +10792,7 @@
       <c r="G150" s="3" t="inlineStr"/>
       <c r="H150" s="3" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="I150" s="3" t="inlineStr">
@@ -10815,7 +10815,7 @@
       </c>
       <c r="O150" s="3" t="inlineStr">
         <is>
-          <t>11.3 °C</t>
+          <t>11.4 °C</t>
         </is>
       </c>
     </row>
@@ -10842,7 +10842,7 @@
       </c>
       <c r="E151" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:38</t>
+          <t>2026-02-07 17:33:55</t>
         </is>
       </c>
       <c r="F151" s="3" t="inlineStr">
@@ -10863,12 +10863,12 @@
       </c>
       <c r="J151" s="3" t="inlineStr">
         <is>
-          <t>1004.0 hPa</t>
+          <t>1004.1 hPa</t>
         </is>
       </c>
       <c r="K151" s="3" t="inlineStr">
         <is>
-          <t>11.4 MJ/m2</t>
+          <t>11.5 MJ/m2</t>
         </is>
       </c>
       <c r="L151" s="3" t="inlineStr">
@@ -10888,7 +10888,7 @@
       </c>
       <c r="O151" s="3" t="inlineStr">
         <is>
-          <t>10.5 °C</t>
+          <t>10.6 °C</t>
         </is>
       </c>
     </row>
@@ -10915,7 +10915,7 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:40</t>
+          <t>2026-02-07 17:33:57</t>
         </is>
       </c>
       <c r="F152" s="3" t="inlineStr">
@@ -10957,7 +10957,7 @@
       </c>
       <c r="O152" s="3" t="inlineStr">
         <is>
-          <t>10.9 °C</t>
+          <t>11.0 °C</t>
         </is>
       </c>
     </row>
@@ -10984,7 +10984,7 @@
       </c>
       <c r="E153" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:43</t>
+          <t>2026-02-07 17:33:59</t>
         </is>
       </c>
       <c r="F153" s="3" t="inlineStr">
@@ -11005,7 +11005,7 @@
       </c>
       <c r="J153" s="3" t="inlineStr">
         <is>
-          <t>1005.9 hPa</t>
+          <t>1006.0 hPa</t>
         </is>
       </c>
       <c r="K153" s="3" t="inlineStr">
@@ -11057,7 +11057,7 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:45</t>
+          <t>2026-02-07 17:34:01</t>
         </is>
       </c>
       <c r="F154" s="3" t="inlineStr">
@@ -11126,7 +11126,7 @@
       </c>
       <c r="E155" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:49</t>
+          <t>2026-02-07 17:34:04</t>
         </is>
       </c>
       <c r="F155" s="3" t="inlineStr">
@@ -11148,7 +11148,7 @@
       <c r="J155" s="3" t="inlineStr"/>
       <c r="K155" s="3" t="inlineStr">
         <is>
-          <t>11.8 MJ/m2</t>
+          <t>11.9 MJ/m2</t>
         </is>
       </c>
       <c r="L155" s="3" t="inlineStr">
@@ -11195,7 +11195,7 @@
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:51</t>
+          <t>2026-02-07 17:34:06</t>
         </is>
       </c>
       <c r="F156" s="3" t="inlineStr">
@@ -11206,7 +11206,7 @@
       <c r="G156" s="3" t="inlineStr"/>
       <c r="H156" s="3" t="inlineStr">
         <is>
-          <t>76%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="I156" s="3" t="inlineStr">
@@ -11237,7 +11237,7 @@
       </c>
       <c r="O156" s="3" t="inlineStr">
         <is>
-          <t>8.4 °C</t>
+          <t>8.6 °C</t>
         </is>
       </c>
     </row>
@@ -11264,7 +11264,7 @@
       </c>
       <c r="E157" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:53</t>
+          <t>2026-02-07 17:34:09</t>
         </is>
       </c>
       <c r="F157" s="3" t="inlineStr">
@@ -11295,7 +11295,7 @@
       </c>
       <c r="L157" s="3" t="inlineStr">
         <is>
-          <t>34.2 km/h - 327º 3:18 TU</t>
+          <t>37.1 km/h - 296º 16:59 TU</t>
         </is>
       </c>
       <c r="M157" s="3" t="inlineStr">
@@ -11337,7 +11337,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:55</t>
+          <t>2026-02-07 17:34:12</t>
         </is>
       </c>
       <c r="F158" s="3" t="inlineStr">
@@ -11383,7 +11383,7 @@
       </c>
       <c r="O158" s="3" t="inlineStr">
         <is>
-          <t>5.9 °C</t>
+          <t>6.0 °C</t>
         </is>
       </c>
     </row>
@@ -11410,7 +11410,7 @@
       </c>
       <c r="E159" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:42:58</t>
+          <t>2026-02-07 17:34:14</t>
         </is>
       </c>
       <c r="F159" s="3" t="inlineStr">
@@ -11425,7 +11425,7 @@
       </c>
       <c r="H159" s="3" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="I159" s="3" t="inlineStr">
@@ -11435,7 +11435,7 @@
       </c>
       <c r="J159" s="3" t="inlineStr">
         <is>
-          <t>1006.6 hPa</t>
+          <t>1006.7 hPa</t>
         </is>
       </c>
       <c r="K159" s="3" t="inlineStr"/>
@@ -11479,7 +11479,7 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:00</t>
+          <t>2026-02-07 17:34:16</t>
         </is>
       </c>
       <c r="F160" s="3" t="inlineStr">
@@ -11540,7 +11540,7 @@
       </c>
       <c r="E161" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:02</t>
+          <t>2026-02-07 17:34:18</t>
         </is>
       </c>
       <c r="F161" s="3" t="inlineStr">
@@ -11613,7 +11613,7 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:05</t>
+          <t>2026-02-07 17:34:21</t>
         </is>
       </c>
       <c r="F162" s="3" t="inlineStr">
@@ -11682,7 +11682,7 @@
       </c>
       <c r="E163" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:07</t>
+          <t>2026-02-07 17:34:23</t>
         </is>
       </c>
       <c r="F163" s="3" t="inlineStr">
@@ -11724,7 +11724,7 @@
       </c>
       <c r="O163" s="3" t="inlineStr">
         <is>
-          <t>9.2 °C</t>
+          <t>9.3 °C</t>
         </is>
       </c>
     </row>
@@ -11751,7 +11751,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:10</t>
+          <t>2026-02-07 17:34:26</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr">
@@ -11762,7 +11762,7 @@
       <c r="G164" s="3" t="inlineStr"/>
       <c r="H164" s="3" t="inlineStr">
         <is>
-          <t>57%</t>
+          <t>58%</t>
         </is>
       </c>
       <c r="I164" s="3" t="inlineStr">
@@ -11824,7 +11824,7 @@
       </c>
       <c r="E165" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:12</t>
+          <t>2026-02-07 17:34:28</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr">
@@ -11835,7 +11835,7 @@
       <c r="G165" s="3" t="inlineStr"/>
       <c r="H165" s="3" t="inlineStr">
         <is>
-          <t>74%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="I165" s="3" t="inlineStr">
@@ -11846,7 +11846,7 @@
       <c r="J165" s="3" t="inlineStr"/>
       <c r="K165" s="3" t="inlineStr">
         <is>
-          <t>10.3 MJ/m2</t>
+          <t>10.4 MJ/m2</t>
         </is>
       </c>
       <c r="L165" s="3" t="inlineStr">
@@ -11893,7 +11893,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:15</t>
+          <t>2026-02-07 17:34:31</t>
         </is>
       </c>
       <c r="F166" s="3" t="inlineStr">
@@ -11954,7 +11954,7 @@
       </c>
       <c r="E167" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:17</t>
+          <t>2026-02-07 17:34:33</t>
         </is>
       </c>
       <c r="F167" s="3" t="inlineStr">
@@ -11965,7 +11965,7 @@
       <c r="G167" s="3" t="inlineStr"/>
       <c r="H167" s="3" t="inlineStr">
         <is>
-          <t>76%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="I167" s="3" t="inlineStr">
@@ -11988,7 +11988,7 @@
       </c>
       <c r="O167" s="3" t="inlineStr">
         <is>
-          <t>10.5 °C</t>
+          <t>10.6 °C</t>
         </is>
       </c>
     </row>
@@ -12015,7 +12015,7 @@
       </c>
       <c r="E168" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:19</t>
+          <t>2026-02-07 17:34:35</t>
         </is>
       </c>
       <c r="F168" s="3" t="inlineStr">
@@ -12026,7 +12026,7 @@
       <c r="G168" s="3" t="inlineStr"/>
       <c r="H168" s="3" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="I168" s="3" t="inlineStr">
@@ -12037,7 +12037,7 @@
       <c r="J168" s="3" t="inlineStr"/>
       <c r="K168" s="3" t="inlineStr">
         <is>
-          <t>11.7 MJ/m2</t>
+          <t>11.8 MJ/m2</t>
         </is>
       </c>
       <c r="L168" s="3" t="inlineStr">
@@ -12084,7 +12084,7 @@
       </c>
       <c r="E169" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:22</t>
+          <t>2026-02-07 17:34:37</t>
         </is>
       </c>
       <c r="F169" s="3" t="inlineStr">
@@ -12095,7 +12095,7 @@
       <c r="G169" s="3" t="inlineStr"/>
       <c r="H169" s="3" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I169" s="3" t="inlineStr">
@@ -12106,7 +12106,7 @@
       <c r="J169" s="3" t="inlineStr"/>
       <c r="K169" s="3" t="inlineStr">
         <is>
-          <t>11.2 MJ/m2</t>
+          <t>11.3 MJ/m2</t>
         </is>
       </c>
       <c r="L169" s="3" t="inlineStr">
@@ -12126,7 +12126,7 @@
       </c>
       <c r="O169" s="3" t="inlineStr">
         <is>
-          <t>5.7 °C</t>
+          <t>5.9 °C</t>
         </is>
       </c>
     </row>
@@ -12153,7 +12153,7 @@
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:24</t>
+          <t>2026-02-07 17:34:40</t>
         </is>
       </c>
       <c r="F170" s="3" t="inlineStr">
@@ -12164,7 +12164,7 @@
       <c r="G170" s="3" t="inlineStr"/>
       <c r="H170" s="3" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I170" s="3" t="inlineStr">
@@ -12179,7 +12179,7 @@
       </c>
       <c r="K170" s="3" t="inlineStr">
         <is>
-          <t>11.7 MJ/m2</t>
+          <t>11.8 MJ/m2</t>
         </is>
       </c>
       <c r="L170" s="3" t="inlineStr">
@@ -12199,7 +12199,7 @@
       </c>
       <c r="O170" s="3" t="inlineStr">
         <is>
-          <t>7.2 °C</t>
+          <t>7.3 °C</t>
         </is>
       </c>
     </row>
@@ -12226,7 +12226,7 @@
       </c>
       <c r="E171" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:26</t>
+          <t>2026-02-07 17:34:42</t>
         </is>
       </c>
       <c r="F171" s="3" t="inlineStr">
@@ -12237,7 +12237,7 @@
       <c r="G171" s="3" t="inlineStr"/>
       <c r="H171" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I171" s="3" t="inlineStr">
@@ -12252,7 +12252,7 @@
       </c>
       <c r="K171" s="3" t="inlineStr">
         <is>
-          <t>10.1 MJ/m2</t>
+          <t>10.2 MJ/m2</t>
         </is>
       </c>
       <c r="L171" s="3" t="inlineStr">
@@ -12272,7 +12272,7 @@
       </c>
       <c r="O171" s="3" t="inlineStr">
         <is>
-          <t>4.3 °C</t>
+          <t>4.4 °C</t>
         </is>
       </c>
     </row>
@@ -12299,7 +12299,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:28</t>
+          <t>2026-02-07 17:34:45</t>
         </is>
       </c>
       <c r="F172" s="3" t="inlineStr">
@@ -12321,7 +12321,7 @@
       <c r="J172" s="3" t="inlineStr"/>
       <c r="K172" s="3" t="inlineStr">
         <is>
-          <t>11.4 MJ/m2</t>
+          <t>11.5 MJ/m2</t>
         </is>
       </c>
       <c r="L172" s="3" t="inlineStr">
@@ -12368,7 +12368,7 @@
       </c>
       <c r="E173" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:31</t>
+          <t>2026-02-07 17:34:47</t>
         </is>
       </c>
       <c r="F173" s="3" t="inlineStr">
@@ -12389,12 +12389,12 @@
       </c>
       <c r="J173" s="3" t="inlineStr">
         <is>
-          <t>1007.5 hPa</t>
+          <t>1007.6 hPa</t>
         </is>
       </c>
       <c r="K173" s="3" t="inlineStr">
         <is>
-          <t>11.3 MJ/m2</t>
+          <t>11.4 MJ/m2</t>
         </is>
       </c>
       <c r="L173" s="3" t="inlineStr">
@@ -12441,7 +12441,7 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:33</t>
+          <t>2026-02-07 17:34:50</t>
         </is>
       </c>
       <c r="F174" s="3" t="inlineStr">
@@ -12452,7 +12452,7 @@
       <c r="G174" s="3" t="inlineStr"/>
       <c r="H174" s="3" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="I174" s="3" t="inlineStr">
@@ -12462,7 +12462,7 @@
       </c>
       <c r="J174" s="3" t="inlineStr">
         <is>
-          <t>1005.3 hPa</t>
+          <t>1005.4 hPa</t>
         </is>
       </c>
       <c r="K174" s="3" t="inlineStr"/>
@@ -12506,7 +12506,7 @@
       </c>
       <c r="E175" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:36</t>
+          <t>2026-02-07 17:34:52</t>
         </is>
       </c>
       <c r="F175" s="3" t="inlineStr">
@@ -12517,7 +12517,7 @@
       <c r="G175" s="3" t="inlineStr"/>
       <c r="H175" s="3" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I175" s="3" t="inlineStr">
@@ -12575,7 +12575,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:38</t>
+          <t>2026-02-07 17:34:55</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
@@ -12648,7 +12648,7 @@
       </c>
       <c r="E177" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:41</t>
+          <t>2026-02-07 17:34:57</t>
         </is>
       </c>
       <c r="F177" s="3" t="inlineStr">
@@ -12717,7 +12717,7 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:43</t>
+          <t>2026-02-07 17:34:59</t>
         </is>
       </c>
       <c r="F178" s="3" t="inlineStr">
@@ -12743,7 +12743,7 @@
       <c r="J178" s="3" t="inlineStr"/>
       <c r="K178" s="3" t="inlineStr">
         <is>
-          <t>5.9 MJ/m2</t>
+          <t>6.0 MJ/m2</t>
         </is>
       </c>
       <c r="L178" s="3" t="inlineStr">
@@ -12763,7 +12763,7 @@
       </c>
       <c r="O178" s="3" t="inlineStr">
         <is>
-          <t>-4.3 °C</t>
+          <t>-4.2 °C</t>
         </is>
       </c>
     </row>
@@ -12790,7 +12790,7 @@
       </c>
       <c r="E179" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:45</t>
+          <t>2026-02-07 17:35:02</t>
         </is>
       </c>
       <c r="F179" s="3" t="inlineStr">
@@ -12867,7 +12867,7 @@
       </c>
       <c r="E180" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:48</t>
+          <t>2026-02-07 17:35:04</t>
         </is>
       </c>
       <c r="F180" s="3" t="inlineStr">
@@ -12940,7 +12940,7 @@
       </c>
       <c r="E181" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:50</t>
+          <t>2026-02-07 17:35:07</t>
         </is>
       </c>
       <c r="F181" s="3" t="inlineStr">
@@ -12951,7 +12951,7 @@
       <c r="G181" s="3" t="inlineStr"/>
       <c r="H181" s="3" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="I181" s="3" t="inlineStr">
@@ -12962,7 +12962,7 @@
       <c r="J181" s="3" t="inlineStr"/>
       <c r="K181" s="3" t="inlineStr">
         <is>
-          <t>10.6 MJ/m2</t>
+          <t>10.7 MJ/m2</t>
         </is>
       </c>
       <c r="L181" s="3" t="inlineStr">
@@ -13009,7 +13009,7 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:53</t>
+          <t>2026-02-07 17:35:09</t>
         </is>
       </c>
       <c r="F182" s="3" t="inlineStr">
@@ -13030,12 +13030,12 @@
       </c>
       <c r="J182" s="3" t="inlineStr">
         <is>
-          <t>1004.3 hPa</t>
+          <t>1004.4 hPa</t>
         </is>
       </c>
       <c r="K182" s="3" t="inlineStr">
         <is>
-          <t>11.0 MJ/m2</t>
+          <t>11.1 MJ/m2</t>
         </is>
       </c>
       <c r="L182" s="3" t="inlineStr">
@@ -13082,7 +13082,7 @@
       </c>
       <c r="E183" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:55</t>
+          <t>2026-02-07 17:35:11</t>
         </is>
       </c>
       <c r="F183" s="3" t="inlineStr">
@@ -13104,7 +13104,7 @@
       <c r="J183" s="3" t="inlineStr"/>
       <c r="K183" s="3" t="inlineStr">
         <is>
-          <t>12.6 MJ/m2</t>
+          <t>12.7 MJ/m2</t>
         </is>
       </c>
       <c r="L183" s="3" t="inlineStr">
@@ -13151,7 +13151,7 @@
       </c>
       <c r="E184" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:43:57</t>
+          <t>2026-02-07 17:35:14</t>
         </is>
       </c>
       <c r="F184" s="3" t="inlineStr">
@@ -13193,7 +13193,7 @@
       </c>
       <c r="O184" s="3" t="inlineStr">
         <is>
-          <t>6.5 °C</t>
+          <t>6.6 °C</t>
         </is>
       </c>
     </row>
@@ -13220,7 +13220,7 @@
       </c>
       <c r="E185" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:44:00</t>
+          <t>2026-02-07 17:35:16</t>
         </is>
       </c>
       <c r="F185" s="3" t="inlineStr">
@@ -13261,7 +13261,7 @@
       </c>
       <c r="E186" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:44:02</t>
+          <t>2026-02-07 17:35:19</t>
         </is>
       </c>
       <c r="F186" s="3" t="inlineStr">
@@ -13303,7 +13303,7 @@
       </c>
       <c r="O186" s="3" t="inlineStr">
         <is>
-          <t>7.6 °C</t>
+          <t>7.7 °C</t>
         </is>
       </c>
     </row>
@@ -13330,7 +13330,7 @@
       </c>
       <c r="E187" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:44:04</t>
+          <t>2026-02-07 17:35:21</t>
         </is>
       </c>
       <c r="F187" s="3" t="inlineStr">
@@ -13341,7 +13341,7 @@
       <c r="G187" s="3" t="inlineStr"/>
       <c r="H187" s="3" t="inlineStr">
         <is>
-          <t>56%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="I187" s="3" t="inlineStr">
@@ -13376,7 +13376,7 @@
       </c>
       <c r="O187" s="3" t="inlineStr">
         <is>
-          <t>11.9 °C</t>
+          <t>12.0 °C</t>
         </is>
       </c>
     </row>
@@ -13403,7 +13403,7 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:44:07</t>
+          <t>2026-02-07 17:35:24</t>
         </is>
       </c>
       <c r="F188" s="3" t="inlineStr">
@@ -13414,7 +13414,7 @@
       <c r="G188" s="3" t="inlineStr"/>
       <c r="H188" s="3" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="I188" s="3" t="inlineStr">
@@ -13429,7 +13429,7 @@
       </c>
       <c r="K188" s="3" t="inlineStr">
         <is>
-          <t>11.5 MJ/m2</t>
+          <t>11.6 MJ/m2</t>
         </is>
       </c>
       <c r="L188" s="3" t="inlineStr">
@@ -13449,7 +13449,7 @@
       </c>
       <c r="O188" s="3" t="inlineStr">
         <is>
-          <t>8.7 °C</t>
+          <t>8.8 °C</t>
         </is>
       </c>
     </row>
@@ -13476,7 +13476,7 @@
       </c>
       <c r="E189" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:44:09</t>
+          <t>2026-02-07 17:35:26</t>
         </is>
       </c>
       <c r="F189" s="3" t="inlineStr">
@@ -13545,7 +13545,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 16:44:12</t>
+          <t>2026-02-07 17:35:29</t>
         </is>
       </c>
       <c r="F190" s="3" t="inlineStr">
@@ -13556,7 +13556,7 @@
       <c r="G190" s="3" t="inlineStr"/>
       <c r="H190" s="3" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="I190" s="3" t="inlineStr">
@@ -13566,12 +13566,12 @@
       </c>
       <c r="J190" s="3" t="inlineStr">
         <is>
-          <t>1006.0 hPa</t>
+          <t>1006.1 hPa</t>
         </is>
       </c>
       <c r="K190" s="3" t="inlineStr">
         <is>
-          <t>11.6 MJ/m2</t>
+          <t>11.7 MJ/m2</t>
         </is>
       </c>
       <c r="L190" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Update automàtic: dades i banners [2026-02-07 18:04]
</commit_message>
<xml_diff>
--- a/config/data/resum_diari_meteocat.xlsx
+++ b/config/data/resum_diari_meteocat.xlsx
@@ -565,7 +565,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:27:53</t>
+          <t>2026-02-07 17:57:17</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
@@ -576,7 +576,7 @@
       <c r="G2" s="3" t="inlineStr"/>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I2" s="3" t="inlineStr">
@@ -607,7 +607,7 @@
       </c>
       <c r="O2" s="3" t="inlineStr">
         <is>
-          <t>7.5 °C</t>
+          <t>7.6 °C</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:27:56</t>
+          <t>2026-02-07 17:57:20</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
@@ -699,7 +699,7 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:27:58</t>
+          <t>2026-02-07 17:57:22</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
@@ -710,7 +710,7 @@
       <c r="G4" s="3" t="inlineStr"/>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>46%</t>
+          <t>47%</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="O4" s="3" t="inlineStr">
         <is>
-          <t>13.7 °C</t>
+          <t>13.6 °C</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:01</t>
+          <t>2026-02-07 17:57:24</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:03</t>
+          <t>2026-02-07 17:57:27</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
@@ -844,7 +844,7 @@
       <c r="G6" s="3" t="inlineStr"/>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I6" s="3" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:05</t>
+          <t>2026-02-07 17:57:29</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
@@ -948,7 +948,7 @@
       </c>
       <c r="O7" s="3" t="inlineStr">
         <is>
-          <t>6.4 °C</t>
+          <t>6.5 °C</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:08</t>
+          <t>2026-02-07 17:57:32</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
@@ -1001,7 +1001,7 @@
       <c r="J8" s="3" t="inlineStr"/>
       <c r="K8" s="3" t="inlineStr">
         <is>
-          <t>3.4 MJ/m2</t>
+          <t>3.5 MJ/m2</t>
         </is>
       </c>
       <c r="L8" s="3" t="inlineStr">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:10</t>
+          <t>2026-02-07 17:57:34</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="O9" s="3" t="inlineStr">
         <is>
-          <t>-0.7 °C</t>
+          <t>-0.6 °C</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:13</t>
+          <t>2026-02-07 17:57:36</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="L10" s="3" t="inlineStr">
         <is>
-          <t>31.7 km/h - 115º 15:49 TU</t>
+          <t>33.5 km/h - 116º 17:27 TU</t>
         </is>
       </c>
       <c r="M10" s="3" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:15</t>
+          <t>2026-02-07 17:57:39</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
@@ -1201,7 +1201,7 @@
       <c r="G11" s="3" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>56%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="I11" s="3" t="inlineStr">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:18</t>
+          <t>2026-02-07 17:57:41</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:20</t>
+          <t>2026-02-07 17:57:44</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
@@ -1339,7 +1339,7 @@
       <c r="G13" s="3" t="inlineStr"/>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="I13" s="3" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:23</t>
+          <t>2026-02-07 17:57:46</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:25</t>
+          <t>2026-02-07 17:57:49</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:28</t>
+          <t>2026-02-07 17:57:51</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
@@ -1554,7 +1554,7 @@
       <c r="G16" s="3" t="inlineStr"/>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:30</t>
+          <t>2026-02-07 17:57:53</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="O17" s="3" t="inlineStr">
         <is>
-          <t>9.4 °C</t>
+          <t>9.5 °C</t>
         </is>
       </c>
     </row>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:32</t>
+          <t>2026-02-07 17:57:56</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
@@ -1684,7 +1684,7 @@
       <c r="G18" s="3" t="inlineStr"/>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t>51%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="I18" s="3" t="inlineStr">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>1005.6 hPa</t>
+          <t>1005.7 hPa</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr">
@@ -1719,7 +1719,7 @@
       </c>
       <c r="O18" s="3" t="inlineStr">
         <is>
-          <t>12.4 °C</t>
+          <t>12.5 °C</t>
         </is>
       </c>
     </row>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:35</t>
+          <t>2026-02-07 17:57:58</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
@@ -1757,7 +1757,7 @@
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="J19" s="3" t="inlineStr">
         <is>
-          <t>1003.5 hPa</t>
+          <t>1003.6 hPa</t>
         </is>
       </c>
       <c r="K19" s="3" t="inlineStr">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:37</t>
+          <t>2026-02-07 17:58:00</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
@@ -1830,7 +1830,7 @@
       <c r="G20" s="3" t="inlineStr"/>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t>47%</t>
+          <t>48%</t>
         </is>
       </c>
       <c r="I20" s="3" t="inlineStr">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:40</t>
+          <t>2026-02-07 17:58:03</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:42</t>
+          <t>2026-02-07 17:58:05</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="J22" s="3" t="inlineStr">
         <is>
-          <t>1005.0 hPa</t>
+          <t>1005.1 hPa</t>
         </is>
       </c>
       <c r="K22" s="3" t="inlineStr">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:45</t>
+          <t>2026-02-07 17:58:08</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="O23" s="3" t="inlineStr">
         <is>
-          <t>8.0 °C</t>
+          <t>8.1 °C</t>
         </is>
       </c>
     </row>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:47</t>
+          <t>2026-02-07 17:58:10</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
@@ -2119,7 +2119,7 @@
       </c>
       <c r="I24" s="3" t="inlineStr">
         <is>
-          <t>0.0 mm</t>
+          <t>0.1 mm</t>
         </is>
       </c>
       <c r="J24" s="3" t="inlineStr"/>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:50</t>
+          <t>2026-02-07 17:58:12</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:52</t>
+          <t>2026-02-07 17:58:15</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
@@ -2268,7 +2268,7 @@
       </c>
       <c r="L26" s="3" t="inlineStr">
         <is>
-          <t>38.2 km/h - 305º 16:24 TU</t>
+          <t>39.6 km/h - 313º 17:07 TU</t>
         </is>
       </c>
       <c r="M26" s="3" t="inlineStr">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:54</t>
+          <t>2026-02-07 17:58:17</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="O27" s="3" t="inlineStr">
         <is>
-          <t>7.9 °C</t>
+          <t>8.0 °C</t>
         </is>
       </c>
     </row>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:56</t>
+          <t>2026-02-07 17:58:20</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="O28" s="3" t="inlineStr">
         <is>
-          <t>11.9 °C</t>
+          <t>11.8 °C</t>
         </is>
       </c>
     </row>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:28:58</t>
+          <t>2026-02-07 17:58:22</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
@@ -2451,7 +2451,7 @@
       <c r="G29" s="3" t="inlineStr"/>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t>53%</t>
+          <t>52%</t>
         </is>
       </c>
       <c r="I29" s="3" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:01</t>
+          <t>2026-02-07 17:58:25</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
@@ -2586,7 +2586,7 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:03</t>
+          <t>2026-02-07 17:58:27</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
@@ -2655,7 +2655,7 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:06</t>
+          <t>2026-02-07 17:58:30</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
@@ -2724,7 +2724,7 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:08</t>
+          <t>2026-02-07 17:58:32</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
@@ -2785,7 +2785,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:11</t>
+          <t>2026-02-07 17:58:34</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
@@ -2854,7 +2854,7 @@
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:13</t>
+          <t>2026-02-07 17:58:37</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
@@ -2875,7 +2875,7 @@
       </c>
       <c r="J35" s="3" t="inlineStr">
         <is>
-          <t>1003.9 hPa</t>
+          <t>1004.0 hPa</t>
         </is>
       </c>
       <c r="K35" s="3" t="inlineStr">
@@ -2927,7 +2927,7 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:16</t>
+          <t>2026-02-07 17:58:39</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
@@ -2938,7 +2938,7 @@
       <c r="G36" s="3" t="inlineStr"/>
       <c r="H36" s="3" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I36" s="3" t="inlineStr">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:18</t>
+          <t>2026-02-07 17:58:42</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:20</t>
+          <t>2026-02-07 17:58:44</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:23</t>
+          <t>2026-02-07 17:58:47</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="J39" s="3" t="inlineStr">
         <is>
-          <t>1007.1 hPa</t>
+          <t>1007.2 hPa</t>
         </is>
       </c>
       <c r="K39" s="3" t="inlineStr">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="O39" s="3" t="inlineStr">
         <is>
-          <t>7.9 °C</t>
+          <t>8.0 °C</t>
         </is>
       </c>
     </row>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:25</t>
+          <t>2026-02-07 17:58:49</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
@@ -3264,7 +3264,7 @@
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:27</t>
+          <t>2026-02-07 17:58:51</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:30</t>
+          <t>2026-02-07 17:58:54</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
@@ -3348,7 +3348,7 @@
       <c r="G42" s="3" t="inlineStr"/>
       <c r="H42" s="3" t="inlineStr">
         <is>
-          <t>53%</t>
+          <t>54%</t>
         </is>
       </c>
       <c r="I42" s="3" t="inlineStr">
@@ -3358,7 +3358,7 @@
       </c>
       <c r="J42" s="3" t="inlineStr">
         <is>
-          <t>1006.2 hPa</t>
+          <t>1006.3 hPa</t>
         </is>
       </c>
       <c r="K42" s="3" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:32</t>
+          <t>2026-02-07 17:58:56</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
@@ -3483,7 +3483,7 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:35</t>
+          <t>2026-02-07 17:58:59</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
@@ -3556,7 +3556,7 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:37</t>
+          <t>2026-02-07 17:59:01</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:40</t>
+          <t>2026-02-07 17:59:03</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
@@ -3702,7 +3702,7 @@
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:42</t>
+          <t>2026-02-07 17:59:06</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
@@ -3740,7 +3740,7 @@
       </c>
       <c r="O47" s="3" t="inlineStr">
         <is>
-          <t>9.5 °C</t>
+          <t>9.6 °C</t>
         </is>
       </c>
     </row>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:44</t>
+          <t>2026-02-07 17:59:08</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:47</t>
+          <t>2026-02-07 17:59:11</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
@@ -3847,7 +3847,7 @@
       <c r="G49" s="3" t="inlineStr"/>
       <c r="H49" s="3" t="inlineStr">
         <is>
-          <t>52%</t>
+          <t>53%</t>
         </is>
       </c>
       <c r="I49" s="3" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:49</t>
+          <t>2026-02-07 17:59:13</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
@@ -3931,7 +3931,7 @@
       <c r="J50" s="3" t="inlineStr"/>
       <c r="K50" s="3" t="inlineStr">
         <is>
-          <t>12.0 MJ/m2</t>
+          <t>12.1 MJ/m2</t>
         </is>
       </c>
       <c r="L50" s="3" t="inlineStr">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="O50" s="3" t="inlineStr">
         <is>
-          <t>7.9 °C</t>
+          <t>8.0 °C</t>
         </is>
       </c>
     </row>
@@ -3978,7 +3978,7 @@
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:52</t>
+          <t>2026-02-07 17:59:15</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
@@ -3989,7 +3989,7 @@
       <c r="G51" s="3" t="inlineStr"/>
       <c r="H51" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I51" s="3" t="inlineStr">
@@ -4024,7 +4024,7 @@
       </c>
       <c r="O51" s="3" t="inlineStr">
         <is>
-          <t>4.3 °C</t>
+          <t>4.4 °C</t>
         </is>
       </c>
     </row>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:54</t>
+          <t>2026-02-07 17:59:18</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
@@ -4062,7 +4062,7 @@
       <c r="G52" s="3" t="inlineStr"/>
       <c r="H52" s="3" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="I52" s="3" t="inlineStr">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:57</t>
+          <t>2026-02-07 17:59:20</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:29:59</t>
+          <t>2026-02-07 17:59:23</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:01</t>
+          <t>2026-02-07 17:59:25</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
@@ -4280,7 +4280,7 @@
       </c>
       <c r="O55" s="3" t="inlineStr">
         <is>
-          <t>12.1 °C</t>
+          <t>12.0 °C</t>
         </is>
       </c>
     </row>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:04</t>
+          <t>2026-02-07 17:59:27</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
@@ -4318,7 +4318,7 @@
       <c r="G56" s="3" t="inlineStr"/>
       <c r="H56" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I56" s="3" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="O56" s="3" t="inlineStr">
         <is>
-          <t>8.0 °C</t>
+          <t>8.1 °C</t>
         </is>
       </c>
     </row>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:06</t>
+          <t>2026-02-07 17:59:30</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
@@ -4393,7 +4393,7 @@
       </c>
       <c r="J57" s="3" t="inlineStr">
         <is>
-          <t>1005.5 hPa</t>
+          <t>1005.6 hPa</t>
         </is>
       </c>
       <c r="K57" s="3" t="inlineStr">
@@ -4445,7 +4445,7 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:09</t>
+          <t>2026-02-07 17:59:32</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="O58" s="3" t="inlineStr">
         <is>
-          <t>6.9 °C</t>
+          <t>7.0 °C</t>
         </is>
       </c>
     </row>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:11</t>
+          <t>2026-02-07 17:59:35</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:13</t>
+          <t>2026-02-07 17:59:37</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
@@ -4590,7 +4590,7 @@
       </c>
       <c r="H60" s="3" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="I60" s="3" t="inlineStr">
@@ -4621,7 +4621,7 @@
       </c>
       <c r="O60" s="3" t="inlineStr">
         <is>
-          <t>-5.7 °C</t>
+          <t>-5.6 °C</t>
         </is>
       </c>
     </row>
@@ -4648,7 +4648,7 @@
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:16</t>
+          <t>2026-02-07 17:59:39</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
@@ -4659,7 +4659,7 @@
       <c r="G61" s="3" t="inlineStr"/>
       <c r="H61" s="3" t="inlineStr">
         <is>
-          <t>72%</t>
+          <t>71%</t>
         </is>
       </c>
       <c r="I61" s="3" t="inlineStr">
@@ -4694,7 +4694,7 @@
       </c>
       <c r="O61" s="3" t="inlineStr">
         <is>
-          <t>8.7 °C</t>
+          <t>8.8 °C</t>
         </is>
       </c>
     </row>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:18</t>
+          <t>2026-02-07 17:59:42</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
@@ -4755,7 +4755,7 @@
       </c>
       <c r="O62" s="3" t="inlineStr">
         <is>
-          <t>10.8 °C</t>
+          <t>10.9 °C</t>
         </is>
       </c>
     </row>
@@ -4782,7 +4782,7 @@
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:21</t>
+          <t>2026-02-07 17:59:44</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
@@ -4823,7 +4823,7 @@
       </c>
       <c r="N63" s="3" t="inlineStr">
         <is>
-          <t>-1.3 °C 3:20 TU</t>
+          <t>-1.6 °C 17:29 TU</t>
         </is>
       </c>
       <c r="O63" s="3" t="inlineStr">
@@ -4855,7 +4855,7 @@
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:23</t>
+          <t>2026-02-07 17:59:46</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
@@ -4876,7 +4876,7 @@
       </c>
       <c r="J64" s="3" t="inlineStr">
         <is>
-          <t>1005.4 hPa</t>
+          <t>1005.5 hPa</t>
         </is>
       </c>
       <c r="K64" s="3" t="inlineStr">
@@ -4896,7 +4896,7 @@
       </c>
       <c r="N64" s="3" t="inlineStr">
         <is>
-          <t>7.7 °C 1:51 TU</t>
+          <t>7.5 °C 17:29 TU</t>
         </is>
       </c>
       <c r="O64" s="3" t="inlineStr">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:26</t>
+          <t>2026-02-07 17:59:49</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
@@ -4989,7 +4989,7 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:28</t>
+          <t>2026-02-07 17:59:51</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
@@ -5050,7 +5050,7 @@
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:30</t>
+          <t>2026-02-07 17:59:53</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
@@ -5072,7 +5072,7 @@
       <c r="J67" s="3" t="inlineStr"/>
       <c r="K67" s="3" t="inlineStr">
         <is>
-          <t>12.1 MJ/m2</t>
+          <t>12.2 MJ/m2</t>
         </is>
       </c>
       <c r="L67" s="3" t="inlineStr">
@@ -5092,7 +5092,7 @@
       </c>
       <c r="O67" s="3" t="inlineStr">
         <is>
-          <t>8.6 °C</t>
+          <t>8.7 °C</t>
         </is>
       </c>
     </row>
@@ -5119,7 +5119,7 @@
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:33</t>
+          <t>2026-02-07 17:59:56</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="O68" s="3" t="inlineStr">
         <is>
-          <t>7.4 °C</t>
+          <t>7.5 °C</t>
         </is>
       </c>
     </row>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:35</t>
+          <t>2026-02-07 17:59:58</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
@@ -5199,7 +5199,7 @@
       <c r="G69" s="3" t="inlineStr"/>
       <c r="H69" s="3" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>69%</t>
         </is>
       </c>
       <c r="I69" s="3" t="inlineStr">
@@ -5209,7 +5209,7 @@
       </c>
       <c r="J69" s="3" t="inlineStr">
         <is>
-          <t>1003.8 hPa</t>
+          <t>1003.9 hPa</t>
         </is>
       </c>
       <c r="K69" s="3" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:37</t>
+          <t>2026-02-07 18:00:01</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:40</t>
+          <t>2026-02-07 18:00:03</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
@@ -5333,7 +5333,7 @@
       <c r="G71" s="3" t="inlineStr"/>
       <c r="H71" s="3" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>74%</t>
         </is>
       </c>
       <c r="I71" s="3" t="inlineStr">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:42</t>
+          <t>2026-02-07 18:00:06</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
@@ -5452,7 +5452,7 @@
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:45</t>
+          <t>2026-02-07 18:00:08</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
@@ -5498,7 +5498,7 @@
       </c>
       <c r="O73" s="3" t="inlineStr">
         <is>
-          <t>4.8 °C</t>
+          <t>4.9 °C</t>
         </is>
       </c>
     </row>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:47</t>
+          <t>2026-02-07 18:00:10</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
@@ -5536,7 +5536,7 @@
       <c r="G74" s="3" t="inlineStr"/>
       <c r="H74" s="3" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I74" s="3" t="inlineStr">
@@ -5586,7 +5586,7 @@
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:49</t>
+          <t>2026-02-07 18:00:13</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
@@ -5607,7 +5607,7 @@
       </c>
       <c r="J75" s="3" t="inlineStr">
         <is>
-          <t>1007.8 hPa</t>
+          <t>1007.7 hPa</t>
         </is>
       </c>
       <c r="K75" s="3" t="inlineStr">
@@ -5632,7 +5632,7 @@
       </c>
       <c r="O75" s="3" t="inlineStr">
         <is>
-          <t>7.6 °C</t>
+          <t>7.7 °C</t>
         </is>
       </c>
     </row>
@@ -5659,7 +5659,7 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:52</t>
+          <t>2026-02-07 18:00:15</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
@@ -5670,7 +5670,7 @@
       <c r="G76" s="3" t="inlineStr"/>
       <c r="H76" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I76" s="3" t="inlineStr">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:54</t>
+          <t>2026-02-07 18:00:17</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
@@ -5743,7 +5743,7 @@
       <c r="G77" s="3" t="inlineStr"/>
       <c r="H77" s="3" t="inlineStr">
         <is>
-          <t>48%</t>
+          <t>49%</t>
         </is>
       </c>
       <c r="I77" s="3" t="inlineStr">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="O77" s="3" t="inlineStr">
         <is>
-          <t>13.4 °C</t>
+          <t>13.3 °C</t>
         </is>
       </c>
     </row>
@@ -5801,7 +5801,7 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:57</t>
+          <t>2026-02-07 18:00:20</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
@@ -5870,7 +5870,7 @@
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:30:59</t>
+          <t>2026-02-07 18:00:22</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
@@ -5896,7 +5896,7 @@
       </c>
       <c r="K79" s="3" t="inlineStr">
         <is>
-          <t>11.8 MJ/m2</t>
+          <t>11.9 MJ/m2</t>
         </is>
       </c>
       <c r="L79" s="3" t="inlineStr">
@@ -5943,7 +5943,7 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:02</t>
+          <t>2026-02-07 18:00:24</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
@@ -6012,7 +6012,7 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:04</t>
+          <t>2026-02-07 18:00:27</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:07</t>
+          <t>2026-02-07 18:00:29</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:09</t>
+          <t>2026-02-07 18:00:31</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
@@ -6187,12 +6187,12 @@
       </c>
       <c r="N83" s="3" t="inlineStr">
         <is>
-          <t>-7.1 °C 7:40 TU</t>
+          <t>-7.6 °C 17:29 TU</t>
         </is>
       </c>
       <c r="O83" s="3" t="inlineStr">
         <is>
-          <t>-5.2 °C</t>
+          <t>-5.3 °C</t>
         </is>
       </c>
     </row>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:11</t>
+          <t>2026-02-07 18:00:33</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
@@ -6288,7 +6288,7 @@
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:14</t>
+          <t>2026-02-07 18:00:36</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:16</t>
+          <t>2026-02-07 18:00:38</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
@@ -6395,7 +6395,7 @@
       </c>
       <c r="O86" s="3" t="inlineStr">
         <is>
-          <t>6.0 °C</t>
+          <t>6.1 °C</t>
         </is>
       </c>
     </row>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:19</t>
+          <t>2026-02-07 18:00:42</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
@@ -6433,7 +6433,7 @@
       <c r="G87" s="3" t="inlineStr"/>
       <c r="H87" s="3" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I87" s="3" t="inlineStr">
@@ -6464,7 +6464,7 @@
       </c>
       <c r="O87" s="3" t="inlineStr">
         <is>
-          <t>4.5 °C</t>
+          <t>4.6 °C</t>
         </is>
       </c>
     </row>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:21</t>
+          <t>2026-02-07 18:00:44</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:23</t>
+          <t>2026-02-07 18:00:46</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:26</t>
+          <t>2026-02-07 18:00:49</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
@@ -6616,7 +6616,7 @@
       <c r="G90" s="3" t="inlineStr"/>
       <c r="H90" s="3" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I90" s="3" t="inlineStr">
@@ -6678,7 +6678,7 @@
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:29</t>
+          <t>2026-02-07 18:00:51</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
@@ -6747,7 +6747,7 @@
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:31</t>
+          <t>2026-02-07 18:00:53</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
@@ -6785,7 +6785,7 @@
       </c>
       <c r="O92" s="3" t="inlineStr">
         <is>
-          <t>-5.9 °C</t>
+          <t>-6.0 °C</t>
         </is>
       </c>
     </row>
@@ -6812,7 +6812,7 @@
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:33</t>
+          <t>2026-02-07 18:00:56</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
@@ -6854,7 +6854,7 @@
       </c>
       <c r="O93" s="3" t="inlineStr">
         <is>
-          <t>9.3 °C</t>
+          <t>9.4 °C</t>
         </is>
       </c>
     </row>
@@ -6881,7 +6881,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:36</t>
+          <t>2026-02-07 18:00:58</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
@@ -6954,7 +6954,7 @@
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:38</t>
+          <t>2026-02-07 18:01:01</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
@@ -7027,7 +7027,7 @@
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:41</t>
+          <t>2026-02-07 18:01:03</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
@@ -7096,7 +7096,7 @@
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:43</t>
+          <t>2026-02-07 18:01:06</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
@@ -7127,7 +7127,7 @@
       </c>
       <c r="L97" s="3" t="inlineStr">
         <is>
-          <t>15.5 km/h - 234º 14:48 TU</t>
+          <t>22.3 km/h - 244º 17:08 TU</t>
         </is>
       </c>
       <c r="M97" s="3" t="inlineStr">
@@ -7169,7 +7169,7 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:45</t>
+          <t>2026-02-07 18:01:08</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
@@ -7211,7 +7211,7 @@
       </c>
       <c r="O98" s="3" t="inlineStr">
         <is>
-          <t>5.2 °C</t>
+          <t>5.3 °C</t>
         </is>
       </c>
     </row>
@@ -7238,7 +7238,7 @@
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:48</t>
+          <t>2026-02-07 18:01:11</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
@@ -7249,7 +7249,7 @@
       <c r="G99" s="3" t="inlineStr"/>
       <c r="H99" s="3" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>74%</t>
         </is>
       </c>
       <c r="I99" s="3" t="inlineStr">
@@ -7280,7 +7280,7 @@
       </c>
       <c r="O99" s="3" t="inlineStr">
         <is>
-          <t>8.4 °C</t>
+          <t>8.5 °C</t>
         </is>
       </c>
     </row>
@@ -7307,7 +7307,7 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:50</t>
+          <t>2026-02-07 18:01:13</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
@@ -7318,7 +7318,7 @@
       <c r="G100" s="3" t="inlineStr"/>
       <c r="H100" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I100" s="3" t="inlineStr">
@@ -7380,7 +7380,7 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:53</t>
+          <t>2026-02-07 18:01:16</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
@@ -7391,7 +7391,7 @@
       <c r="G101" s="3" t="inlineStr"/>
       <c r="H101" s="3" t="inlineStr">
         <is>
-          <t>76%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="I101" s="3" t="inlineStr">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="O101" s="3" t="inlineStr">
         <is>
-          <t>7.1 °C</t>
+          <t>7.2 °C</t>
         </is>
       </c>
     </row>
@@ -7449,7 +7449,7 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:55</t>
+          <t>2026-02-07 18:01:18</t>
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="J102" s="3" t="inlineStr">
         <is>
-          <t>1004.0 hPa</t>
+          <t>1004.1 hPa</t>
         </is>
       </c>
       <c r="K102" s="3" t="inlineStr">
@@ -7522,7 +7522,7 @@
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:31:58</t>
+          <t>2026-02-07 18:01:20</t>
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
@@ -7568,7 +7568,7 @@
       </c>
       <c r="O103" s="3" t="inlineStr">
         <is>
-          <t>7.0 °C</t>
+          <t>7.1 °C</t>
         </is>
       </c>
     </row>
@@ -7595,7 +7595,7 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:00</t>
+          <t>2026-02-07 18:01:22</t>
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
@@ -7668,7 +7668,7 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:03</t>
+          <t>2026-02-07 18:01:25</t>
         </is>
       </c>
       <c r="F105" s="3" t="inlineStr">
@@ -7679,7 +7679,7 @@
       <c r="G105" s="3" t="inlineStr"/>
       <c r="H105" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I105" s="3" t="inlineStr">
@@ -7737,7 +7737,7 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:05</t>
+          <t>2026-02-07 18:01:27</t>
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
@@ -7802,7 +7802,7 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:08</t>
+          <t>2026-02-07 18:01:30</t>
         </is>
       </c>
       <c r="F107" s="3" t="inlineStr">
@@ -7824,7 +7824,7 @@
       <c r="J107" s="3" t="inlineStr"/>
       <c r="K107" s="3" t="inlineStr">
         <is>
-          <t>12.3 MJ/m2</t>
+          <t>12.4 MJ/m2</t>
         </is>
       </c>
       <c r="L107" s="3" t="inlineStr">
@@ -7871,7 +7871,7 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:10</t>
+          <t>2026-02-07 18:01:32</t>
         </is>
       </c>
       <c r="F108" s="3" t="inlineStr">
@@ -7944,7 +7944,7 @@
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:12</t>
+          <t>2026-02-07 18:01:35</t>
         </is>
       </c>
       <c r="F109" s="3" t="inlineStr">
@@ -7970,7 +7970,7 @@
       </c>
       <c r="K109" s="3" t="inlineStr">
         <is>
-          <t>11.9 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L109" s="3" t="inlineStr">
@@ -7990,7 +7990,7 @@
       </c>
       <c r="O109" s="3" t="inlineStr">
         <is>
-          <t>8.4 °C</t>
+          <t>8.5 °C</t>
         </is>
       </c>
     </row>
@@ -8017,7 +8017,7 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:15</t>
+          <t>2026-02-07 18:01:37</t>
         </is>
       </c>
       <c r="F110" s="3" t="inlineStr">
@@ -8032,7 +8032,7 @@
       </c>
       <c r="H110" s="3" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>71%</t>
         </is>
       </c>
       <c r="I110" s="3" t="inlineStr">
@@ -8042,7 +8042,7 @@
       </c>
       <c r="J110" s="3" t="inlineStr">
         <is>
-          <t>1003.6 hPa</t>
+          <t>1003.7 hPa</t>
         </is>
       </c>
       <c r="K110" s="3" t="inlineStr">
@@ -8094,7 +8094,7 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:17</t>
+          <t>2026-02-07 18:01:40</t>
         </is>
       </c>
       <c r="F111" s="3" t="inlineStr">
@@ -8163,7 +8163,7 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:20</t>
+          <t>2026-02-07 18:01:42</t>
         </is>
       </c>
       <c r="F112" s="3" t="inlineStr">
@@ -8174,7 +8174,7 @@
       <c r="G112" s="3" t="inlineStr"/>
       <c r="H112" s="3" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="I112" s="3" t="inlineStr">
@@ -8184,7 +8184,7 @@
       </c>
       <c r="J112" s="3" t="inlineStr">
         <is>
-          <t>1006.5 hPa</t>
+          <t>1006.6 hPa</t>
         </is>
       </c>
       <c r="K112" s="3" t="inlineStr">
@@ -8236,7 +8236,7 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:22</t>
+          <t>2026-02-07 18:01:45</t>
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
@@ -8277,12 +8277,12 @@
       </c>
       <c r="N113" s="3" t="inlineStr">
         <is>
-          <t>-6.1 °C 6:54 TU</t>
+          <t>-6.2 °C 17:07 TU</t>
         </is>
       </c>
       <c r="O113" s="3" t="inlineStr">
         <is>
-          <t>-3.7 °C</t>
+          <t>-3.8 °C</t>
         </is>
       </c>
     </row>
@@ -8309,7 +8309,7 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:25</t>
+          <t>2026-02-07 18:01:47</t>
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
@@ -8320,7 +8320,7 @@
       <c r="G114" s="3" t="inlineStr"/>
       <c r="H114" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I114" s="3" t="inlineStr">
@@ -8370,7 +8370,7 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:27</t>
+          <t>2026-02-07 18:01:49</t>
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
@@ -8443,7 +8443,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:30</t>
+          <t>2026-02-07 18:01:52</t>
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
@@ -8464,7 +8464,7 @@
       </c>
       <c r="J116" s="3" t="inlineStr">
         <is>
-          <t>1004.7 hPa</t>
+          <t>1004.8 hPa</t>
         </is>
       </c>
       <c r="K116" s="3" t="inlineStr">
@@ -8516,7 +8516,7 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:32</t>
+          <t>2026-02-07 18:01:54</t>
         </is>
       </c>
       <c r="F117" s="3" t="inlineStr">
@@ -8585,7 +8585,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:34</t>
+          <t>2026-02-07 18:01:56</t>
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
@@ -8626,7 +8626,7 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:37</t>
+          <t>2026-02-07 18:01:59</t>
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
@@ -8687,7 +8687,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:39</t>
+          <t>2026-02-07 18:02:01</t>
         </is>
       </c>
       <c r="F120" s="3" t="inlineStr">
@@ -8729,7 +8729,7 @@
       </c>
       <c r="O120" s="3" t="inlineStr">
         <is>
-          <t>6.1 °C</t>
+          <t>6.2 °C</t>
         </is>
       </c>
     </row>
@@ -8756,7 +8756,7 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:41</t>
+          <t>2026-02-07 18:02:03</t>
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
@@ -8825,7 +8825,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:44</t>
+          <t>2026-02-07 18:02:06</t>
         </is>
       </c>
       <c r="F122" s="3" t="inlineStr">
@@ -8846,7 +8846,7 @@
       </c>
       <c r="J122" s="3" t="inlineStr">
         <is>
-          <t>1003.7 hPa</t>
+          <t>1003.8 hPa</t>
         </is>
       </c>
       <c r="K122" s="3" t="inlineStr">
@@ -8898,7 +8898,7 @@
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:46</t>
+          <t>2026-02-07 18:02:08</t>
         </is>
       </c>
       <c r="F123" s="3" t="inlineStr">
@@ -8909,7 +8909,7 @@
       <c r="G123" s="3" t="inlineStr"/>
       <c r="H123" s="3" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="I123" s="3" t="inlineStr">
@@ -8971,7 +8971,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:49</t>
+          <t>2026-02-07 18:02:11</t>
         </is>
       </c>
       <c r="F124" s="3" t="inlineStr">
@@ -8992,7 +8992,7 @@
       </c>
       <c r="J124" s="3" t="inlineStr">
         <is>
-          <t>1005.0 hPa</t>
+          <t>1005.1 hPa</t>
         </is>
       </c>
       <c r="K124" s="3" t="inlineStr">
@@ -9002,7 +9002,7 @@
       </c>
       <c r="L124" s="3" t="inlineStr">
         <is>
-          <t>26.6 km/h - 251º 16:37 TU</t>
+          <t>31.0 km/h - 175º 17:25 TU</t>
         </is>
       </c>
       <c r="M124" s="3" t="inlineStr">
@@ -9044,7 +9044,7 @@
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:51</t>
+          <t>2026-02-07 18:02:13</t>
         </is>
       </c>
       <c r="F125" s="3" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:54</t>
+          <t>2026-02-07 18:02:15</t>
         </is>
       </c>
       <c r="F126" s="3" t="inlineStr">
@@ -9182,7 +9182,7 @@
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:56</t>
+          <t>2026-02-07 18:02:18</t>
         </is>
       </c>
       <c r="F127" s="3" t="inlineStr">
@@ -9203,7 +9203,7 @@
       </c>
       <c r="J127" s="3" t="inlineStr">
         <is>
-          <t>1003.5 hPa</t>
+          <t>1003.6 hPa</t>
         </is>
       </c>
       <c r="K127" s="3" t="inlineStr">
@@ -9255,7 +9255,7 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:32:58</t>
+          <t>2026-02-07 18:02:20</t>
         </is>
       </c>
       <c r="F128" s="3" t="inlineStr">
@@ -9266,7 +9266,7 @@
       <c r="G128" s="3" t="inlineStr"/>
       <c r="H128" s="3" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="I128" s="3" t="inlineStr">
@@ -9276,7 +9276,7 @@
       </c>
       <c r="J128" s="3" t="inlineStr">
         <is>
-          <t>1005.2 hPa</t>
+          <t>1005.3 hPa</t>
         </is>
       </c>
       <c r="K128" s="3" t="inlineStr">
@@ -9301,7 +9301,7 @@
       </c>
       <c r="O128" s="3" t="inlineStr">
         <is>
-          <t>11.5 °C</t>
+          <t>11.6 °C</t>
         </is>
       </c>
     </row>
@@ -9328,7 +9328,7 @@
       </c>
       <c r="E129" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:01</t>
+          <t>2026-02-07 18:02:23</t>
         </is>
       </c>
       <c r="F129" s="3" t="inlineStr">
@@ -9339,7 +9339,7 @@
       <c r="G129" s="3" t="inlineStr"/>
       <c r="H129" s="3" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I129" s="3" t="inlineStr">
@@ -9370,7 +9370,7 @@
       </c>
       <c r="O129" s="3" t="inlineStr">
         <is>
-          <t>5.1 °C</t>
+          <t>5.2 °C</t>
         </is>
       </c>
     </row>
@@ -9397,7 +9397,7 @@
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:03</t>
+          <t>2026-02-07 18:02:25</t>
         </is>
       </c>
       <c r="F130" s="3" t="inlineStr">
@@ -9439,7 +9439,7 @@
       </c>
       <c r="O130" s="3" t="inlineStr">
         <is>
-          <t>5.4 °C</t>
+          <t>5.5 °C</t>
         </is>
       </c>
     </row>
@@ -9466,7 +9466,7 @@
       </c>
       <c r="E131" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:06</t>
+          <t>2026-02-07 18:02:27</t>
         </is>
       </c>
       <c r="F131" s="3" t="inlineStr">
@@ -9477,7 +9477,7 @@
       <c r="G131" s="3" t="inlineStr"/>
       <c r="H131" s="3" t="inlineStr">
         <is>
-          <t>72%</t>
+          <t>71%</t>
         </is>
       </c>
       <c r="I131" s="3" t="inlineStr">
@@ -9512,7 +9512,7 @@
       </c>
       <c r="O131" s="3" t="inlineStr">
         <is>
-          <t>11.2 °C</t>
+          <t>11.3 °C</t>
         </is>
       </c>
     </row>
@@ -9539,7 +9539,7 @@
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:08</t>
+          <t>2026-02-07 18:02:30</t>
         </is>
       </c>
       <c r="F132" s="3" t="inlineStr">
@@ -9612,7 +9612,7 @@
       </c>
       <c r="E133" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:11</t>
+          <t>2026-02-07 18:02:32</t>
         </is>
       </c>
       <c r="F133" s="3" t="inlineStr">
@@ -9685,7 +9685,7 @@
       </c>
       <c r="E134" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:13</t>
+          <t>2026-02-07 18:02:35</t>
         </is>
       </c>
       <c r="F134" s="3" t="inlineStr">
@@ -9696,7 +9696,7 @@
       <c r="G134" s="3" t="inlineStr"/>
       <c r="H134" s="3" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="I134" s="3" t="inlineStr">
@@ -9727,7 +9727,7 @@
       </c>
       <c r="O134" s="3" t="inlineStr">
         <is>
-          <t>4.7 °C</t>
+          <t>4.8 °C</t>
         </is>
       </c>
     </row>
@@ -9754,7 +9754,7 @@
       </c>
       <c r="E135" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:15</t>
+          <t>2026-02-07 18:02:37</t>
         </is>
       </c>
       <c r="F135" s="3" t="inlineStr">
@@ -9827,7 +9827,7 @@
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:18</t>
+          <t>2026-02-07 18:02:40</t>
         </is>
       </c>
       <c r="F136" s="3" t="inlineStr">
@@ -9838,7 +9838,7 @@
       <c r="G136" s="3" t="inlineStr"/>
       <c r="H136" s="3" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="I136" s="3" t="inlineStr">
@@ -9896,7 +9896,7 @@
       </c>
       <c r="E137" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:20</t>
+          <t>2026-02-07 18:02:42</t>
         </is>
       </c>
       <c r="F137" s="3" t="inlineStr">
@@ -9965,7 +9965,7 @@
       </c>
       <c r="E138" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:23</t>
+          <t>2026-02-07 18:02:45</t>
         </is>
       </c>
       <c r="F138" s="3" t="inlineStr">
@@ -10034,7 +10034,7 @@
       </c>
       <c r="E139" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:25</t>
+          <t>2026-02-07 18:02:47</t>
         </is>
       </c>
       <c r="F139" s="3" t="inlineStr">
@@ -10111,7 +10111,7 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:28</t>
+          <t>2026-02-07 18:02:50</t>
         </is>
       </c>
       <c r="F140" s="3" t="inlineStr">
@@ -10184,7 +10184,7 @@
       </c>
       <c r="E141" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:30</t>
+          <t>2026-02-07 18:02:52</t>
         </is>
       </c>
       <c r="F141" s="3" t="inlineStr">
@@ -10195,7 +10195,7 @@
       <c r="G141" s="3" t="inlineStr"/>
       <c r="H141" s="3" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>68%</t>
         </is>
       </c>
       <c r="I141" s="3" t="inlineStr">
@@ -10230,7 +10230,7 @@
       </c>
       <c r="O141" s="3" t="inlineStr">
         <is>
-          <t>10.3 °C</t>
+          <t>10.4 °C</t>
         </is>
       </c>
     </row>
@@ -10257,7 +10257,7 @@
       </c>
       <c r="E142" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:33</t>
+          <t>2026-02-07 18:02:55</t>
         </is>
       </c>
       <c r="F142" s="3" t="inlineStr">
@@ -10326,7 +10326,7 @@
       </c>
       <c r="E143" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:35</t>
+          <t>2026-02-07 18:02:57</t>
         </is>
       </c>
       <c r="F143" s="3" t="inlineStr">
@@ -10395,7 +10395,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:38</t>
+          <t>2026-02-07 18:03:00</t>
         </is>
       </c>
       <c r="F144" s="3" t="inlineStr">
@@ -10468,7 +10468,7 @@
       </c>
       <c r="E145" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:40</t>
+          <t>2026-02-07 18:03:02</t>
         </is>
       </c>
       <c r="F145" s="3" t="inlineStr">
@@ -10509,7 +10509,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:42</t>
+          <t>2026-02-07 18:03:04</t>
         </is>
       </c>
       <c r="F146" s="3" t="inlineStr">
@@ -10520,7 +10520,7 @@
       <c r="G146" s="3" t="inlineStr"/>
       <c r="H146" s="3" t="inlineStr">
         <is>
-          <t>72%</t>
+          <t>71%</t>
         </is>
       </c>
       <c r="I146" s="3" t="inlineStr">
@@ -10574,7 +10574,7 @@
       </c>
       <c r="E147" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:45</t>
+          <t>2026-02-07 18:03:06</t>
         </is>
       </c>
       <c r="F147" s="3" t="inlineStr">
@@ -10643,7 +10643,7 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:47</t>
+          <t>2026-02-07 18:03:09</t>
         </is>
       </c>
       <c r="F148" s="3" t="inlineStr">
@@ -10654,7 +10654,7 @@
       <c r="G148" s="3" t="inlineStr"/>
       <c r="H148" s="3" t="inlineStr">
         <is>
-          <t>56%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="I148" s="3" t="inlineStr">
@@ -10712,7 +10712,7 @@
       </c>
       <c r="E149" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:50</t>
+          <t>2026-02-07 18:03:11</t>
         </is>
       </c>
       <c r="F149" s="3" t="inlineStr">
@@ -10781,7 +10781,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:52</t>
+          <t>2026-02-07 18:03:14</t>
         </is>
       </c>
       <c r="F150" s="3" t="inlineStr">
@@ -10842,7 +10842,7 @@
       </c>
       <c r="E151" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:55</t>
+          <t>2026-02-07 18:03:16</t>
         </is>
       </c>
       <c r="F151" s="3" t="inlineStr">
@@ -10853,7 +10853,7 @@
       <c r="G151" s="3" t="inlineStr"/>
       <c r="H151" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I151" s="3" t="inlineStr">
@@ -10915,7 +10915,7 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:57</t>
+          <t>2026-02-07 18:03:19</t>
         </is>
       </c>
       <c r="F152" s="3" t="inlineStr">
@@ -10984,7 +10984,7 @@
       </c>
       <c r="E153" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:33:59</t>
+          <t>2026-02-07 18:03:21</t>
         </is>
       </c>
       <c r="F153" s="3" t="inlineStr">
@@ -11057,7 +11057,7 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:01</t>
+          <t>2026-02-07 18:03:24</t>
         </is>
       </c>
       <c r="F154" s="3" t="inlineStr">
@@ -11126,7 +11126,7 @@
       </c>
       <c r="E155" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:04</t>
+          <t>2026-02-07 18:03:26</t>
         </is>
       </c>
       <c r="F155" s="3" t="inlineStr">
@@ -11195,7 +11195,7 @@
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:06</t>
+          <t>2026-02-07 18:03:28</t>
         </is>
       </c>
       <c r="F156" s="3" t="inlineStr">
@@ -11264,7 +11264,7 @@
       </c>
       <c r="E157" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:09</t>
+          <t>2026-02-07 18:03:31</t>
         </is>
       </c>
       <c r="F157" s="3" t="inlineStr">
@@ -11279,7 +11279,7 @@
       </c>
       <c r="H157" s="3" t="inlineStr">
         <is>
-          <t>74%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="I157" s="3" t="inlineStr">
@@ -11295,12 +11295,12 @@
       </c>
       <c r="L157" s="3" t="inlineStr">
         <is>
-          <t>37.1 km/h - 296º 16:59 TU</t>
+          <t>43.2 km/h - 302º 17:23 TU</t>
         </is>
       </c>
       <c r="M157" s="3" t="inlineStr">
         <is>
-          <t>-2.3 °C 12:53 TU</t>
+          <t>-1.5 °C 17:29 TU</t>
         </is>
       </c>
       <c r="N157" s="3" t="inlineStr">
@@ -11337,7 +11337,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:12</t>
+          <t>2026-02-07 18:03:33</t>
         </is>
       </c>
       <c r="F158" s="3" t="inlineStr">
@@ -11358,7 +11358,7 @@
       </c>
       <c r="J158" s="3" t="inlineStr">
         <is>
-          <t>1005.5 hPa</t>
+          <t>1005.6 hPa</t>
         </is>
       </c>
       <c r="K158" s="3" t="inlineStr">
@@ -11410,7 +11410,7 @@
       </c>
       <c r="E159" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:14</t>
+          <t>2026-02-07 18:03:36</t>
         </is>
       </c>
       <c r="F159" s="3" t="inlineStr">
@@ -11479,7 +11479,7 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:16</t>
+          <t>2026-02-07 18:03:38</t>
         </is>
       </c>
       <c r="F160" s="3" t="inlineStr">
@@ -11490,7 +11490,7 @@
       <c r="G160" s="3" t="inlineStr"/>
       <c r="H160" s="3" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="I160" s="3" t="inlineStr">
@@ -11540,7 +11540,7 @@
       </c>
       <c r="E161" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:18</t>
+          <t>2026-02-07 18:03:41</t>
         </is>
       </c>
       <c r="F161" s="3" t="inlineStr">
@@ -11551,7 +11551,7 @@
       <c r="G161" s="3" t="inlineStr"/>
       <c r="H161" s="3" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>51%</t>
         </is>
       </c>
       <c r="I161" s="3" t="inlineStr">
@@ -11613,7 +11613,7 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:21</t>
+          <t>2026-02-07 18:03:43</t>
         </is>
       </c>
       <c r="F162" s="3" t="inlineStr">
@@ -11624,7 +11624,7 @@
       <c r="G162" s="3" t="inlineStr"/>
       <c r="H162" s="3" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="I162" s="3" t="inlineStr">
@@ -11682,7 +11682,7 @@
       </c>
       <c r="E163" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:23</t>
+          <t>2026-02-07 18:03:45</t>
         </is>
       </c>
       <c r="F163" s="3" t="inlineStr">
@@ -11751,7 +11751,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:26</t>
+          <t>2026-02-07 18:03:48</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr">
@@ -11797,7 +11797,7 @@
       </c>
       <c r="O164" s="3" t="inlineStr">
         <is>
-          <t>12.1 °C</t>
+          <t>12.2 °C</t>
         </is>
       </c>
     </row>
@@ -11824,7 +11824,7 @@
       </c>
       <c r="E165" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:28</t>
+          <t>2026-02-07 18:03:50</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr">
@@ -11866,7 +11866,7 @@
       </c>
       <c r="O165" s="3" t="inlineStr">
         <is>
-          <t>8.8 °C</t>
+          <t>8.9 °C</t>
         </is>
       </c>
     </row>
@@ -11893,7 +11893,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:31</t>
+          <t>2026-02-07 18:03:53</t>
         </is>
       </c>
       <c r="F166" s="3" t="inlineStr">
@@ -11904,7 +11904,7 @@
       <c r="G166" s="3" t="inlineStr"/>
       <c r="H166" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I166" s="3" t="inlineStr">
@@ -11927,7 +11927,7 @@
       </c>
       <c r="O166" s="3" t="inlineStr">
         <is>
-          <t>10.0 °C</t>
+          <t>10.1 °C</t>
         </is>
       </c>
     </row>
@@ -11954,7 +11954,7 @@
       </c>
       <c r="E167" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:33</t>
+          <t>2026-02-07 18:03:55</t>
         </is>
       </c>
       <c r="F167" s="3" t="inlineStr">
@@ -12015,7 +12015,7 @@
       </c>
       <c r="E168" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:35</t>
+          <t>2026-02-07 18:03:57</t>
         </is>
       </c>
       <c r="F168" s="3" t="inlineStr">
@@ -12084,7 +12084,7 @@
       </c>
       <c r="E169" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:37</t>
+          <t>2026-02-07 18:04:00</t>
         </is>
       </c>
       <c r="F169" s="3" t="inlineStr">
@@ -12095,7 +12095,7 @@
       <c r="G169" s="3" t="inlineStr"/>
       <c r="H169" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="I169" s="3" t="inlineStr">
@@ -12153,7 +12153,7 @@
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:40</t>
+          <t>2026-02-07 18:04:02</t>
         </is>
       </c>
       <c r="F170" s="3" t="inlineStr">
@@ -12226,7 +12226,7 @@
       </c>
       <c r="E171" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:42</t>
+          <t>2026-02-07 18:04:05</t>
         </is>
       </c>
       <c r="F171" s="3" t="inlineStr">
@@ -12237,7 +12237,7 @@
       <c r="G171" s="3" t="inlineStr"/>
       <c r="H171" s="3" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="I171" s="3" t="inlineStr">
@@ -12299,7 +12299,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:45</t>
+          <t>2026-02-07 18:04:07</t>
         </is>
       </c>
       <c r="F172" s="3" t="inlineStr">
@@ -12310,7 +12310,7 @@
       <c r="G172" s="3" t="inlineStr"/>
       <c r="H172" s="3" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>51%</t>
         </is>
       </c>
       <c r="I172" s="3" t="inlineStr">
@@ -12368,7 +12368,7 @@
       </c>
       <c r="E173" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:47</t>
+          <t>2026-02-07 18:04:09</t>
         </is>
       </c>
       <c r="F173" s="3" t="inlineStr">
@@ -12441,7 +12441,7 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:50</t>
+          <t>2026-02-07 18:04:12</t>
         </is>
       </c>
       <c r="F174" s="3" t="inlineStr">
@@ -12462,7 +12462,7 @@
       </c>
       <c r="J174" s="3" t="inlineStr">
         <is>
-          <t>1005.4 hPa</t>
+          <t>1005.5 hPa</t>
         </is>
       </c>
       <c r="K174" s="3" t="inlineStr"/>
@@ -12506,7 +12506,7 @@
       </c>
       <c r="E175" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:52</t>
+          <t>2026-02-07 18:04:14</t>
         </is>
       </c>
       <c r="F175" s="3" t="inlineStr">
@@ -12548,7 +12548,7 @@
       </c>
       <c r="O175" s="3" t="inlineStr">
         <is>
-          <t>8.0 °C</t>
+          <t>8.1 °C</t>
         </is>
       </c>
     </row>
@@ -12575,7 +12575,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:55</t>
+          <t>2026-02-07 18:04:17</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
@@ -12586,7 +12586,7 @@
       <c r="G176" s="3" t="inlineStr"/>
       <c r="H176" s="3" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="I176" s="3" t="inlineStr">
@@ -12596,7 +12596,7 @@
       </c>
       <c r="J176" s="3" t="inlineStr">
         <is>
-          <t>1004.8 hPa</t>
+          <t>1004.9 hPa</t>
         </is>
       </c>
       <c r="K176" s="3" t="inlineStr">
@@ -12648,7 +12648,7 @@
       </c>
       <c r="E177" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:57</t>
+          <t>2026-02-07 18:04:19</t>
         </is>
       </c>
       <c r="F177" s="3" t="inlineStr">
@@ -12659,7 +12659,7 @@
       <c r="G177" s="3" t="inlineStr"/>
       <c r="H177" s="3" t="inlineStr">
         <is>
-          <t>71%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="I177" s="3" t="inlineStr">
@@ -12690,7 +12690,7 @@
       </c>
       <c r="O177" s="3" t="inlineStr">
         <is>
-          <t>7.8 °C</t>
+          <t>7.9 °C</t>
         </is>
       </c>
     </row>
@@ -12717,7 +12717,7 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:34:59</t>
+          <t>2026-02-07 18:04:21</t>
         </is>
       </c>
       <c r="F178" s="3" t="inlineStr">
@@ -12790,7 +12790,7 @@
       </c>
       <c r="E179" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:02</t>
+          <t>2026-02-07 18:04:24</t>
         </is>
       </c>
       <c r="F179" s="3" t="inlineStr">
@@ -12805,7 +12805,7 @@
       </c>
       <c r="H179" s="3" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="I179" s="3" t="inlineStr">
@@ -12815,7 +12815,7 @@
       </c>
       <c r="J179" s="3" t="inlineStr">
         <is>
-          <t>1005.0 hPa</t>
+          <t>1004.9 hPa</t>
         </is>
       </c>
       <c r="K179" s="3" t="inlineStr">
@@ -12840,7 +12840,7 @@
       </c>
       <c r="O179" s="3" t="inlineStr">
         <is>
-          <t>3.8 °C</t>
+          <t>3.9 °C</t>
         </is>
       </c>
     </row>
@@ -12867,7 +12867,7 @@
       </c>
       <c r="E180" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:04</t>
+          <t>2026-02-07 18:04:26</t>
         </is>
       </c>
       <c r="F180" s="3" t="inlineStr">
@@ -12888,7 +12888,7 @@
       </c>
       <c r="J180" s="3" t="inlineStr">
         <is>
-          <t>1006.6 hPa</t>
+          <t>1006.7 hPa</t>
         </is>
       </c>
       <c r="K180" s="3" t="inlineStr">
@@ -12940,7 +12940,7 @@
       </c>
       <c r="E181" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:07</t>
+          <t>2026-02-07 18:04:29</t>
         </is>
       </c>
       <c r="F181" s="3" t="inlineStr">
@@ -13009,7 +13009,7 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:09</t>
+          <t>2026-02-07 18:04:31</t>
         </is>
       </c>
       <c r="F182" s="3" t="inlineStr">
@@ -13030,7 +13030,7 @@
       </c>
       <c r="J182" s="3" t="inlineStr">
         <is>
-          <t>1004.4 hPa</t>
+          <t>1004.5 hPa</t>
         </is>
       </c>
       <c r="K182" s="3" t="inlineStr">
@@ -13082,7 +13082,7 @@
       </c>
       <c r="E183" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:11</t>
+          <t>2026-02-07 18:04:34</t>
         </is>
       </c>
       <c r="F183" s="3" t="inlineStr">
@@ -13151,7 +13151,7 @@
       </c>
       <c r="E184" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:14</t>
+          <t>2026-02-07 18:04:36</t>
         </is>
       </c>
       <c r="F184" s="3" t="inlineStr">
@@ -13162,7 +13162,7 @@
       <c r="G184" s="3" t="inlineStr"/>
       <c r="H184" s="3" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="I184" s="3" t="inlineStr">
@@ -13220,7 +13220,7 @@
       </c>
       <c r="E185" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:16</t>
+          <t>2026-02-07 18:04:38</t>
         </is>
       </c>
       <c r="F185" s="3" t="inlineStr">
@@ -13261,7 +13261,7 @@
       </c>
       <c r="E186" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:19</t>
+          <t>2026-02-07 18:04:40</t>
         </is>
       </c>
       <c r="F186" s="3" t="inlineStr">
@@ -13303,7 +13303,7 @@
       </c>
       <c r="O186" s="3" t="inlineStr">
         <is>
-          <t>7.7 °C</t>
+          <t>7.8 °C</t>
         </is>
       </c>
     </row>
@@ -13330,7 +13330,7 @@
       </c>
       <c r="E187" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:21</t>
+          <t>2026-02-07 18:04:43</t>
         </is>
       </c>
       <c r="F187" s="3" t="inlineStr">
@@ -13403,7 +13403,7 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:24</t>
+          <t>2026-02-07 18:04:45</t>
         </is>
       </c>
       <c r="F188" s="3" t="inlineStr">
@@ -13449,7 +13449,7 @@
       </c>
       <c r="O188" s="3" t="inlineStr">
         <is>
-          <t>8.8 °C</t>
+          <t>8.9 °C</t>
         </is>
       </c>
     </row>
@@ -13476,7 +13476,7 @@
       </c>
       <c r="E189" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:26</t>
+          <t>2026-02-07 18:04:47</t>
         </is>
       </c>
       <c r="F189" s="3" t="inlineStr">
@@ -13487,7 +13487,7 @@
       <c r="G189" s="3" t="inlineStr"/>
       <c r="H189" s="3" t="inlineStr">
         <is>
-          <t>53%</t>
+          <t>54%</t>
         </is>
       </c>
       <c r="I189" s="3" t="inlineStr">
@@ -13498,7 +13498,7 @@
       <c r="J189" s="3" t="inlineStr"/>
       <c r="K189" s="3" t="inlineStr">
         <is>
-          <t>12.0 MJ/m2</t>
+          <t>12.1 MJ/m2</t>
         </is>
       </c>
       <c r="L189" s="3" t="inlineStr">
@@ -13545,7 +13545,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:35:29</t>
+          <t>2026-02-07 18:04:50</t>
         </is>
       </c>
       <c r="F190" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Update automàtic: dades i banners [2026-02-07 18:37]
</commit_message>
<xml_diff>
--- a/config/data/resum_diari_meteocat.xlsx
+++ b/config/data/resum_diari_meteocat.xlsx
@@ -565,7 +565,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:17</t>
+          <t>2026-02-07 18:28:53</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:20</t>
+          <t>2026-02-07 18:28:55</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="O3" s="3" t="inlineStr">
         <is>
-          <t>8.2 °C</t>
+          <t>8.3 °C</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:22</t>
+          <t>2026-02-07 18:28:58</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
@@ -768,7 +768,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:24</t>
+          <t>2026-02-07 18:29:01</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="O5" s="3" t="inlineStr">
         <is>
-          <t>7.4 °C</t>
+          <t>7.5 °C</t>
         </is>
       </c>
     </row>
@@ -833,7 +833,7 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:27</t>
+          <t>2026-02-07 18:29:03</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="O6" s="3" t="inlineStr">
         <is>
-          <t>7.5 °C</t>
+          <t>7.6 °C</t>
         </is>
       </c>
     </row>
@@ -902,7 +902,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:29</t>
+          <t>2026-02-07 18:29:06</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
@@ -913,7 +913,7 @@
       <c r="G7" s="3" t="inlineStr"/>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr">
@@ -948,7 +948,7 @@
       </c>
       <c r="O7" s="3" t="inlineStr">
         <is>
-          <t>6.5 °C</t>
+          <t>6.6 °C</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:32</t>
+          <t>2026-02-07 18:29:09</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="O8" s="3" t="inlineStr">
         <is>
-          <t>-5.7 °C</t>
+          <t>-5.8 °C</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:34</t>
+          <t>2026-02-07 18:29:11</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="O9" s="3" t="inlineStr">
         <is>
-          <t>-0.6 °C</t>
+          <t>-0.7 °C</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:36</t>
+          <t>2026-02-07 18:29:14</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:39</t>
+          <t>2026-02-07 18:29:17</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
@@ -1201,7 +1201,7 @@
       <c r="G11" s="3" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>57%</t>
+          <t>58%</t>
         </is>
       </c>
       <c r="I11" s="3" t="inlineStr">
@@ -1236,7 +1236,7 @@
       </c>
       <c r="O11" s="3" t="inlineStr">
         <is>
-          <t>13.0 °C</t>
+          <t>12.9 °C</t>
         </is>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:41</t>
+          <t>2026-02-07 18:29:20</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:44</t>
+          <t>2026-02-07 18:29:22</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="J13" s="3" t="inlineStr">
         <is>
-          <t>1003.6 hPa</t>
+          <t>1003.7 hPa</t>
         </is>
       </c>
       <c r="K13" s="3" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:46</t>
+          <t>2026-02-07 18:29:25</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:49</t>
+          <t>2026-02-07 18:29:28</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:51</t>
+          <t>2026-02-07 18:29:30</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:53</t>
+          <t>2026-02-07 18:29:33</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:56</t>
+          <t>2026-02-07 18:29:35</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>1005.7 hPa</t>
+          <t>1005.8 hPa</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:57:58</t>
+          <t>2026-02-07 18:29:38</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="O19" s="3" t="inlineStr">
         <is>
-          <t>10.7 °C</t>
+          <t>10.8 °C</t>
         </is>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:00</t>
+          <t>2026-02-07 18:29:41</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="J20" s="3" t="inlineStr">
         <is>
-          <t>1005.2 hPa</t>
+          <t>1005.3 hPa</t>
         </is>
       </c>
       <c r="K20" s="3" t="inlineStr">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:03</t>
+          <t>2026-02-07 18:29:43</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="J21" s="3" t="inlineStr">
         <is>
-          <t>1004.7 hPa</t>
+          <t>1004.8 hPa</t>
         </is>
       </c>
       <c r="K21" s="3" t="inlineStr">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:05</t>
+          <t>2026-02-07 18:29:46</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
@@ -1976,7 +1976,7 @@
       <c r="G22" s="3" t="inlineStr"/>
       <c r="H22" s="3" t="inlineStr">
         <is>
-          <t>51%</t>
+          <t>52%</t>
         </is>
       </c>
       <c r="I22" s="3" t="inlineStr">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="J22" s="3" t="inlineStr">
         <is>
-          <t>1005.1 hPa</t>
+          <t>1005.2 hPa</t>
         </is>
       </c>
       <c r="K22" s="3" t="inlineStr">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:08</t>
+          <t>2026-02-07 18:29:49</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:10</t>
+          <t>2026-02-07 18:29:51</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
@@ -2114,7 +2114,7 @@
       <c r="G24" s="3" t="inlineStr"/>
       <c r="H24" s="3" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>65%</t>
         </is>
       </c>
       <c r="I24" s="3" t="inlineStr">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:12</t>
+          <t>2026-02-07 18:29:54</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:15</t>
+          <t>2026-02-07 18:29:57</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:17</t>
+          <t>2026-02-07 18:29:59</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
@@ -2321,7 +2321,7 @@
       <c r="G27" s="3" t="inlineStr"/>
       <c r="H27" s="3" t="inlineStr">
         <is>
-          <t>72%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="I27" s="3" t="inlineStr">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="O27" s="3" t="inlineStr">
         <is>
-          <t>8.0 °C</t>
+          <t>7.9 °C</t>
         </is>
       </c>
     </row>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:20</t>
+          <t>2026-02-07 18:30:01</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
@@ -2382,7 +2382,7 @@
       <c r="G28" s="3" t="inlineStr"/>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="I28" s="3" t="inlineStr">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:22</t>
+          <t>2026-02-07 18:30:04</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="J29" s="3" t="inlineStr">
         <is>
-          <t>1004.5 hPa</t>
+          <t>1004.6 hPa</t>
         </is>
       </c>
       <c r="K29" s="3" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="O29" s="3" t="inlineStr">
         <is>
-          <t>12.6 °C</t>
+          <t>12.5 °C</t>
         </is>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:25</t>
+          <t>2026-02-07 18:30:06</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
@@ -2524,7 +2524,7 @@
       <c r="G30" s="3" t="inlineStr"/>
       <c r="H30" s="3" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="I30" s="3" t="inlineStr">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="J30" s="3" t="inlineStr">
         <is>
-          <t>1004.7 hPa</t>
+          <t>1004.8 hPa</t>
         </is>
       </c>
       <c r="K30" s="3" t="inlineStr">
@@ -2586,7 +2586,7 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:27</t>
+          <t>2026-02-07 18:30:09</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
@@ -2597,7 +2597,7 @@
       <c r="G31" s="3" t="inlineStr"/>
       <c r="H31" s="3" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="I31" s="3" t="inlineStr">
@@ -2655,7 +2655,7 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:30</t>
+          <t>2026-02-07 18:30:12</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="O32" s="3" t="inlineStr">
         <is>
-          <t>11.9 °C</t>
+          <t>11.8 °C</t>
         </is>
       </c>
     </row>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:32</t>
+          <t>2026-02-07 18:30:14</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
@@ -2785,7 +2785,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:34</t>
+          <t>2026-02-07 18:30:17</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="O34" s="3" t="inlineStr">
         <is>
-          <t>9.0 °C</t>
+          <t>8.9 °C</t>
         </is>
       </c>
     </row>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:37</t>
+          <t>2026-02-07 18:30:20</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
@@ -2927,7 +2927,7 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:39</t>
+          <t>2026-02-07 18:30:22</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:42</t>
+          <t>2026-02-07 18:30:25</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
@@ -3009,7 +3009,7 @@
       </c>
       <c r="J37" s="3" t="inlineStr">
         <is>
-          <t>1005.7 hPa</t>
+          <t>1005.8 hPa</t>
         </is>
       </c>
       <c r="K37" s="3" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:44</t>
+          <t>2026-02-07 18:30:28</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
@@ -3072,7 +3072,7 @@
       <c r="G38" s="3" t="inlineStr"/>
       <c r="H38" s="3" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="I38" s="3" t="inlineStr">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:47</t>
+          <t>2026-02-07 18:30:30</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
@@ -3141,7 +3141,7 @@
       <c r="G39" s="3" t="inlineStr"/>
       <c r="H39" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I39" s="3" t="inlineStr">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:49</t>
+          <t>2026-02-07 18:30:33</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
@@ -3214,7 +3214,7 @@
       <c r="G40" s="3" t="inlineStr"/>
       <c r="H40" s="3" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I40" s="3" t="inlineStr">
@@ -3264,7 +3264,7 @@
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:51</t>
+          <t>2026-02-07 18:30:36</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
@@ -3275,7 +3275,7 @@
       <c r="G41" s="3" t="inlineStr"/>
       <c r="H41" s="3" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="I41" s="3" t="inlineStr">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="O41" s="3" t="inlineStr">
         <is>
-          <t>6.2 °C</t>
+          <t>6.3 °C</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:54</t>
+          <t>2026-02-07 18:30:39</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
@@ -3348,7 +3348,7 @@
       <c r="G42" s="3" t="inlineStr"/>
       <c r="H42" s="3" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="I42" s="3" t="inlineStr">
@@ -3383,7 +3383,7 @@
       </c>
       <c r="O42" s="3" t="inlineStr">
         <is>
-          <t>11.8 °C</t>
+          <t>11.7 °C</t>
         </is>
       </c>
     </row>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:56</t>
+          <t>2026-02-07 18:30:41</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
@@ -3483,7 +3483,7 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:58:59</t>
+          <t>2026-02-07 18:30:43</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
@@ -3494,7 +3494,7 @@
       <c r="G44" s="3" t="inlineStr"/>
       <c r="H44" s="3" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="I44" s="3" t="inlineStr">
@@ -3556,7 +3556,7 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:01</t>
+          <t>2026-02-07 18:30:46</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:03</t>
+          <t>2026-02-07 18:30:49</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
@@ -3644,7 +3644,7 @@
       <c r="G46" s="3" t="inlineStr"/>
       <c r="H46" s="3" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="I46" s="3" t="inlineStr">
@@ -3675,7 +3675,7 @@
       </c>
       <c r="O46" s="3" t="inlineStr">
         <is>
-          <t>9.2 °C</t>
+          <t>9.1 °C</t>
         </is>
       </c>
     </row>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:06</t>
+          <t>2026-02-07 18:30:51</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
@@ -3767,7 +3767,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:08</t>
+          <t>2026-02-07 18:30:54</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:11</t>
+          <t>2026-02-07 18:30:56</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:13</t>
+          <t>2026-02-07 18:30:59</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
@@ -3931,7 +3931,7 @@
       <c r="J50" s="3" t="inlineStr"/>
       <c r="K50" s="3" t="inlineStr">
         <is>
-          <t>12.1 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L50" s="3" t="inlineStr">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:15</t>
+          <t>2026-02-07 18:31:02</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
@@ -3989,7 +3989,7 @@
       <c r="G51" s="3" t="inlineStr"/>
       <c r="H51" s="3" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I51" s="3" t="inlineStr">
@@ -4024,7 +4024,7 @@
       </c>
       <c r="O51" s="3" t="inlineStr">
         <is>
-          <t>4.4 °C</t>
+          <t>4.3 °C</t>
         </is>
       </c>
     </row>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:18</t>
+          <t>2026-02-07 18:31:05</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:20</t>
+          <t>2026-02-07 18:31:07</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:23</t>
+          <t>2026-02-07 18:31:09</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
@@ -4182,7 +4182,7 @@
       </c>
       <c r="J54" s="3" t="inlineStr">
         <is>
-          <t>1005.3 hPa</t>
+          <t>1005.4 hPa</t>
         </is>
       </c>
       <c r="K54" s="3" t="inlineStr">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:25</t>
+          <t>2026-02-07 18:31:12</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
@@ -4245,7 +4245,7 @@
       <c r="G55" s="3" t="inlineStr"/>
       <c r="H55" s="3" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="I55" s="3" t="inlineStr">
@@ -4307,7 +4307,7 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:27</t>
+          <t>2026-02-07 18:31:15</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
@@ -4372,7 +4372,7 @@
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:30</t>
+          <t>2026-02-07 18:31:18</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
@@ -4445,7 +4445,7 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:32</t>
+          <t>2026-02-07 18:31:20</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
@@ -4514,7 +4514,7 @@
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:35</t>
+          <t>2026-02-07 18:31:22</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="O59" s="3" t="inlineStr">
         <is>
-          <t>11.5 °C</t>
+          <t>11.4 °C</t>
         </is>
       </c>
     </row>
@@ -4575,7 +4575,7 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:37</t>
+          <t>2026-02-07 18:31:24</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
@@ -4590,7 +4590,7 @@
       </c>
       <c r="H60" s="3" t="inlineStr">
         <is>
-          <t>59%</t>
+          <t>58%</t>
         </is>
       </c>
       <c r="I60" s="3" t="inlineStr">
@@ -4648,7 +4648,7 @@
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:39</t>
+          <t>2026-02-07 18:31:27</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:42</t>
+          <t>2026-02-07 18:31:30</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
@@ -4732,7 +4732,7 @@
       <c r="G62" s="3" t="inlineStr"/>
       <c r="H62" s="3" t="inlineStr">
         <is>
-          <t>63%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="I62" s="3" t="inlineStr">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:44</t>
+          <t>2026-02-07 18:31:32</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="H63" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="I63" s="3" t="inlineStr">
@@ -4823,12 +4823,12 @@
       </c>
       <c r="N63" s="3" t="inlineStr">
         <is>
-          <t>-1.6 °C 17:29 TU</t>
+          <t>-1.8 °C 17:59 TU</t>
         </is>
       </c>
       <c r="O63" s="3" t="inlineStr">
         <is>
-          <t>0.6 °C</t>
+          <t>0.5 °C</t>
         </is>
       </c>
     </row>
@@ -4855,7 +4855,7 @@
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:46</t>
+          <t>2026-02-07 18:31:35</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
@@ -4866,7 +4866,7 @@
       <c r="G64" s="3" t="inlineStr"/>
       <c r="H64" s="3" t="inlineStr">
         <is>
-          <t>56%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="I64" s="3" t="inlineStr">
@@ -4896,12 +4896,12 @@
       </c>
       <c r="N64" s="3" t="inlineStr">
         <is>
-          <t>7.5 °C 17:29 TU</t>
+          <t>7.0 °C 17:32 TU</t>
         </is>
       </c>
       <c r="O64" s="3" t="inlineStr">
         <is>
-          <t>9.5 °C</t>
+          <t>9.4 °C</t>
         </is>
       </c>
     </row>
@@ -4928,7 +4928,7 @@
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:49</t>
+          <t>2026-02-07 18:31:37</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
@@ -4989,7 +4989,7 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:51</t>
+          <t>2026-02-07 18:31:40</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
@@ -5050,7 +5050,7 @@
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:53</t>
+          <t>2026-02-07 18:31:42</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
@@ -5119,7 +5119,7 @@
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:56</t>
+          <t>2026-02-07 18:31:45</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="O68" s="3" t="inlineStr">
         <is>
-          <t>7.5 °C</t>
+          <t>7.4 °C</t>
         </is>
       </c>
     </row>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 17:59:58</t>
+          <t>2026-02-07 18:31:47</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:01</t>
+          <t>2026-02-07 18:31:49</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:03</t>
+          <t>2026-02-07 18:31:52</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
@@ -5364,7 +5364,7 @@
       </c>
       <c r="O71" s="3" t="inlineStr">
         <is>
-          <t>8.2 °C</t>
+          <t>8.3 °C</t>
         </is>
       </c>
     </row>
@@ -5391,7 +5391,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:06</t>
+          <t>2026-02-07 18:31:55</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
@@ -5452,7 +5452,7 @@
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:08</t>
+          <t>2026-02-07 18:31:57</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
@@ -5463,7 +5463,7 @@
       <c r="G73" s="3" t="inlineStr"/>
       <c r="H73" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I73" s="3" t="inlineStr">
@@ -5525,7 +5525,7 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:10</t>
+          <t>2026-02-07 18:32:00</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
@@ -5536,7 +5536,7 @@
       <c r="G74" s="3" t="inlineStr"/>
       <c r="H74" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="I74" s="3" t="inlineStr">
@@ -5586,7 +5586,7 @@
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:13</t>
+          <t>2026-02-07 18:32:02</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
@@ -5632,7 +5632,7 @@
       </c>
       <c r="O75" s="3" t="inlineStr">
         <is>
-          <t>7.7 °C</t>
+          <t>7.8 °C</t>
         </is>
       </c>
     </row>
@@ -5659,7 +5659,7 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:15</t>
+          <t>2026-02-07 18:32:05</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:17</t>
+          <t>2026-02-07 18:32:08</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
@@ -5743,7 +5743,7 @@
       <c r="G77" s="3" t="inlineStr"/>
       <c r="H77" s="3" t="inlineStr">
         <is>
-          <t>49%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="I77" s="3" t="inlineStr">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:20</t>
+          <t>2026-02-07 18:32:10</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
@@ -5812,7 +5812,7 @@
       <c r="G78" s="3" t="inlineStr"/>
       <c r="H78" s="3" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="I78" s="3" t="inlineStr">
@@ -5870,7 +5870,7 @@
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:22</t>
+          <t>2026-02-07 18:32:13</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
@@ -5896,7 +5896,7 @@
       </c>
       <c r="K79" s="3" t="inlineStr">
         <is>
-          <t>11.9 MJ/m2</t>
+          <t>11.8 MJ/m2</t>
         </is>
       </c>
       <c r="L79" s="3" t="inlineStr">
@@ -5943,7 +5943,7 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:24</t>
+          <t>2026-02-07 18:32:16</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
@@ -6012,7 +6012,7 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:27</t>
+          <t>2026-02-07 18:32:18</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
@@ -6033,7 +6033,7 @@
       </c>
       <c r="J81" s="3" t="inlineStr">
         <is>
-          <t>1003.6 hPa</t>
+          <t>1003.7 hPa</t>
         </is>
       </c>
       <c r="K81" s="3" t="inlineStr">
@@ -6058,7 +6058,7 @@
       </c>
       <c r="O81" s="3" t="inlineStr">
         <is>
-          <t>10.5 °C</t>
+          <t>10.4 °C</t>
         </is>
       </c>
     </row>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:29</t>
+          <t>2026-02-07 18:32:21</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
@@ -6096,7 +6096,7 @@
       <c r="G82" s="3" t="inlineStr"/>
       <c r="H82" s="3" t="inlineStr">
         <is>
-          <t>58%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="I82" s="3" t="inlineStr">
@@ -6119,7 +6119,7 @@
       </c>
       <c r="O82" s="3" t="inlineStr">
         <is>
-          <t>10.8 °C</t>
+          <t>10.7 °C</t>
         </is>
       </c>
     </row>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:31</t>
+          <t>2026-02-07 18:32:23</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
@@ -6187,12 +6187,12 @@
       </c>
       <c r="N83" s="3" t="inlineStr">
         <is>
-          <t>-7.6 °C 17:29 TU</t>
+          <t>-7.7 °C 17:59 TU</t>
         </is>
       </c>
       <c r="O83" s="3" t="inlineStr">
         <is>
-          <t>-5.3 °C</t>
+          <t>-5.4 °C</t>
         </is>
       </c>
     </row>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:33</t>
+          <t>2026-02-07 18:32:26</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
@@ -6288,7 +6288,7 @@
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:36</t>
+          <t>2026-02-07 18:32:29</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
@@ -6322,7 +6322,7 @@
       </c>
       <c r="O85" s="3" t="inlineStr">
         <is>
-          <t>7.4 °C</t>
+          <t>7.3 °C</t>
         </is>
       </c>
     </row>
@@ -6349,7 +6349,7 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:38</t>
+          <t>2026-02-07 18:32:31</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
@@ -6422,7 +6422,7 @@
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:42</t>
+          <t>2026-02-07 18:32:34</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
@@ -6443,7 +6443,7 @@
       </c>
       <c r="J87" s="3" t="inlineStr">
         <is>
-          <t>1005.3 hPa</t>
+          <t>1005.4 hPa</t>
         </is>
       </c>
       <c r="K87" s="3" t="inlineStr"/>
@@ -6464,7 +6464,7 @@
       </c>
       <c r="O87" s="3" t="inlineStr">
         <is>
-          <t>4.6 °C</t>
+          <t>4.5 °C</t>
         </is>
       </c>
     </row>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:44</t>
+          <t>2026-02-07 18:32:36</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:46</t>
+          <t>2026-02-07 18:32:39</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
@@ -6543,7 +6543,7 @@
       <c r="G89" s="3" t="inlineStr"/>
       <c r="H89" s="3" t="inlineStr">
         <is>
-          <t>62%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="I89" s="3" t="inlineStr">
@@ -6553,7 +6553,7 @@
       </c>
       <c r="J89" s="3" t="inlineStr">
         <is>
-          <t>1007.2 hPa</t>
+          <t>1007.1 hPa</t>
         </is>
       </c>
       <c r="K89" s="3" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:49</t>
+          <t>2026-02-07 18:32:41</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
@@ -6626,7 +6626,7 @@
       </c>
       <c r="J90" s="3" t="inlineStr">
         <is>
-          <t>1005.8 hPa</t>
+          <t>1005.9 hPa</t>
         </is>
       </c>
       <c r="K90" s="3" t="inlineStr">
@@ -6678,7 +6678,7 @@
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:51</t>
+          <t>2026-02-07 18:32:44</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
@@ -6747,7 +6747,7 @@
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:53</t>
+          <t>2026-02-07 18:32:46</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
@@ -6758,7 +6758,7 @@
       <c r="G92" s="3" t="inlineStr"/>
       <c r="H92" s="3" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="I92" s="3" t="inlineStr"/>
@@ -6812,7 +6812,7 @@
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:56</t>
+          <t>2026-02-07 18:32:49</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
@@ -6881,7 +6881,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:00:58</t>
+          <t>2026-02-07 18:32:51</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
@@ -6912,7 +6912,7 @@
       </c>
       <c r="L94" s="3" t="inlineStr">
         <is>
-          <t>13.7 km/h - 295º 4:16 TU</t>
+          <t>19.1 km/h - 229º 17:50 TU</t>
         </is>
       </c>
       <c r="M94" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
       </c>
       <c r="O94" s="3" t="inlineStr">
         <is>
-          <t>-5.7 °C</t>
+          <t>-5.8 °C</t>
         </is>
       </c>
     </row>
@@ -6954,7 +6954,7 @@
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:01</t>
+          <t>2026-02-07 18:32:53</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
@@ -7027,7 +7027,7 @@
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:03</t>
+          <t>2026-02-07 18:32:56</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
@@ -7038,7 +7038,7 @@
       <c r="G96" s="3" t="inlineStr"/>
       <c r="H96" s="3" t="inlineStr">
         <is>
-          <t>59%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="I96" s="3" t="inlineStr">
@@ -7096,7 +7096,7 @@
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:06</t>
+          <t>2026-02-07 18:32:59</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
@@ -7169,7 +7169,7 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:08</t>
+          <t>2026-02-07 18:33:02</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
@@ -7211,7 +7211,7 @@
       </c>
       <c r="O98" s="3" t="inlineStr">
         <is>
-          <t>5.3 °C</t>
+          <t>5.2 °C</t>
         </is>
       </c>
     </row>
@@ -7238,7 +7238,7 @@
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:11</t>
+          <t>2026-02-07 18:33:05</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
@@ -7280,7 +7280,7 @@
       </c>
       <c r="O99" s="3" t="inlineStr">
         <is>
-          <t>8.5 °C</t>
+          <t>8.6 °C</t>
         </is>
       </c>
     </row>
@@ -7307,7 +7307,7 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:13</t>
+          <t>2026-02-07 18:33:07</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
@@ -7353,7 +7353,7 @@
       </c>
       <c r="O100" s="3" t="inlineStr">
         <is>
-          <t>7.3 °C</t>
+          <t>7.4 °C</t>
         </is>
       </c>
     </row>
@@ -7380,7 +7380,7 @@
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:16</t>
+          <t>2026-02-07 18:33:10</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
@@ -7391,7 +7391,7 @@
       <c r="G101" s="3" t="inlineStr"/>
       <c r="H101" s="3" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="I101" s="3" t="inlineStr">
@@ -7449,7 +7449,7 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:18</t>
+          <t>2026-02-07 18:33:13</t>
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
@@ -7460,7 +7460,7 @@
       <c r="G102" s="3" t="inlineStr"/>
       <c r="H102" s="3" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="I102" s="3" t="inlineStr">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="J102" s="3" t="inlineStr">
         <is>
-          <t>1004.1 hPa</t>
+          <t>1004.2 hPa</t>
         </is>
       </c>
       <c r="K102" s="3" t="inlineStr">
@@ -7495,7 +7495,7 @@
       </c>
       <c r="O102" s="3" t="inlineStr">
         <is>
-          <t>11.7 °C</t>
+          <t>11.8 °C</t>
         </is>
       </c>
     </row>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:20</t>
+          <t>2026-02-07 18:33:15</t>
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
@@ -7533,7 +7533,7 @@
       <c r="G103" s="3" t="inlineStr"/>
       <c r="H103" s="3" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="I103" s="3" t="inlineStr">
@@ -7543,7 +7543,7 @@
       </c>
       <c r="J103" s="3" t="inlineStr">
         <is>
-          <t>1007.9 hPa</t>
+          <t>1007.8 hPa</t>
         </is>
       </c>
       <c r="K103" s="3" t="inlineStr">
@@ -7595,7 +7595,7 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:22</t>
+          <t>2026-02-07 18:33:18</t>
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
@@ -7606,7 +7606,7 @@
       <c r="G104" s="3" t="inlineStr"/>
       <c r="H104" s="3" t="inlineStr">
         <is>
-          <t>46%</t>
+          <t>47%</t>
         </is>
       </c>
       <c r="I104" s="3" t="inlineStr">
@@ -7641,7 +7641,7 @@
       </c>
       <c r="O104" s="3" t="inlineStr">
         <is>
-          <t>12.4 °C</t>
+          <t>12.3 °C</t>
         </is>
       </c>
     </row>
@@ -7668,7 +7668,7 @@
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:25</t>
+          <t>2026-02-07 18:33:21</t>
         </is>
       </c>
       <c r="F105" s="3" t="inlineStr">
@@ -7737,7 +7737,7 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:27</t>
+          <t>2026-02-07 18:33:24</t>
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
@@ -7748,7 +7748,7 @@
       <c r="G106" s="3" t="inlineStr"/>
       <c r="H106" s="3" t="inlineStr">
         <is>
-          <t>53%</t>
+          <t>52%</t>
         </is>
       </c>
       <c r="I106" s="3" t="inlineStr">
@@ -7802,7 +7802,7 @@
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:30</t>
+          <t>2026-02-07 18:33:26</t>
         </is>
       </c>
       <c r="F107" s="3" t="inlineStr">
@@ -7813,7 +7813,7 @@
       <c r="G107" s="3" t="inlineStr"/>
       <c r="H107" s="3" t="inlineStr">
         <is>
-          <t>63%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="I107" s="3" t="inlineStr">
@@ -7824,7 +7824,7 @@
       <c r="J107" s="3" t="inlineStr"/>
       <c r="K107" s="3" t="inlineStr">
         <is>
-          <t>12.4 MJ/m2</t>
+          <t>12.3 MJ/m2</t>
         </is>
       </c>
       <c r="L107" s="3" t="inlineStr">
@@ -7871,7 +7871,7 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:32</t>
+          <t>2026-02-07 18:33:29</t>
         </is>
       </c>
       <c r="F108" s="3" t="inlineStr">
@@ -7944,7 +7944,7 @@
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:35</t>
+          <t>2026-02-07 18:33:32</t>
         </is>
       </c>
       <c r="F109" s="3" t="inlineStr">
@@ -7955,7 +7955,7 @@
       <c r="G109" s="3" t="inlineStr"/>
       <c r="H109" s="3" t="inlineStr">
         <is>
-          <t>74%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="I109" s="3" t="inlineStr">
@@ -8017,7 +8017,7 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:37</t>
+          <t>2026-02-07 18:33:34</t>
         </is>
       </c>
       <c r="F110" s="3" t="inlineStr">
@@ -8042,7 +8042,7 @@
       </c>
       <c r="J110" s="3" t="inlineStr">
         <is>
-          <t>1003.7 hPa</t>
+          <t>1003.8 hPa</t>
         </is>
       </c>
       <c r="K110" s="3" t="inlineStr">
@@ -8094,7 +8094,7 @@
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:40</t>
+          <t>2026-02-07 18:33:37</t>
         </is>
       </c>
       <c r="F111" s="3" t="inlineStr">
@@ -8163,7 +8163,7 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:42</t>
+          <t>2026-02-07 18:33:40</t>
         </is>
       </c>
       <c r="F112" s="3" t="inlineStr">
@@ -8204,12 +8204,12 @@
       </c>
       <c r="N112" s="3" t="inlineStr">
         <is>
-          <t>9.4 °C 2:41 TU</t>
+          <t>9.1 °C 17:59 TU</t>
         </is>
       </c>
       <c r="O112" s="3" t="inlineStr">
         <is>
-          <t>12.5 °C</t>
+          <t>12.4 °C</t>
         </is>
       </c>
     </row>
@@ -8236,7 +8236,7 @@
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:45</t>
+          <t>2026-02-07 18:33:42</t>
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
@@ -8277,7 +8277,7 @@
       </c>
       <c r="N113" s="3" t="inlineStr">
         <is>
-          <t>-6.2 °C 17:07 TU</t>
+          <t>-6.4 °C 17:48 TU</t>
         </is>
       </c>
       <c r="O113" s="3" t="inlineStr">
@@ -8309,7 +8309,7 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:47</t>
+          <t>2026-02-07 18:33:45</t>
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
@@ -8343,7 +8343,7 @@
       </c>
       <c r="O114" s="3" t="inlineStr">
         <is>
-          <t>6.0 °C</t>
+          <t>6.1 °C</t>
         </is>
       </c>
     </row>
@@ -8370,7 +8370,7 @@
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:49</t>
+          <t>2026-02-07 18:33:47</t>
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
@@ -8391,7 +8391,7 @@
       </c>
       <c r="J115" s="3" t="inlineStr">
         <is>
-          <t>1007.3 hPa</t>
+          <t>1007.4 hPa</t>
         </is>
       </c>
       <c r="K115" s="3" t="inlineStr">
@@ -8443,7 +8443,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:52</t>
+          <t>2026-02-07 18:33:50</t>
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
@@ -8516,7 +8516,7 @@
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:54</t>
+          <t>2026-02-07 18:33:53</t>
         </is>
       </c>
       <c r="F117" s="3" t="inlineStr">
@@ -8585,7 +8585,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:56</t>
+          <t>2026-02-07 18:33:56</t>
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
@@ -8626,7 +8626,7 @@
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:01:59</t>
+          <t>2026-02-07 18:33:58</t>
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
@@ -8637,7 +8637,7 @@
       <c r="G119" s="3" t="inlineStr"/>
       <c r="H119" s="3" t="inlineStr">
         <is>
-          <t>56%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="I119" s="3" t="inlineStr">
@@ -8687,7 +8687,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:01</t>
+          <t>2026-02-07 18:34:01</t>
         </is>
       </c>
       <c r="F120" s="3" t="inlineStr">
@@ -8756,7 +8756,7 @@
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:03</t>
+          <t>2026-02-07 18:34:04</t>
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
@@ -8825,7 +8825,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:06</t>
+          <t>2026-02-07 18:34:07</t>
         </is>
       </c>
       <c r="F122" s="3" t="inlineStr">
@@ -8836,7 +8836,7 @@
       <c r="G122" s="3" t="inlineStr"/>
       <c r="H122" s="3" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>65%</t>
         </is>
       </c>
       <c r="I122" s="3" t="inlineStr">
@@ -8871,7 +8871,7 @@
       </c>
       <c r="O122" s="3" t="inlineStr">
         <is>
-          <t>8.7 °C</t>
+          <t>8.8 °C</t>
         </is>
       </c>
     </row>
@@ -8898,7 +8898,7 @@
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:08</t>
+          <t>2026-02-07 18:34:09</t>
         </is>
       </c>
       <c r="F123" s="3" t="inlineStr">
@@ -8924,7 +8924,7 @@
       </c>
       <c r="K123" s="3" t="inlineStr">
         <is>
-          <t>7.1 MJ/m2</t>
+          <t>7.0 MJ/m2</t>
         </is>
       </c>
       <c r="L123" s="3" t="inlineStr">
@@ -8944,7 +8944,7 @@
       </c>
       <c r="O123" s="3" t="inlineStr">
         <is>
-          <t>5.4 °C</t>
+          <t>5.5 °C</t>
         </is>
       </c>
     </row>
@@ -8971,7 +8971,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:11</t>
+          <t>2026-02-07 18:34:12</t>
         </is>
       </c>
       <c r="F124" s="3" t="inlineStr">
@@ -9002,7 +9002,7 @@
       </c>
       <c r="L124" s="3" t="inlineStr">
         <is>
-          <t>31.0 km/h - 175º 17:25 TU</t>
+          <t>31.3 km/h - 188º 17:30 TU</t>
         </is>
       </c>
       <c r="M124" s="3" t="inlineStr">
@@ -9044,7 +9044,7 @@
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:13</t>
+          <t>2026-02-07 18:34:15</t>
         </is>
       </c>
       <c r="F125" s="3" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:15</t>
+          <t>2026-02-07 18:34:17</t>
         </is>
       </c>
       <c r="F126" s="3" t="inlineStr">
@@ -9182,7 +9182,7 @@
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:18</t>
+          <t>2026-02-07 18:34:20</t>
         </is>
       </c>
       <c r="F127" s="3" t="inlineStr">
@@ -9193,7 +9193,7 @@
       <c r="G127" s="3" t="inlineStr"/>
       <c r="H127" s="3" t="inlineStr">
         <is>
-          <t>76%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="I127" s="3" t="inlineStr">
@@ -9228,7 +9228,7 @@
       </c>
       <c r="O127" s="3" t="inlineStr">
         <is>
-          <t>10.5 °C</t>
+          <t>10.4 °C</t>
         </is>
       </c>
     </row>
@@ -9255,7 +9255,7 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:20</t>
+          <t>2026-02-07 18:34:23</t>
         </is>
       </c>
       <c r="F128" s="3" t="inlineStr">
@@ -9276,7 +9276,7 @@
       </c>
       <c r="J128" s="3" t="inlineStr">
         <is>
-          <t>1005.3 hPa</t>
+          <t>1005.4 hPa</t>
         </is>
       </c>
       <c r="K128" s="3" t="inlineStr">
@@ -9328,7 +9328,7 @@
       </c>
       <c r="E129" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:23</t>
+          <t>2026-02-07 18:34:25</t>
         </is>
       </c>
       <c r="F129" s="3" t="inlineStr">
@@ -9350,7 +9350,7 @@
       <c r="J129" s="3" t="inlineStr"/>
       <c r="K129" s="3" t="inlineStr">
         <is>
-          <t>8.9 MJ/m2</t>
+          <t>8.8 MJ/m2</t>
         </is>
       </c>
       <c r="L129" s="3" t="inlineStr">
@@ -9397,7 +9397,7 @@
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:25</t>
+          <t>2026-02-07 18:34:28</t>
         </is>
       </c>
       <c r="F130" s="3" t="inlineStr">
@@ -9408,7 +9408,7 @@
       <c r="G130" s="3" t="inlineStr"/>
       <c r="H130" s="3" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="I130" s="3" t="inlineStr">
@@ -9439,7 +9439,7 @@
       </c>
       <c r="O130" s="3" t="inlineStr">
         <is>
-          <t>5.5 °C</t>
+          <t>5.4 °C</t>
         </is>
       </c>
     </row>
@@ -9466,7 +9466,7 @@
       </c>
       <c r="E131" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:27</t>
+          <t>2026-02-07 18:34:31</t>
         </is>
       </c>
       <c r="F131" s="3" t="inlineStr">
@@ -9487,7 +9487,7 @@
       </c>
       <c r="J131" s="3" t="inlineStr">
         <is>
-          <t>1003.0 hPa</t>
+          <t>1003.1 hPa</t>
         </is>
       </c>
       <c r="K131" s="3" t="inlineStr">
@@ -9539,7 +9539,7 @@
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:30</t>
+          <t>2026-02-07 18:34:34</t>
         </is>
       </c>
       <c r="F132" s="3" t="inlineStr">
@@ -9612,7 +9612,7 @@
       </c>
       <c r="E133" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:32</t>
+          <t>2026-02-07 18:34:36</t>
         </is>
       </c>
       <c r="F133" s="3" t="inlineStr">
@@ -9685,7 +9685,7 @@
       </c>
       <c r="E134" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:35</t>
+          <t>2026-02-07 18:34:39</t>
         </is>
       </c>
       <c r="F134" s="3" t="inlineStr">
@@ -9754,7 +9754,7 @@
       </c>
       <c r="E135" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:37</t>
+          <t>2026-02-07 18:34:42</t>
         </is>
       </c>
       <c r="F135" s="3" t="inlineStr">
@@ -9795,12 +9795,12 @@
       </c>
       <c r="N135" s="3" t="inlineStr">
         <is>
-          <t>-5.4 °C 5:53 TU</t>
+          <t>-5.5 °C 17:43 TU</t>
         </is>
       </c>
       <c r="O135" s="3" t="inlineStr">
         <is>
-          <t>-1.9 °C</t>
+          <t>-2.0 °C</t>
         </is>
       </c>
     </row>
@@ -9827,7 +9827,7 @@
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:40</t>
+          <t>2026-02-07 18:34:45</t>
         </is>
       </c>
       <c r="F136" s="3" t="inlineStr">
@@ -9896,7 +9896,7 @@
       </c>
       <c r="E137" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:42</t>
+          <t>2026-02-07 18:34:48</t>
         </is>
       </c>
       <c r="F137" s="3" t="inlineStr">
@@ -9965,7 +9965,7 @@
       </c>
       <c r="E138" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:45</t>
+          <t>2026-02-07 18:34:50</t>
         </is>
       </c>
       <c r="F138" s="3" t="inlineStr">
@@ -9976,7 +9976,7 @@
       <c r="G138" s="3" t="inlineStr"/>
       <c r="H138" s="3" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="I138" s="3" t="inlineStr">
@@ -10034,7 +10034,7 @@
       </c>
       <c r="E139" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:47</t>
+          <t>2026-02-07 18:34:53</t>
         </is>
       </c>
       <c r="F139" s="3" t="inlineStr">
@@ -10111,7 +10111,7 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:50</t>
+          <t>2026-02-07 18:34:56</t>
         </is>
       </c>
       <c r="F140" s="3" t="inlineStr">
@@ -10122,7 +10122,7 @@
       <c r="G140" s="3" t="inlineStr"/>
       <c r="H140" s="3" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>74%</t>
         </is>
       </c>
       <c r="I140" s="3" t="inlineStr">
@@ -10132,7 +10132,7 @@
       </c>
       <c r="J140" s="3" t="inlineStr">
         <is>
-          <t>1003.7 hPa</t>
+          <t>1003.8 hPa</t>
         </is>
       </c>
       <c r="K140" s="3" t="inlineStr">
@@ -10184,7 +10184,7 @@
       </c>
       <c r="E141" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:52</t>
+          <t>2026-02-07 18:34:58</t>
         </is>
       </c>
       <c r="F141" s="3" t="inlineStr">
@@ -10205,7 +10205,7 @@
       </c>
       <c r="J141" s="3" t="inlineStr">
         <is>
-          <t>1005.0 hPa</t>
+          <t>1005.1 hPa</t>
         </is>
       </c>
       <c r="K141" s="3" t="inlineStr">
@@ -10257,7 +10257,7 @@
       </c>
       <c r="E142" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:55</t>
+          <t>2026-02-07 18:35:01</t>
         </is>
       </c>
       <c r="F142" s="3" t="inlineStr">
@@ -10326,7 +10326,7 @@
       </c>
       <c r="E143" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:02:57</t>
+          <t>2026-02-07 18:35:04</t>
         </is>
       </c>
       <c r="F143" s="3" t="inlineStr">
@@ -10395,7 +10395,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:00</t>
+          <t>2026-02-07 18:35:06</t>
         </is>
       </c>
       <c r="F144" s="3" t="inlineStr">
@@ -10441,7 +10441,7 @@
       </c>
       <c r="O144" s="3" t="inlineStr">
         <is>
-          <t>12.9 °C</t>
+          <t>13.0 °C</t>
         </is>
       </c>
     </row>
@@ -10468,7 +10468,7 @@
       </c>
       <c r="E145" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:02</t>
+          <t>2026-02-07 18:35:09</t>
         </is>
       </c>
       <c r="F145" s="3" t="inlineStr">
@@ -10509,7 +10509,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:04</t>
+          <t>2026-02-07 18:35:11</t>
         </is>
       </c>
       <c r="F146" s="3" t="inlineStr">
@@ -10574,7 +10574,7 @@
       </c>
       <c r="E147" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:06</t>
+          <t>2026-02-07 18:35:14</t>
         </is>
       </c>
       <c r="F147" s="3" t="inlineStr">
@@ -10643,7 +10643,7 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:09</t>
+          <t>2026-02-07 18:35:17</t>
         </is>
       </c>
       <c r="F148" s="3" t="inlineStr">
@@ -10712,7 +10712,7 @@
       </c>
       <c r="E149" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:11</t>
+          <t>2026-02-07 18:35:19</t>
         </is>
       </c>
       <c r="F149" s="3" t="inlineStr">
@@ -10723,7 +10723,7 @@
       <c r="G149" s="3" t="inlineStr"/>
       <c r="H149" s="3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="I149" s="3" t="inlineStr">
@@ -10733,7 +10733,7 @@
       </c>
       <c r="J149" s="3" t="inlineStr">
         <is>
-          <t>1005.5 hPa</t>
+          <t>1005.6 hPa</t>
         </is>
       </c>
       <c r="K149" s="3" t="inlineStr"/>
@@ -10754,7 +10754,7 @@
       </c>
       <c r="O149" s="3" t="inlineStr">
         <is>
-          <t>4.9 °C</t>
+          <t>5.0 °C</t>
         </is>
       </c>
     </row>
@@ -10781,7 +10781,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:14</t>
+          <t>2026-02-07 18:35:22</t>
         </is>
       </c>
       <c r="F150" s="3" t="inlineStr">
@@ -10792,7 +10792,7 @@
       <c r="G150" s="3" t="inlineStr"/>
       <c r="H150" s="3" t="inlineStr">
         <is>
-          <t>56%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="I150" s="3" t="inlineStr">
@@ -10815,7 +10815,7 @@
       </c>
       <c r="O150" s="3" t="inlineStr">
         <is>
-          <t>11.4 °C</t>
+          <t>11.3 °C</t>
         </is>
       </c>
     </row>
@@ -10842,7 +10842,7 @@
       </c>
       <c r="E151" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:16</t>
+          <t>2026-02-07 18:35:24</t>
         </is>
       </c>
       <c r="F151" s="3" t="inlineStr">
@@ -10853,7 +10853,7 @@
       <c r="G151" s="3" t="inlineStr"/>
       <c r="H151" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="I151" s="3" t="inlineStr">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="J151" s="3" t="inlineStr">
         <is>
-          <t>1004.1 hPa</t>
+          <t>1004.2 hPa</t>
         </is>
       </c>
       <c r="K151" s="3" t="inlineStr">
@@ -10915,7 +10915,7 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:19</t>
+          <t>2026-02-07 18:35:27</t>
         </is>
       </c>
       <c r="F152" s="3" t="inlineStr">
@@ -10926,7 +10926,7 @@
       <c r="G152" s="3" t="inlineStr"/>
       <c r="H152" s="3" t="inlineStr">
         <is>
-          <t>58%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="I152" s="3" t="inlineStr">
@@ -10957,7 +10957,7 @@
       </c>
       <c r="O152" s="3" t="inlineStr">
         <is>
-          <t>11.0 °C</t>
+          <t>10.9 °C</t>
         </is>
       </c>
     </row>
@@ -10984,7 +10984,7 @@
       </c>
       <c r="E153" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:21</t>
+          <t>2026-02-07 18:35:30</t>
         </is>
       </c>
       <c r="F153" s="3" t="inlineStr">
@@ -11005,7 +11005,7 @@
       </c>
       <c r="J153" s="3" t="inlineStr">
         <is>
-          <t>1006.0 hPa</t>
+          <t>1006.1 hPa</t>
         </is>
       </c>
       <c r="K153" s="3" t="inlineStr">
@@ -11057,7 +11057,7 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:24</t>
+          <t>2026-02-07 18:35:32</t>
         </is>
       </c>
       <c r="F154" s="3" t="inlineStr">
@@ -11126,7 +11126,7 @@
       </c>
       <c r="E155" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:26</t>
+          <t>2026-02-07 18:35:35</t>
         </is>
       </c>
       <c r="F155" s="3" t="inlineStr">
@@ -11195,7 +11195,7 @@
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:28</t>
+          <t>2026-02-07 18:35:37</t>
         </is>
       </c>
       <c r="F156" s="3" t="inlineStr">
@@ -11237,7 +11237,7 @@
       </c>
       <c r="O156" s="3" t="inlineStr">
         <is>
-          <t>8.6 °C</t>
+          <t>8.7 °C</t>
         </is>
       </c>
     </row>
@@ -11264,7 +11264,7 @@
       </c>
       <c r="E157" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:31</t>
+          <t>2026-02-07 18:35:39</t>
         </is>
       </c>
       <c r="F157" s="3" t="inlineStr">
@@ -11279,7 +11279,7 @@
       </c>
       <c r="H157" s="3" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="I157" s="3" t="inlineStr">
@@ -11295,12 +11295,12 @@
       </c>
       <c r="L157" s="3" t="inlineStr">
         <is>
-          <t>43.2 km/h - 302º 17:23 TU</t>
+          <t>48.6 km/h - 300º 17:56 TU</t>
         </is>
       </c>
       <c r="M157" s="3" t="inlineStr">
         <is>
-          <t>-1.5 °C 17:29 TU</t>
+          <t>-1.2 °C 17:59 TU</t>
         </is>
       </c>
       <c r="N157" s="3" t="inlineStr">
@@ -11310,7 +11310,7 @@
       </c>
       <c r="O157" s="3" t="inlineStr">
         <is>
-          <t>-4.7 °C</t>
+          <t>-4.6 °C</t>
         </is>
       </c>
     </row>
@@ -11337,7 +11337,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:33</t>
+          <t>2026-02-07 18:35:42</t>
         </is>
       </c>
       <c r="F158" s="3" t="inlineStr">
@@ -11348,7 +11348,7 @@
       <c r="G158" s="3" t="inlineStr"/>
       <c r="H158" s="3" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="I158" s="3" t="inlineStr">
@@ -11410,7 +11410,7 @@
       </c>
       <c r="E159" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:36</t>
+          <t>2026-02-07 18:35:44</t>
         </is>
       </c>
       <c r="F159" s="3" t="inlineStr">
@@ -11479,7 +11479,7 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:38</t>
+          <t>2026-02-07 18:35:47</t>
         </is>
       </c>
       <c r="F160" s="3" t="inlineStr">
@@ -11540,7 +11540,7 @@
       </c>
       <c r="E161" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:41</t>
+          <t>2026-02-07 18:35:49</t>
         </is>
       </c>
       <c r="F161" s="3" t="inlineStr">
@@ -11613,7 +11613,7 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:43</t>
+          <t>2026-02-07 18:35:52</t>
         </is>
       </c>
       <c r="F162" s="3" t="inlineStr">
@@ -11682,7 +11682,7 @@
       </c>
       <c r="E163" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:45</t>
+          <t>2026-02-07 18:35:54</t>
         </is>
       </c>
       <c r="F163" s="3" t="inlineStr">
@@ -11693,7 +11693,7 @@
       <c r="G163" s="3" t="inlineStr"/>
       <c r="H163" s="3" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>65%</t>
         </is>
       </c>
       <c r="I163" s="3" t="inlineStr">
@@ -11724,7 +11724,7 @@
       </c>
       <c r="O163" s="3" t="inlineStr">
         <is>
-          <t>9.3 °C</t>
+          <t>9.4 °C</t>
         </is>
       </c>
     </row>
@@ -11751,7 +11751,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:48</t>
+          <t>2026-02-07 18:35:57</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr">
@@ -11772,7 +11772,7 @@
       </c>
       <c r="J164" s="3" t="inlineStr">
         <is>
-          <t>1006.1 hPa</t>
+          <t>1006.2 hPa</t>
         </is>
       </c>
       <c r="K164" s="3" t="inlineStr">
@@ -11824,7 +11824,7 @@
       </c>
       <c r="E165" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:50</t>
+          <t>2026-02-07 18:35:59</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr">
@@ -11835,7 +11835,7 @@
       <c r="G165" s="3" t="inlineStr"/>
       <c r="H165" s="3" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="I165" s="3" t="inlineStr">
@@ -11893,7 +11893,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:53</t>
+          <t>2026-02-07 18:36:02</t>
         </is>
       </c>
       <c r="F166" s="3" t="inlineStr">
@@ -11954,7 +11954,7 @@
       </c>
       <c r="E167" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:55</t>
+          <t>2026-02-07 18:36:03</t>
         </is>
       </c>
       <c r="F167" s="3" t="inlineStr">
@@ -12015,7 +12015,7 @@
       </c>
       <c r="E168" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:03:57</t>
+          <t>2026-02-07 18:36:06</t>
         </is>
       </c>
       <c r="F168" s="3" t="inlineStr">
@@ -12084,7 +12084,7 @@
       </c>
       <c r="E169" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:00</t>
+          <t>2026-02-07 18:36:09</t>
         </is>
       </c>
       <c r="F169" s="3" t="inlineStr">
@@ -12126,7 +12126,7 @@
       </c>
       <c r="O169" s="3" t="inlineStr">
         <is>
-          <t>5.9 °C</t>
+          <t>6.0 °C</t>
         </is>
       </c>
     </row>
@@ -12153,7 +12153,7 @@
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:02</t>
+          <t>2026-02-07 18:36:12</t>
         </is>
       </c>
       <c r="F170" s="3" t="inlineStr">
@@ -12174,7 +12174,7 @@
       </c>
       <c r="J170" s="3" t="inlineStr">
         <is>
-          <t>1006.8 hPa</t>
+          <t>1006.9 hPa</t>
         </is>
       </c>
       <c r="K170" s="3" t="inlineStr">
@@ -12226,7 +12226,7 @@
       </c>
       <c r="E171" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:05</t>
+          <t>2026-02-07 18:36:14</t>
         </is>
       </c>
       <c r="F171" s="3" t="inlineStr">
@@ -12247,7 +12247,7 @@
       </c>
       <c r="J171" s="3" t="inlineStr">
         <is>
-          <t>1006.0 hPa</t>
+          <t>1006.1 hPa</t>
         </is>
       </c>
       <c r="K171" s="3" t="inlineStr">
@@ -12299,7 +12299,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:07</t>
+          <t>2026-02-07 18:36:17</t>
         </is>
       </c>
       <c r="F172" s="3" t="inlineStr">
@@ -12310,7 +12310,7 @@
       <c r="G172" s="3" t="inlineStr"/>
       <c r="H172" s="3" t="inlineStr">
         <is>
-          <t>51%</t>
+          <t>52%</t>
         </is>
       </c>
       <c r="I172" s="3" t="inlineStr">
@@ -12368,7 +12368,7 @@
       </c>
       <c r="E173" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:09</t>
+          <t>2026-02-07 18:36:19</t>
         </is>
       </c>
       <c r="F173" s="3" t="inlineStr">
@@ -12441,7 +12441,7 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:12</t>
+          <t>2026-02-07 18:36:22</t>
         </is>
       </c>
       <c r="F174" s="3" t="inlineStr">
@@ -12506,7 +12506,7 @@
       </c>
       <c r="E175" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:14</t>
+          <t>2026-02-07 18:36:24</t>
         </is>
       </c>
       <c r="F175" s="3" t="inlineStr">
@@ -12575,7 +12575,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:17</t>
+          <t>2026-02-07 18:36:27</t>
         </is>
       </c>
       <c r="F176" s="3" t="inlineStr">
@@ -12596,7 +12596,7 @@
       </c>
       <c r="J176" s="3" t="inlineStr">
         <is>
-          <t>1004.9 hPa</t>
+          <t>1005.0 hPa</t>
         </is>
       </c>
       <c r="K176" s="3" t="inlineStr">
@@ -12648,7 +12648,7 @@
       </c>
       <c r="E177" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:19</t>
+          <t>2026-02-07 18:36:29</t>
         </is>
       </c>
       <c r="F177" s="3" t="inlineStr">
@@ -12717,7 +12717,7 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:21</t>
+          <t>2026-02-07 18:36:31</t>
         </is>
       </c>
       <c r="F178" s="3" t="inlineStr">
@@ -12763,7 +12763,7 @@
       </c>
       <c r="O178" s="3" t="inlineStr">
         <is>
-          <t>-4.2 °C</t>
+          <t>-4.3 °C</t>
         </is>
       </c>
     </row>
@@ -12790,7 +12790,7 @@
       </c>
       <c r="E179" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:24</t>
+          <t>2026-02-07 18:36:34</t>
         </is>
       </c>
       <c r="F179" s="3" t="inlineStr">
@@ -12867,7 +12867,7 @@
       </c>
       <c r="E180" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:26</t>
+          <t>2026-02-07 18:36:36</t>
         </is>
       </c>
       <c r="F180" s="3" t="inlineStr">
@@ -12878,7 +12878,7 @@
       <c r="G180" s="3" t="inlineStr"/>
       <c r="H180" s="3" t="inlineStr">
         <is>
-          <t>59%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="I180" s="3" t="inlineStr">
@@ -12940,7 +12940,7 @@
       </c>
       <c r="E181" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:29</t>
+          <t>2026-02-07 18:36:39</t>
         </is>
       </c>
       <c r="F181" s="3" t="inlineStr">
@@ -13009,7 +13009,7 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:31</t>
+          <t>2026-02-07 18:36:42</t>
         </is>
       </c>
       <c r="F182" s="3" t="inlineStr">
@@ -13030,7 +13030,7 @@
       </c>
       <c r="J182" s="3" t="inlineStr">
         <is>
-          <t>1004.5 hPa</t>
+          <t>1004.6 hPa</t>
         </is>
       </c>
       <c r="K182" s="3" t="inlineStr">
@@ -13055,7 +13055,7 @@
       </c>
       <c r="O182" s="3" t="inlineStr">
         <is>
-          <t>5.2 °C</t>
+          <t>5.1 °C</t>
         </is>
       </c>
     </row>
@@ -13082,7 +13082,7 @@
       </c>
       <c r="E183" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:34</t>
+          <t>2026-02-07 18:36:45</t>
         </is>
       </c>
       <c r="F183" s="3" t="inlineStr">
@@ -13093,7 +13093,7 @@
       <c r="G183" s="3" t="inlineStr"/>
       <c r="H183" s="3" t="inlineStr">
         <is>
-          <t>58%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="I183" s="3" t="inlineStr">
@@ -13151,7 +13151,7 @@
       </c>
       <c r="E184" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:36</t>
+          <t>2026-02-07 18:36:47</t>
         </is>
       </c>
       <c r="F184" s="3" t="inlineStr">
@@ -13172,7 +13172,7 @@
       </c>
       <c r="J184" s="3" t="inlineStr">
         <is>
-          <t>1006.5 hPa</t>
+          <t>1006.6 hPa</t>
         </is>
       </c>
       <c r="K184" s="3" t="inlineStr"/>
@@ -13220,7 +13220,7 @@
       </c>
       <c r="E185" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:38</t>
+          <t>2026-02-07 18:36:49</t>
         </is>
       </c>
       <c r="F185" s="3" t="inlineStr">
@@ -13261,7 +13261,7 @@
       </c>
       <c r="E186" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:40</t>
+          <t>2026-02-07 18:36:51</t>
         </is>
       </c>
       <c r="F186" s="3" t="inlineStr">
@@ -13330,7 +13330,7 @@
       </c>
       <c r="E187" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:43</t>
+          <t>2026-02-07 18:36:54</t>
         </is>
       </c>
       <c r="F187" s="3" t="inlineStr">
@@ -13351,7 +13351,7 @@
       </c>
       <c r="J187" s="3" t="inlineStr">
         <is>
-          <t>1006.7 hPa</t>
+          <t>1006.8 hPa</t>
         </is>
       </c>
       <c r="K187" s="3" t="inlineStr">
@@ -13403,7 +13403,7 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:45</t>
+          <t>2026-02-07 18:36:57</t>
         </is>
       </c>
       <c r="F188" s="3" t="inlineStr">
@@ -13476,7 +13476,7 @@
       </c>
       <c r="E189" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:47</t>
+          <t>2026-02-07 18:36:59</t>
         </is>
       </c>
       <c r="F189" s="3" t="inlineStr">
@@ -13487,7 +13487,7 @@
       <c r="G189" s="3" t="inlineStr"/>
       <c r="H189" s="3" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="I189" s="3" t="inlineStr">
@@ -13498,7 +13498,7 @@
       <c r="J189" s="3" t="inlineStr"/>
       <c r="K189" s="3" t="inlineStr">
         <is>
-          <t>12.1 MJ/m2</t>
+          <t>12.0 MJ/m2</t>
         </is>
       </c>
       <c r="L189" s="3" t="inlineStr">
@@ -13518,7 +13518,7 @@
       </c>
       <c r="O189" s="3" t="inlineStr">
         <is>
-          <t>12.6 °C</t>
+          <t>12.5 °C</t>
         </is>
       </c>
     </row>
@@ -13545,7 +13545,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>2026-02-07 18:04:50</t>
+          <t>2026-02-07 18:37:02</t>
         </is>
       </c>
       <c r="F190" s="3" t="inlineStr">
@@ -13556,7 +13556,7 @@
       <c r="G190" s="3" t="inlineStr"/>
       <c r="H190" s="3" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>67%</t>
         </is>
       </c>
       <c r="I190" s="3" t="inlineStr">
@@ -13566,7 +13566,7 @@
       </c>
       <c r="J190" s="3" t="inlineStr">
         <is>
-          <t>1006.1 hPa</t>
+          <t>1006.2 hPa</t>
         </is>
       </c>
       <c r="K190" s="3" t="inlineStr">

</xml_diff>